<commit_message>
generated data all the way back to 2008 and continued work on the machine learning model
</commit_message>
<xml_diff>
--- a/current_games_spread.xlsx
+++ b/current_games_spread.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>year</t>
   </si>
@@ -175,46 +175,58 @@
     <t>calc_home_prob</t>
   </si>
   <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>SanAntonio</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
     <t>Orlando</t>
   </si>
   <si>
-    <t>Detroit</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Portland</t>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>GoldenState</t>
+  </si>
+  <si>
+    <t>OklahomaCity</t>
   </si>
   <si>
     <t>Sacramento</t>
   </si>
   <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>Milwaukee</t>
+    <t>Toronto</t>
   </si>
   <si>
     <t>Atlanta</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
-    <t>SanAntonio</t>
-  </si>
-  <si>
-    <t>Memphis</t>
   </si>
 </sst>
 </file>
@@ -572,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB8"/>
+  <dimension ref="A1:BB10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -747,145 +759,145 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J2">
-        <v>110.9130434782609</v>
+        <v>112.6346153846154</v>
       </c>
       <c r="K2">
-        <v>118.531914893617</v>
+        <v>113</v>
       </c>
       <c r="L2">
-        <v>98.35869565217394</v>
+        <v>99.57115384615385</v>
       </c>
       <c r="M2">
-        <v>98.49148936170212</v>
+        <v>98.55600000000003</v>
       </c>
       <c r="N2">
-        <v>112.295652173913</v>
+        <v>112.5057692307692</v>
       </c>
       <c r="O2">
-        <v>119.3148936170213</v>
+        <v>114.31</v>
       </c>
       <c r="P2">
-        <v>116.1130434782609</v>
+        <v>119.7846153846154</v>
       </c>
       <c r="Q2">
-        <v>112.7659574468085</v>
+        <v>114.362</v>
       </c>
       <c r="R2">
-        <v>76.46739130434784</v>
+        <v>74.34807692307692</v>
       </c>
       <c r="S2">
-        <v>78.64468085106384</v>
+        <v>76.85600000000001</v>
       </c>
       <c r="T2">
-        <v>0.3678260869565218</v>
+        <v>0.378653846153846</v>
       </c>
       <c r="U2">
-        <v>0.4719148936170212</v>
+        <v>0.36522</v>
       </c>
       <c r="V2">
-        <v>0.5782173913043477</v>
+        <v>0.5656153846153846</v>
       </c>
       <c r="W2">
-        <v>0.6035106382978724</v>
+        <v>0.58114</v>
       </c>
       <c r="X2">
-        <v>0.2997173913043478</v>
+        <v>0.3138269230769231</v>
       </c>
       <c r="Y2">
-        <v>0.2570425531914894</v>
+        <v>0.2713599999999999</v>
       </c>
       <c r="Z2">
-        <v>13.19565217391304</v>
+        <v>12.52115384615385</v>
       </c>
       <c r="AA2">
-        <v>11.55744680851064</v>
+        <v>11.964</v>
       </c>
       <c r="AB2">
-        <v>11.89130434782608</v>
+        <v>12.05</v>
       </c>
       <c r="AC2">
-        <v>11.17872340425532</v>
+        <v>10.572</v>
       </c>
       <c r="AD2">
-        <v>0.2243478260869565</v>
+        <v>0.2371634615384615</v>
       </c>
       <c r="AE2">
-        <v>0.1967659574468085</v>
+        <v>0.2073099999999999</v>
       </c>
       <c r="AF2">
-        <v>0.9720687421407614</v>
+        <v>0.9862926040684359</v>
       </c>
       <c r="AG2">
-        <v>1.038842374177187</v>
+        <v>0.989492119089317</v>
       </c>
       <c r="AH2">
-        <v>1.072912583300666</v>
+        <v>1.032838199305674</v>
       </c>
       <c r="AI2">
-        <v>1.003949021719619</v>
+        <v>1.026548672566372</v>
       </c>
       <c r="AJ2">
-        <v>10.28681318581458</v>
+        <v>11.51592350108493</v>
       </c>
       <c r="AK2">
-        <v>10.63885104944756</v>
+        <v>10.59433811051922</v>
       </c>
       <c r="AL2">
-        <v>0.3695652173913043</v>
+        <v>0.25</v>
       </c>
       <c r="AM2">
-        <v>0.7446808510638298</v>
+        <v>0.48</v>
       </c>
       <c r="AN2">
-        <v>26.5</v>
+        <v>29.5</v>
       </c>
       <c r="AO2">
-        <v>54.5</v>
+        <v>35.5</v>
       </c>
       <c r="AP2">
-        <v>74.59999999999999</v>
+        <v>74.2</v>
       </c>
       <c r="AQ2">
-        <v>78.59999999999999</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="AR2">
-        <v>0.5</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AS2">
-        <v>0.6363636363636364</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="AT2">
-        <v>0.5071318902825623</v>
+        <v>0.5257344810205941</v>
       </c>
       <c r="AU2">
-        <v>0.4695083700980355</v>
+        <v>0.4891954111467336</v>
       </c>
       <c r="AV2">
-        <v>-7.67</v>
+        <v>-7.35</v>
       </c>
       <c r="AW2">
-        <v>7.02</v>
+        <v>-3.23</v>
       </c>
       <c r="AZ2">
-        <v>0.03548007246376812</v>
+        <v>0.04517761752136754</v>
       </c>
       <c r="BA2">
-        <v>0.2066252955082742</v>
+        <v>0.02946527777777778</v>
       </c>
       <c r="BB2">
-        <v>0.4700677829830625</v>
+        <v>0.4758239727410554</v>
       </c>
     </row>
     <row r="3" spans="1:54">
@@ -896,145 +908,145 @@
         <v>2023</v>
       </c>
       <c r="D3">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E3">
-        <v>11</v>
+        <v>-5</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J3">
-        <v>112.0416666666667</v>
+        <v>116.66</v>
       </c>
       <c r="K3">
-        <v>112.3913043478261</v>
+        <v>114.12</v>
       </c>
       <c r="L3">
-        <v>99.39375</v>
+        <v>100.928</v>
       </c>
       <c r="M3">
-        <v>98.48260869565219</v>
+        <v>96.95399999999998</v>
       </c>
       <c r="N3">
-        <v>112.0729166666667</v>
+        <v>115.224</v>
       </c>
       <c r="O3">
-        <v>113.2195652173913</v>
+        <v>117.186</v>
       </c>
       <c r="P3">
-        <v>119.55625</v>
+        <v>110.872</v>
       </c>
       <c r="Q3">
-        <v>112.2</v>
+        <v>116.998</v>
       </c>
       <c r="R3">
-        <v>74.73333333333332</v>
+        <v>75.91</v>
       </c>
       <c r="S3">
-        <v>77.3717391304348</v>
+        <v>76.09599999999999</v>
       </c>
       <c r="T3">
-        <v>0.3767916666666666</v>
+        <v>0.3549</v>
       </c>
       <c r="U3">
-        <v>0.4407826086956522</v>
+        <v>0.4055799999999999</v>
       </c>
       <c r="V3">
-        <v>0.5627500000000001</v>
+        <v>0.56052</v>
       </c>
       <c r="W3">
-        <v>0.5665434782608694</v>
+        <v>0.5981</v>
       </c>
       <c r="X3">
-        <v>0.3097916666666666</v>
+        <v>0.2736999999999999</v>
       </c>
       <c r="Y3">
-        <v>0.2528260869565218</v>
+        <v>0.30222</v>
       </c>
       <c r="Z3">
-        <v>12.46041666666667</v>
+        <v>11.532</v>
       </c>
       <c r="AA3">
-        <v>12.59565217391304</v>
+        <v>12.886</v>
       </c>
       <c r="AB3">
-        <v>11.98958333333334</v>
+        <v>12.696</v>
       </c>
       <c r="AC3">
-        <v>10.51304347826087</v>
+        <v>11.568</v>
       </c>
       <c r="AD3">
-        <v>0.2354166666666666</v>
+        <v>0.2015899999999999</v>
       </c>
       <c r="AE3">
-        <v>0.1825652173913043</v>
+        <v>0.22736</v>
       </c>
       <c r="AF3">
-        <v>0.9819602687700848</v>
+        <v>1.0215411558669</v>
       </c>
       <c r="AG3">
-        <v>0.9850245779827003</v>
+        <v>0.9992994746059545</v>
       </c>
       <c r="AH3">
-        <v>0.9579769431015247</v>
+        <v>0.9486256357506144</v>
       </c>
       <c r="AI3">
-        <v>1.079561573178594</v>
+        <v>1.074891926626942</v>
       </c>
       <c r="AJ3">
-        <v>11.37973039614247</v>
+        <v>11.88042086796592</v>
       </c>
       <c r="AK3">
-        <v>11.54853324183669</v>
+        <v>13.13566138418618</v>
       </c>
       <c r="AL3">
-        <v>0.25</v>
+        <v>0.64</v>
       </c>
       <c r="AM3">
-        <v>0.6304347826086957</v>
+        <v>0.48</v>
       </c>
       <c r="AN3">
-        <v>29.5</v>
+        <v>49.5</v>
       </c>
       <c r="AO3">
-        <v>53.5</v>
+        <v>39.5</v>
       </c>
       <c r="AP3">
-        <v>74.2</v>
+        <v>75.2</v>
       </c>
       <c r="AQ3">
-        <v>76.09999999999999</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="AR3">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="AS3">
-        <v>0.6666666666666666</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AT3">
-        <v>0.5282592340912388</v>
+        <v>0.4616853744497145</v>
       </c>
       <c r="AU3">
-        <v>0.4802409576447534</v>
+        <v>0.4833922264901451</v>
       </c>
       <c r="AV3">
-        <v>-7.35</v>
+        <v>5.37</v>
       </c>
       <c r="AW3">
-        <v>3.22</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="AZ3">
-        <v>0.09423032407407408</v>
+        <v>0.09444027777777778</v>
       </c>
       <c r="BA3">
-        <v>0.01678894927536232</v>
+        <v>0.06464861111111112</v>
       </c>
       <c r="BB3">
-        <v>0.5022798415288673</v>
+        <v>0.5546961072000478</v>
       </c>
     </row>
     <row r="4" spans="1:54">
@@ -1045,145 +1057,145 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>239.5</v>
+        <v>230.5</v>
       </c>
       <c r="E4">
-        <v>-1</v>
+        <v>-9</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J4">
-        <v>114.8</v>
+        <v>114.6734693877551</v>
       </c>
       <c r="K4">
-        <v>115.9574468085106</v>
+        <v>111.2549019607843</v>
       </c>
       <c r="L4">
-        <v>99.10444444444444</v>
+        <v>97.16326530612247</v>
       </c>
       <c r="M4">
-        <v>100.0617021276596</v>
+        <v>98.38823529411766</v>
       </c>
       <c r="N4">
-        <v>114.6066666666667</v>
+        <v>116.9224489795918</v>
       </c>
       <c r="O4">
-        <v>114.7127659574468</v>
+        <v>112.6647058823529</v>
       </c>
       <c r="P4">
-        <v>114.8355555555556</v>
+        <v>113.2836734693878</v>
       </c>
       <c r="Q4">
-        <v>114.9744680851064</v>
+        <v>115.9705882352942</v>
       </c>
       <c r="R4">
-        <v>78.01111111111111</v>
+        <v>77.1612244897959</v>
       </c>
       <c r="S4">
-        <v>75.41914893617019</v>
+        <v>76.99803921568629</v>
       </c>
       <c r="T4">
-        <v>0.3338666666666666</v>
+        <v>0.3947551020408163</v>
       </c>
       <c r="U4">
-        <v>0.3343829787234042</v>
+        <v>0.366764705882353</v>
       </c>
       <c r="V4">
-        <v>0.5901999999999998</v>
+        <v>0.6018163265306123</v>
       </c>
       <c r="W4">
-        <v>0.5735531914893618</v>
+        <v>0.5807450980392155</v>
       </c>
       <c r="X4">
-        <v>0.2584222222222223</v>
+        <v>0.2889795918367346</v>
       </c>
       <c r="Y4">
-        <v>0.2384893617021277</v>
+        <v>0.3026274509803921</v>
       </c>
       <c r="Z4">
-        <v>11.86666666666667</v>
+        <v>12.2530612244898</v>
       </c>
       <c r="AA4">
-        <v>10.88723404255319</v>
+        <v>13.15882352941177</v>
       </c>
       <c r="AB4">
-        <v>12.74222222222223</v>
+        <v>13.07959183673469</v>
       </c>
       <c r="AC4">
-        <v>12.3468085106383</v>
+        <v>12.06078431372549</v>
       </c>
       <c r="AD4">
-        <v>0.2079555555555556</v>
+        <v>0.2297857142857142</v>
       </c>
       <c r="AE4">
-        <v>0.2075212765957447</v>
+        <v>0.2248627450980392</v>
       </c>
       <c r="AF4">
-        <v>1.006134969325153</v>
+        <v>1.004145966617821</v>
       </c>
       <c r="AG4">
-        <v>1.01627911313331</v>
+        <v>0.9742110504446962</v>
       </c>
       <c r="AH4">
-        <v>1.068524970963995</v>
+        <v>1.081331197722015</v>
       </c>
       <c r="AI4">
-        <v>1.112477064220184</v>
+        <v>0.9977088473739867</v>
       </c>
       <c r="AJ4">
-        <v>10.95972424632826</v>
+        <v>11.68705503154184</v>
       </c>
       <c r="AK4">
-        <v>10.4615963283111</v>
+        <v>10.09531659470128</v>
       </c>
       <c r="AL4">
-        <v>0.4666666666666667</v>
+        <v>0.6530612244897959</v>
       </c>
       <c r="AM4">
-        <v>0.5106382978723404</v>
+        <v>0.392156862745098</v>
       </c>
       <c r="AN4">
-        <v>41.5</v>
+        <v>50.5</v>
       </c>
       <c r="AO4">
-        <v>46.5</v>
+        <v>26.5</v>
       </c>
       <c r="AP4">
-        <v>76.40000000000001</v>
+        <v>76.2</v>
       </c>
       <c r="AQ4">
-        <v>76.8</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="AR4">
-        <v>0.2857142857142857</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="AS4">
-        <v>0.5714285714285714</v>
+        <v>0.4615384615384616</v>
       </c>
       <c r="AT4">
-        <v>0.5119788660790292</v>
+        <v>0.4668807932495382</v>
       </c>
       <c r="AU4">
-        <v>0.4865763855555223</v>
+        <v>0.5144816496194571</v>
       </c>
       <c r="AV4">
-        <v>-0.37</v>
+        <v>2.57</v>
       </c>
       <c r="AW4">
-        <v>1.55</v>
+        <v>-7.67</v>
       </c>
       <c r="AZ4">
-        <v>0.04159567901234568</v>
+        <v>0</v>
       </c>
       <c r="BA4">
-        <v>0</v>
+        <v>0.0320016339869281</v>
       </c>
       <c r="BB4">
-        <v>0.4443271816666012</v>
+        <v>0.4988822868847246</v>
       </c>
     </row>
     <row r="5" spans="1:54">
@@ -1194,145 +1206,145 @@
         <v>2023</v>
       </c>
       <c r="D5">
-        <v>234</v>
+        <v>226.5</v>
       </c>
       <c r="E5">
-        <v>5.5</v>
+        <v>-8.5</v>
       </c>
       <c r="F5" t="s">
         <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J5">
-        <v>109.6739130434783</v>
+        <v>117.7647058823529</v>
       </c>
       <c r="K5">
-        <v>115.3125</v>
+        <v>114.56</v>
       </c>
       <c r="L5">
-        <v>98.68695652173911</v>
+        <v>98.22941176470586</v>
       </c>
       <c r="M5">
-        <v>100.5395833333333</v>
+        <v>97.74400000000003</v>
       </c>
       <c r="N5">
-        <v>110.6108695652174</v>
+        <v>118.4470588235294</v>
       </c>
       <c r="O5">
-        <v>114.5020833333333</v>
+        <v>117.038</v>
       </c>
       <c r="P5">
-        <v>118.5717391304348</v>
+        <v>112.7666666666667</v>
       </c>
       <c r="Q5">
-        <v>114.6958333333333</v>
+        <v>113.862</v>
       </c>
       <c r="R5">
-        <v>76.0891304347826</v>
+        <v>78.54705882352941</v>
       </c>
       <c r="S5">
-        <v>73.325</v>
+        <v>73.85999999999997</v>
       </c>
       <c r="T5">
-        <v>0.3953043478260869</v>
+        <v>0.4725882352941175</v>
       </c>
       <c r="U5">
-        <v>0.3779791666666668</v>
+        <v>0.37594</v>
       </c>
       <c r="V5">
-        <v>0.5515217391304349</v>
+        <v>0.6004901960784313</v>
       </c>
       <c r="W5">
-        <v>0.5974166666666666</v>
+        <v>0.6148200000000001</v>
       </c>
       <c r="X5">
-        <v>0.2888478260869564</v>
+        <v>0.2602549019607844</v>
       </c>
       <c r="Y5">
-        <v>0.2791041666666667</v>
+        <v>0.24718</v>
       </c>
       <c r="Z5">
-        <v>13.91086956521739</v>
+        <v>11.72352941176471</v>
       </c>
       <c r="AA5">
-        <v>13.51458333333333</v>
+        <v>12.754</v>
       </c>
       <c r="AB5">
-        <v>11.70217391304348</v>
+        <v>10.93725490196079</v>
       </c>
       <c r="AC5">
-        <v>13.31041666666666</v>
+        <v>11.748</v>
       </c>
       <c r="AD5">
-        <v>0.2174021739130435</v>
+        <v>0.1979705882352942</v>
       </c>
       <c r="AE5">
-        <v>0.221</v>
+        <v>0.20836</v>
       </c>
       <c r="AF5">
-        <v>0.9612087032732539</v>
+        <v>1.031214587411146</v>
       </c>
       <c r="AG5">
-        <v>1.010626643295355</v>
+        <v>1.003152364273205</v>
       </c>
       <c r="AH5">
-        <v>1.072877436405682</v>
+        <v>0.9538794538794538</v>
       </c>
       <c r="AI5">
-        <v>1.037759710930443</v>
+        <v>1.062034450651769</v>
       </c>
       <c r="AJ5">
-        <v>10.95852724916535</v>
+        <v>11.12247016451622</v>
       </c>
       <c r="AK5">
-        <v>10.73575849284375</v>
+        <v>11.32812429310343</v>
       </c>
       <c r="AL5">
-        <v>0.2173913043478261</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="AM5">
-        <v>0.5</v>
+        <v>0.62</v>
       </c>
       <c r="AN5">
-        <v>23.5</v>
+        <v>54.5</v>
       </c>
       <c r="AO5">
-        <v>49.5</v>
+        <v>50.5</v>
       </c>
       <c r="AP5">
-        <v>73.7</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="AQ5">
-        <v>75.7</v>
+        <v>76.5</v>
       </c>
       <c r="AR5">
-        <v>0.3333333333333333</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="AS5">
-        <v>0.5</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="AT5">
-        <v>0.5409531548535245</v>
+        <v>0.4701593191895224</v>
       </c>
       <c r="AU5">
-        <v>0.4998922843289262</v>
+        <v>0.4971801412612292</v>
       </c>
       <c r="AV5">
-        <v>-8.26</v>
+        <v>7.02</v>
       </c>
       <c r="AW5">
-        <v>2.53</v>
+        <v>0.82</v>
       </c>
       <c r="AZ5">
-        <v>0</v>
+        <v>0.1086996187363834</v>
       </c>
       <c r="BA5">
-        <v>0.08646846064814816</v>
+        <v>0.2389722222222222</v>
       </c>
       <c r="BB5">
-        <v>0.5383599538478676</v>
+        <v>0.5376034404991255</v>
       </c>
     </row>
     <row r="6" spans="1:54">
@@ -1343,145 +1355,145 @@
         <v>2023</v>
       </c>
       <c r="D6">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E6">
-        <v>-8</v>
+        <v>3.5</v>
       </c>
       <c r="F6" t="s">
         <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J6">
-        <v>117.5102040816327</v>
+        <v>115.0754716981132</v>
       </c>
       <c r="K6">
-        <v>112.5744680851064</v>
+        <v>118.1</v>
       </c>
       <c r="L6">
-        <v>99.3938775510204</v>
+        <v>100.5018867924528</v>
       </c>
       <c r="M6">
-        <v>100.1276595744681</v>
+        <v>101.72</v>
       </c>
       <c r="N6">
-        <v>117.4877551020408</v>
+        <v>114.1433962264151</v>
       </c>
       <c r="O6">
-        <v>111.1127659574468</v>
+        <v>115.244</v>
       </c>
       <c r="P6">
-        <v>116.7265306122449</v>
+        <v>114.0113207547169</v>
       </c>
       <c r="Q6">
-        <v>117.3829787234042</v>
+        <v>115.212</v>
       </c>
       <c r="R6">
-        <v>74.9142857142857</v>
+        <v>73.56792452830189</v>
       </c>
       <c r="S6">
-        <v>75.6212765957447</v>
+        <v>76.15799999999999</v>
       </c>
       <c r="T6">
-        <v>0.4429387755102041</v>
+        <v>0.3821320754716982</v>
       </c>
       <c r="U6">
-        <v>0.361872340425532</v>
+        <v>0.4824200000000001</v>
       </c>
       <c r="V6">
-        <v>0.5898163265306122</v>
+        <v>0.5966792452830189</v>
       </c>
       <c r="W6">
-        <v>0.5475531914893618</v>
+        <v>0.5974199999999997</v>
       </c>
       <c r="X6">
-        <v>0.2711632653061224</v>
+        <v>0.2771509433962264</v>
       </c>
       <c r="Y6">
-        <v>0.2542127659574469</v>
+        <v>0.2279200000000001</v>
       </c>
       <c r="Z6">
-        <v>12.80408163265307</v>
+        <v>13.6377358490566</v>
       </c>
       <c r="AA6">
-        <v>11.35106382978723</v>
+        <v>13.908</v>
       </c>
       <c r="AB6">
-        <v>11.63673469387756</v>
+        <v>13.26603773584905</v>
       </c>
       <c r="AC6">
-        <v>12.61489361702127</v>
+        <v>12.144</v>
       </c>
       <c r="AD6">
-        <v>0.2126020408163265</v>
+        <v>0.2184999999999999</v>
       </c>
       <c r="AE6">
-        <v>0.2070744680851063</v>
+        <v>0.20424</v>
       </c>
       <c r="AF6">
-        <v>1.029887853476185</v>
+        <v>1.007666126953706</v>
       </c>
       <c r="AG6">
-        <v>0.9866298692822646</v>
+        <v>1.03415061295972</v>
       </c>
       <c r="AH6">
-        <v>1.015514646289221</v>
+        <v>0.9819642564354812</v>
       </c>
       <c r="AI6">
-        <v>1.071883071883072</v>
+        <v>1.069714930849563</v>
       </c>
       <c r="AJ6">
-        <v>10.29785483700683</v>
+        <v>10.26966416860802</v>
       </c>
       <c r="AK6">
-        <v>11.23585575309244</v>
+        <v>11.1610931364271</v>
       </c>
       <c r="AL6">
-        <v>0.4897959183673469</v>
+        <v>0.5094339622641509</v>
       </c>
       <c r="AM6">
-        <v>0.2765957446808511</v>
+        <v>0.52</v>
       </c>
       <c r="AN6">
-        <v>23.5</v>
+        <v>49.5</v>
       </c>
       <c r="AO6">
-        <v>34.5</v>
+        <v>52.5</v>
       </c>
       <c r="AP6">
-        <v>74.3</v>
+        <v>75.7</v>
       </c>
       <c r="AQ6">
-        <v>75.59999999999999</v>
+        <v>76.3</v>
       </c>
       <c r="AR6">
-        <v>0.45</v>
+        <v>0.4615384615384616</v>
       </c>
       <c r="AS6">
-        <v>0.3846153846153846</v>
+        <v>0.5</v>
       </c>
       <c r="AT6">
-        <v>0.516454935879905</v>
+        <v>0.5006922459857107</v>
       </c>
       <c r="AU6">
-        <v>0.5149182210065953</v>
+        <v>0.4599134479728436</v>
       </c>
       <c r="AV6">
-        <v>5.67</v>
+        <v>2.53</v>
       </c>
       <c r="AW6">
-        <v>0.53</v>
+        <v>5.52</v>
       </c>
       <c r="AZ6">
-        <v>0.09456207482993197</v>
+        <v>0.07831105870020966</v>
       </c>
       <c r="BA6">
-        <v>0</v>
+        <v>0.003536111111111111</v>
       </c>
       <c r="BB6">
-        <v>0.403992335820841</v>
+        <v>0.473056474132357</v>
       </c>
     </row>
     <row r="7" spans="1:54">
@@ -1492,145 +1504,145 @@
         <v>2023</v>
       </c>
       <c r="D7">
-        <v>241</v>
+        <v>232.5</v>
       </c>
       <c r="E7">
-        <v>-8</v>
+        <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J7">
-        <v>112.8478260869565</v>
+        <v>109.58</v>
       </c>
       <c r="K7">
-        <v>112.7608695652174</v>
+        <v>116.86</v>
       </c>
       <c r="L7">
-        <v>97.0586956521739</v>
+        <v>98.76799999999996</v>
       </c>
       <c r="M7">
-        <v>100.5413043478261</v>
+        <v>100.554</v>
       </c>
       <c r="N7">
-        <v>115.7152173913043</v>
+        <v>110.452</v>
       </c>
       <c r="O7">
-        <v>112.1369565217392</v>
+        <v>114.848</v>
       </c>
       <c r="P7">
-        <v>115.8195652173913</v>
+        <v>118.108</v>
       </c>
       <c r="Q7">
-        <v>120.6173913043478</v>
+        <v>113.878</v>
       </c>
       <c r="R7">
-        <v>76.78695652173913</v>
+        <v>76.07799999999999</v>
       </c>
       <c r="S7">
-        <v>75.19130434782608</v>
+        <v>72.774</v>
       </c>
       <c r="T7">
-        <v>0.4063913043478261</v>
+        <v>0.38766</v>
       </c>
       <c r="U7">
-        <v>0.3444782608695652</v>
+        <v>0.3582799999999999</v>
       </c>
       <c r="V7">
-        <v>0.5906739130434783</v>
+        <v>0.5513600000000001</v>
       </c>
       <c r="W7">
-        <v>0.5639130434782608</v>
+        <v>0.5712399999999999</v>
       </c>
       <c r="X7">
-        <v>0.3048913043478261</v>
+        <v>0.2877999999999999</v>
       </c>
       <c r="Y7">
-        <v>0.2390869565217391</v>
+        <v>0.24724</v>
       </c>
       <c r="Z7">
-        <v>13.20434782608696</v>
+        <v>14.056</v>
       </c>
       <c r="AA7">
-        <v>13.10652173913043</v>
+        <v>11.432</v>
       </c>
       <c r="AB7">
-        <v>11.79565217391304</v>
+        <v>11.66</v>
       </c>
       <c r="AC7">
-        <v>12.03260869565217</v>
+        <v>13.746</v>
       </c>
       <c r="AD7">
-        <v>0.229</v>
+        <v>0.2161399999999999</v>
       </c>
       <c r="AE7">
-        <v>0.1864891304347826</v>
+        <v>0.21313</v>
       </c>
       <c r="AF7">
-        <v>0.9890256449338871</v>
+        <v>0.9595446584938704</v>
       </c>
       <c r="AG7">
-        <v>0.9882635369431849</v>
+        <v>1.023292469352014</v>
       </c>
       <c r="AH7">
-        <v>0.9452257111667631</v>
+        <v>0.9582040518342764</v>
       </c>
       <c r="AI7">
-        <v>1.037593984962406</v>
+        <v>1.038279422671002</v>
       </c>
       <c r="AJ7">
-        <v>12.13325898244044</v>
+        <v>10.8850172255261</v>
       </c>
       <c r="AK7">
-        <v>10.91107292099794</v>
+        <v>11.83386665464843</v>
       </c>
       <c r="AL7">
-        <v>0.4565217391304348</v>
+        <v>0.24</v>
       </c>
       <c r="AM7">
-        <v>0.3043478260869565</v>
+        <v>0.48</v>
       </c>
       <c r="AN7">
-        <v>39.5</v>
+        <v>23.5</v>
       </c>
       <c r="AO7">
-        <v>22.5</v>
+        <v>23.5</v>
       </c>
       <c r="AP7">
-        <v>75.09999999999999</v>
+        <v>73.7</v>
       </c>
       <c r="AQ7">
-        <v>73.2</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="AR7">
-        <v>0.4285714285714285</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="AS7">
-        <v>0.4545454545454545</v>
+        <v>0.3125</v>
       </c>
       <c r="AT7">
-        <v>0.4875057282265282</v>
+        <v>0.5336498073718861</v>
       </c>
       <c r="AU7">
-        <v>0.503620387886378</v>
+        <v>0.522953524768202</v>
       </c>
       <c r="AV7">
-        <v>-8.550000000000001</v>
+        <v>-8.26</v>
       </c>
       <c r="AW7">
-        <v>0.02</v>
+        <v>-7.9</v>
       </c>
       <c r="AZ7">
-        <v>0.07027022946859902</v>
+        <v>0.1383333333333333</v>
       </c>
       <c r="BA7">
-        <v>0.08211956521739132</v>
+        <v>0.2209361111111111</v>
       </c>
       <c r="BB7">
-        <v>0.4800476456028397</v>
+        <v>0.5349845143797591</v>
       </c>
     </row>
     <row r="8" spans="1:54">
@@ -1641,145 +1653,443 @@
         <v>2023</v>
       </c>
       <c r="D8">
-        <v>246.5</v>
+        <v>244</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="F8" t="s">
         <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J8">
-        <v>120</v>
+        <v>112.5882352941177</v>
       </c>
       <c r="K8">
-        <v>117.4130434782609</v>
+        <v>119.5102040816327</v>
       </c>
       <c r="L8">
-        <v>100.7177777777778</v>
+        <v>100.4549019607843</v>
       </c>
       <c r="M8">
-        <v>101.0586956521739</v>
+        <v>100.5326530612245</v>
       </c>
       <c r="N8">
-        <v>118.8911111111111</v>
+        <v>111.8627450980393</v>
       </c>
       <c r="O8">
-        <v>115.7434782608696</v>
+        <v>118.3795918367347</v>
       </c>
       <c r="P8">
-        <v>116.0977777777778</v>
+        <v>121.4509803921569</v>
       </c>
       <c r="Q8">
-        <v>110.3434782608696</v>
+        <v>115.5836734693878</v>
       </c>
       <c r="R8">
-        <v>77.62666666666668</v>
+        <v>75.41372549019609</v>
       </c>
       <c r="S8">
-        <v>76.42173913043477</v>
+        <v>77.65510204081633</v>
       </c>
       <c r="T8">
-        <v>0.4204888888888888</v>
+        <v>0.3397058823529411</v>
       </c>
       <c r="U8">
-        <v>0.3533695652173913</v>
+        <v>0.4187755102040815</v>
       </c>
       <c r="V8">
-        <v>0.6080222222222222</v>
+        <v>0.5598823529411765</v>
       </c>
       <c r="W8">
-        <v>0.563108695652174</v>
+        <v>0.6076530612244898</v>
       </c>
       <c r="X8">
-        <v>0.2906888888888889</v>
+        <v>0.2390392156862745</v>
       </c>
       <c r="Y8">
-        <v>0.2763478260869565</v>
+        <v>0.2873265306122449</v>
       </c>
       <c r="Z8">
-        <v>12.10888888888889</v>
+        <v>12.87254901960784</v>
       </c>
       <c r="AA8">
-        <v>11.51304347826087</v>
+        <v>12.30408163265306</v>
       </c>
       <c r="AB8">
-        <v>12.13333333333333</v>
+        <v>11.7921568627451</v>
       </c>
       <c r="AC8">
-        <v>12.25217391304348</v>
+        <v>12.23673469387755</v>
       </c>
       <c r="AD8">
-        <v>0.2210666666666667</v>
+        <v>0.1863137254901961</v>
       </c>
       <c r="AE8">
-        <v>0.2027717391304347</v>
+        <v>0.2159591836734694</v>
       </c>
       <c r="AF8">
-        <v>1.05170902716915</v>
+        <v>0.9858864736787886</v>
       </c>
       <c r="AG8">
-        <v>1.029036314445757</v>
+        <v>1.046499160084349</v>
       </c>
       <c r="AH8">
-        <v>1.002777777777778</v>
+        <v>0.9592476489028213</v>
       </c>
       <c r="AI8">
-        <v>0.9822872307597358</v>
+        <v>0.9008993624772313</v>
       </c>
       <c r="AJ8">
-        <v>11.61990629145615</v>
+        <v>10.83779962941656</v>
       </c>
       <c r="AK8">
-        <v>11.8350549436768</v>
+        <v>11.92000967158146</v>
       </c>
       <c r="AL8">
-        <v>0.5777777777777777</v>
+        <v>0.2745098039215687</v>
       </c>
       <c r="AM8">
-        <v>0.6739130434782609</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="AN8">
+        <v>22.5</v>
+      </c>
+      <c r="AO8">
         <v>34.5</v>
       </c>
-      <c r="AO8">
-        <v>49.5</v>
-      </c>
       <c r="AP8">
+        <v>73.2</v>
+      </c>
+      <c r="AQ8">
         <v>75.90000000000001</v>
       </c>
-      <c r="AQ8">
-        <v>75.2</v>
-      </c>
       <c r="AR8">
+        <v>0.4545454545454545</v>
+      </c>
+      <c r="AS8">
         <v>0.5</v>
       </c>
-      <c r="AS8">
-        <v>0.5454545454545454</v>
-      </c>
       <c r="AT8">
-        <v>0.4761150797887579</v>
+        <v>0.5013878562811607</v>
       </c>
       <c r="AU8">
-        <v>0.457533500158395</v>
+        <v>0.4809311494851381</v>
       </c>
       <c r="AV8">
+        <v>0.02</v>
+      </c>
+      <c r="AW8">
         <v>-5.26</v>
       </c>
-      <c r="AW8">
-        <v>5.37</v>
-      </c>
       <c r="AZ8">
-        <v>0</v>
+        <v>0.0740686274509804</v>
       </c>
       <c r="BA8">
         <v>0</v>
       </c>
       <c r="BB8">
-        <v>0.5362640466121502</v>
+        <v>0.4691531170330834</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2023</v>
+      </c>
+      <c r="D9">
+        <v>230.5</v>
+      </c>
+      <c r="E9">
+        <v>-3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9">
+        <v>117.5</v>
+      </c>
+      <c r="K9">
+        <v>112.7884615384615</v>
+      </c>
+      <c r="L9">
+        <v>99.29615384615384</v>
+      </c>
+      <c r="M9">
+        <v>96.38653846153846</v>
+      </c>
+      <c r="N9">
+        <v>117.6326923076923</v>
+      </c>
+      <c r="O9">
+        <v>116.2365384615385</v>
+      </c>
+      <c r="P9">
+        <v>116.6019230769231</v>
+      </c>
+      <c r="Q9">
+        <v>115.7346153846154</v>
+      </c>
+      <c r="R9">
+        <v>75.2576923076923</v>
+      </c>
+      <c r="S9">
+        <v>76.56923076923077</v>
+      </c>
+      <c r="T9">
+        <v>0.4435384615384615</v>
+      </c>
+      <c r="U9">
+        <v>0.3589807692307693</v>
+      </c>
+      <c r="V9">
+        <v>0.5911923076923076</v>
+      </c>
+      <c r="W9">
+        <v>0.5569038461538461</v>
+      </c>
+      <c r="X9">
+        <v>0.2701730769230769</v>
+      </c>
+      <c r="Y9">
+        <v>0.2793846153846153</v>
+      </c>
+      <c r="Z9">
+        <v>12.84807692307693</v>
+      </c>
+      <c r="AA9">
+        <v>10.05192307692308</v>
+      </c>
+      <c r="AB9">
+        <v>11.64807692307692</v>
+      </c>
+      <c r="AC9">
+        <v>14.53653846153846</v>
+      </c>
+      <c r="AD9">
+        <v>0.2116346153846154</v>
+      </c>
+      <c r="AE9">
+        <v>0.2239423076923077</v>
+      </c>
+      <c r="AF9">
+        <v>1.028896672504378</v>
+      </c>
+      <c r="AG9">
+        <v>0.9876397682877542</v>
+      </c>
+      <c r="AH9">
+        <v>0.9985815602836879</v>
+      </c>
+      <c r="AI9">
+        <v>1.022563228189827</v>
+      </c>
+      <c r="AJ9">
+        <v>10.12897595249164</v>
+      </c>
+      <c r="AK9">
+        <v>10.51982841784163</v>
+      </c>
+      <c r="AL9">
+        <v>0.5</v>
+      </c>
+      <c r="AM9">
+        <v>0.4423076923076923</v>
+      </c>
+      <c r="AN9">
+        <v>23.5</v>
+      </c>
+      <c r="AO9">
+        <v>46.5</v>
+      </c>
+      <c r="AP9">
+        <v>74.3</v>
+      </c>
+      <c r="AQ9">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="AR9">
+        <v>0.45</v>
+      </c>
+      <c r="AS9">
+        <v>0.25</v>
+      </c>
+      <c r="AT9">
+        <v>0.5109802444072918</v>
+      </c>
+      <c r="AU9">
+        <v>0.4632874520987874</v>
+      </c>
+      <c r="AV9">
+        <v>5.67</v>
+      </c>
+      <c r="AW9">
+        <v>2.37</v>
+      </c>
+      <c r="AZ9">
+        <v>0</v>
+      </c>
+      <c r="BA9">
+        <v>0.1291092414529914</v>
+      </c>
+      <c r="BB9">
+        <v>0.4960854202449316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2023</v>
+      </c>
+      <c r="D10">
+        <v>229.5</v>
+      </c>
+      <c r="E10">
+        <v>-1.5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10">
+        <v>112.9230769230769</v>
+      </c>
+      <c r="K10">
+        <v>116.1764705882353</v>
+      </c>
+      <c r="L10">
+        <v>97.08076923076919</v>
+      </c>
+      <c r="M10">
+        <v>99.83529411764708</v>
+      </c>
+      <c r="N10">
+        <v>115.3788461538461</v>
+      </c>
+      <c r="O10">
+        <v>115.2941176470588</v>
+      </c>
+      <c r="P10">
+        <v>114.0269230769231</v>
+      </c>
+      <c r="Q10">
+        <v>115.8960784313725</v>
+      </c>
+      <c r="R10">
+        <v>75.59038461538465</v>
+      </c>
+      <c r="S10">
+        <v>75.74705882352939</v>
+      </c>
+      <c r="T10">
+        <v>0.3688653846153845</v>
+      </c>
+      <c r="U10">
+        <v>0.3343529411764705</v>
+      </c>
+      <c r="V10">
+        <v>0.5693076923076925</v>
+      </c>
+      <c r="W10">
+        <v>0.5748039215686276</v>
+      </c>
+      <c r="X10">
+        <v>0.2390192307692307</v>
+      </c>
+      <c r="Y10">
+        <v>0.2422745098039216</v>
+      </c>
+      <c r="Z10">
+        <v>11.91538461538462</v>
+      </c>
+      <c r="AA10">
+        <v>10.87058823529412</v>
+      </c>
+      <c r="AB10">
+        <v>12.49615384615385</v>
+      </c>
+      <c r="AC10">
+        <v>12.14313725490196</v>
+      </c>
+      <c r="AD10">
+        <v>0.2111442307692308</v>
+      </c>
+      <c r="AE10">
+        <v>0.2071764705882353</v>
+      </c>
+      <c r="AF10">
+        <v>0.9888185369796577</v>
+      </c>
+      <c r="AG10">
+        <v>1.017307097970537</v>
+      </c>
+      <c r="AH10">
+        <v>0.9947774750227066</v>
+      </c>
+      <c r="AI10">
+        <v>1.075949367088608</v>
+      </c>
+      <c r="AJ10">
+        <v>12.83901229403534</v>
+      </c>
+      <c r="AK10">
+        <v>10.78253104695492</v>
+      </c>
+      <c r="AL10">
+        <v>0.5192307692307693</v>
+      </c>
+      <c r="AM10">
+        <v>0.4901960784313725</v>
+      </c>
+      <c r="AN10">
+        <v>52.5</v>
+      </c>
+      <c r="AO10">
+        <v>46.5</v>
+      </c>
+      <c r="AP10">
+        <v>77</v>
+      </c>
+      <c r="AQ10">
+        <v>76.8</v>
+      </c>
+      <c r="AR10">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="AS10">
+        <v>0.5625</v>
+      </c>
+      <c r="AT10">
+        <v>0.5201061141568565</v>
+      </c>
+      <c r="AU10">
+        <v>0.4867434903865058</v>
+      </c>
+      <c r="AV10">
+        <v>6.94</v>
+      </c>
+      <c r="AW10">
+        <v>1.55</v>
+      </c>
+      <c r="AZ10">
+        <v>0.1855128205128205</v>
+      </c>
+      <c r="BA10">
+        <v>0</v>
+      </c>
+      <c r="BB10">
+        <v>0.5081830790651193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more work on machine learning model
</commit_message>
<xml_diff>
--- a/current_games_spread.xlsx
+++ b/current_games_spread.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>year</t>
   </si>
@@ -175,58 +175,70 @@
     <t>calc_home_prob</t>
   </si>
   <si>
-    <t>Detroit</t>
-  </si>
-  <si>
-    <t>Memphis</t>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
   </si>
   <si>
     <t>Philadelphia</t>
   </si>
   <si>
-    <t>Boston</t>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>OklahomaCity</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>GoldenState</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>SanAntonio</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>NewOrleans</t>
   </si>
   <si>
     <t>Minnesota</t>
   </si>
   <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>SanAntonio</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Phoenix</t>
-  </si>
-  <si>
     <t>Washington</t>
   </si>
   <si>
-    <t>Portland</t>
-  </si>
-  <si>
-    <t>Orlando</t>
-  </si>
-  <si>
-    <t>Brooklyn</t>
-  </si>
-  <si>
-    <t>GoldenState</t>
-  </si>
-  <si>
-    <t>OklahomaCity</t>
-  </si>
-  <si>
-    <t>Sacramento</t>
-  </si>
-  <si>
-    <t>Toronto</t>
-  </si>
-  <si>
-    <t>Atlanta</t>
+    <t>LALakers</t>
   </si>
 </sst>
 </file>
@@ -584,7 +596,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB10"/>
+  <dimension ref="A1:BB12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -759,145 +771,157 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>237</v>
+        <v>239.5</v>
       </c>
       <c r="E2">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="H2">
+        <v>0.4107142857142857</v>
+      </c>
+      <c r="I2">
+        <v>0.4642857142857143</v>
       </c>
       <c r="J2">
-        <v>112.6346153846154</v>
+        <v>111.8275862068966</v>
       </c>
       <c r="K2">
-        <v>113</v>
+        <v>116.280701754386</v>
       </c>
       <c r="L2">
-        <v>99.57115384615385</v>
+        <v>100.4551724137931</v>
       </c>
       <c r="M2">
-        <v>98.55600000000003</v>
+        <v>99.8280701754386</v>
       </c>
       <c r="N2">
-        <v>112.5057692307692</v>
+        <v>110.2896551724138</v>
       </c>
       <c r="O2">
-        <v>114.31</v>
+        <v>115.5175438596491</v>
       </c>
       <c r="P2">
-        <v>119.7846153846154</v>
+        <v>117.1620689655172</v>
       </c>
       <c r="Q2">
-        <v>114.362</v>
+        <v>115.4035087719298</v>
       </c>
       <c r="R2">
-        <v>74.34807692307692</v>
+        <v>75.48965517241383</v>
       </c>
       <c r="S2">
-        <v>76.85600000000001</v>
+        <v>75.6140350877193</v>
       </c>
       <c r="T2">
-        <v>0.378653846153846</v>
+        <v>0.3582413793103449</v>
       </c>
       <c r="U2">
-        <v>0.36522</v>
+        <v>0.3334210526315788</v>
       </c>
       <c r="V2">
-        <v>0.5656153846153846</v>
+        <v>0.5457068965517242</v>
       </c>
       <c r="W2">
-        <v>0.58114</v>
+        <v>0.5747368421052632</v>
       </c>
       <c r="X2">
-        <v>0.3138269230769231</v>
+        <v>0.259</v>
       </c>
       <c r="Y2">
-        <v>0.2713599999999999</v>
+        <v>0.2397894736842106</v>
       </c>
       <c r="Z2">
-        <v>12.52115384615385</v>
+        <v>11.41379310344828</v>
       </c>
       <c r="AA2">
-        <v>11.964</v>
+        <v>10.86842105263158</v>
       </c>
       <c r="AB2">
-        <v>12.05</v>
+        <v>12.62413793103448</v>
       </c>
       <c r="AC2">
-        <v>10.572</v>
+        <v>12.10350877192983</v>
       </c>
       <c r="AD2">
-        <v>0.2371634615384615</v>
+        <v>0.2059137931034482</v>
       </c>
       <c r="AE2">
-        <v>0.2073099999999999</v>
+        <v>0.2047280701754386</v>
       </c>
       <c r="AF2">
-        <v>0.9862926040684359</v>
+        <v>0.978369083174948</v>
       </c>
       <c r="AG2">
-        <v>0.989492119089317</v>
+        <v>1.017328974229099</v>
       </c>
       <c r="AH2">
-        <v>1.032838199305674</v>
+        <v>0.9687532120464589</v>
       </c>
       <c r="AI2">
-        <v>1.026548672566372</v>
+        <v>0.9975859987929995</v>
       </c>
       <c r="AJ2">
-        <v>11.51592350108493</v>
+        <v>10.75453061069434</v>
       </c>
       <c r="AK2">
-        <v>10.59433811051922</v>
+        <v>10.60412760742525</v>
       </c>
       <c r="AL2">
-        <v>0.25</v>
+        <v>0.2586206896551724</v>
       </c>
       <c r="AM2">
-        <v>0.48</v>
+        <v>0.5087719298245614</v>
       </c>
       <c r="AN2">
-        <v>29.5</v>
+        <v>34.5</v>
       </c>
       <c r="AO2">
-        <v>35.5</v>
+        <v>46.5</v>
       </c>
       <c r="AP2">
-        <v>74.2</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="AQ2">
-        <v>76.09999999999999</v>
+        <v>76.8</v>
       </c>
       <c r="AR2">
-        <v>0.3333333333333333</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="AS2">
-        <v>0.5714285714285714</v>
+        <v>0.5625</v>
       </c>
       <c r="AT2">
-        <v>0.5257344810205941</v>
+        <v>0.5142371785085557</v>
       </c>
       <c r="AU2">
-        <v>0.4891954111467336</v>
+        <v>0.4884157127775369</v>
       </c>
       <c r="AV2">
-        <v>-7.35</v>
+        <v>0.53</v>
       </c>
       <c r="AW2">
-        <v>-3.23</v>
+        <v>1.55</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
       </c>
       <c r="AZ2">
-        <v>0.04517761752136754</v>
+        <v>0.009606082375478928</v>
       </c>
       <c r="BA2">
-        <v>0.02946527777777778</v>
+        <v>0</v>
       </c>
       <c r="BB2">
-        <v>0.4758239727410554</v>
+        <v>0.4927525502177201</v>
       </c>
     </row>
     <row r="3" spans="1:54">
@@ -908,145 +932,157 @@
         <v>2023</v>
       </c>
       <c r="D3">
-        <v>239</v>
+        <v>224.5</v>
       </c>
       <c r="E3">
-        <v>-5</v>
+        <v>-14.5</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="H3">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="I3">
+        <v>0.4035087719298245</v>
       </c>
       <c r="J3">
-        <v>116.66</v>
+        <v>111.6610169491525</v>
       </c>
       <c r="K3">
-        <v>114.12</v>
+        <v>112.5438596491228</v>
       </c>
       <c r="L3">
-        <v>100.928</v>
+        <v>94.69322033898304</v>
       </c>
       <c r="M3">
-        <v>96.95399999999998</v>
+        <v>100.5964912280702</v>
       </c>
       <c r="N3">
-        <v>115.224</v>
+        <v>116.4915254237288</v>
       </c>
       <c r="O3">
-        <v>117.186</v>
+        <v>111.3105263157895</v>
       </c>
       <c r="P3">
-        <v>110.872</v>
+        <v>110.457627118644</v>
       </c>
       <c r="Q3">
-        <v>116.998</v>
+        <v>121.3385964912281</v>
       </c>
       <c r="R3">
-        <v>75.91</v>
+        <v>78.12881355932201</v>
       </c>
       <c r="S3">
-        <v>76.09599999999999</v>
+        <v>75.28421052631577</v>
       </c>
       <c r="T3">
-        <v>0.3549</v>
+        <v>0.3742711864406779</v>
       </c>
       <c r="U3">
-        <v>0.4055799999999999</v>
+        <v>0.3382105263157894</v>
       </c>
       <c r="V3">
-        <v>0.56052</v>
+        <v>0.5925254237288136</v>
       </c>
       <c r="W3">
-        <v>0.5981</v>
+        <v>0.5595438596491228</v>
       </c>
       <c r="X3">
-        <v>0.2736999999999999</v>
+        <v>0.2726440677966102</v>
       </c>
       <c r="Y3">
-        <v>0.30222</v>
+        <v>0.2357543859649123</v>
       </c>
       <c r="Z3">
-        <v>11.532</v>
+        <v>12.12033898305085</v>
       </c>
       <c r="AA3">
-        <v>12.886</v>
+        <v>13.03859649122807</v>
       </c>
       <c r="AB3">
-        <v>12.696</v>
+        <v>13.32881355932203</v>
       </c>
       <c r="AC3">
-        <v>11.568</v>
+        <v>11.62631578947368</v>
       </c>
       <c r="AD3">
-        <v>0.2015899999999999</v>
+        <v>0.2082203389830509</v>
       </c>
       <c r="AE3">
-        <v>0.22736</v>
+        <v>0.1885964912280702</v>
       </c>
       <c r="AF3">
-        <v>1.0215411558669</v>
+        <v>0.9769117843320433</v>
       </c>
       <c r="AG3">
-        <v>0.9992994746059545</v>
+        <v>0.9846356924682661</v>
       </c>
       <c r="AH3">
-        <v>0.9486256357506144</v>
+        <v>0.9791540174053835</v>
       </c>
       <c r="AI3">
-        <v>1.074891926626942</v>
+        <v>0.9922057677318784</v>
       </c>
       <c r="AJ3">
-        <v>11.88042086796592</v>
+        <v>11.28462306015944</v>
       </c>
       <c r="AK3">
-        <v>13.13566138418618</v>
+        <v>10.94334721467812</v>
       </c>
       <c r="AL3">
-        <v>0.64</v>
+        <v>0.6271186440677966</v>
       </c>
       <c r="AM3">
-        <v>0.48</v>
+        <v>0.2456140350877193</v>
       </c>
       <c r="AN3">
-        <v>49.5</v>
+        <v>46.5</v>
       </c>
       <c r="AO3">
-        <v>39.5</v>
+        <v>22.5</v>
       </c>
       <c r="AP3">
-        <v>75.2</v>
+        <v>77.2</v>
       </c>
       <c r="AQ3">
-        <v>75.09999999999999</v>
+        <v>73.2</v>
       </c>
       <c r="AR3">
-        <v>0.5</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="AS3">
-        <v>0.4666666666666667</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="AT3">
-        <v>0.4616853744497145</v>
+        <v>0.4861200277815768</v>
       </c>
       <c r="AU3">
-        <v>0.4833922264901451</v>
+        <v>0.4997811215277623</v>
       </c>
       <c r="AV3">
-        <v>5.37</v>
+        <v>2.04</v>
       </c>
       <c r="AW3">
-        <v>-8.550000000000001</v>
+        <v>0.02</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
       </c>
       <c r="AZ3">
-        <v>0.09444027777777778</v>
+        <v>0</v>
       </c>
       <c r="BA3">
-        <v>0.06464861111111112</v>
+        <v>0.224900097465887</v>
       </c>
       <c r="BB3">
-        <v>0.5546961072000478</v>
+        <v>0.4571758231346628</v>
       </c>
     </row>
     <row r="4" spans="1:54">
@@ -1057,145 +1093,157 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>230.5</v>
+        <v>225.5</v>
       </c>
       <c r="E4">
-        <v>-9</v>
+        <v>-14.5</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="H4">
+        <v>0.5740740740740741</v>
+      </c>
+      <c r="I4">
+        <v>0.4259259259259259</v>
       </c>
       <c r="J4">
-        <v>114.6734693877551</v>
+        <v>114.1272727272727</v>
       </c>
       <c r="K4">
-        <v>111.2549019607843</v>
+        <v>110.1071428571429</v>
       </c>
       <c r="L4">
-        <v>97.16326530612247</v>
+        <v>96.72727272727275</v>
       </c>
       <c r="M4">
-        <v>98.38823529411766</v>
+        <v>98.74464285714282</v>
       </c>
       <c r="N4">
-        <v>116.9224489795918</v>
+        <v>116.98</v>
       </c>
       <c r="O4">
-        <v>112.6647058823529</v>
+        <v>111.0571428571429</v>
       </c>
       <c r="P4">
-        <v>113.2836734693878</v>
+        <v>113.4072727272728</v>
       </c>
       <c r="Q4">
-        <v>115.9705882352942</v>
+        <v>118.8785714285714</v>
       </c>
       <c r="R4">
-        <v>77.1612244897959</v>
+        <v>77.26363636363635</v>
       </c>
       <c r="S4">
-        <v>76.99803921568629</v>
+        <v>75.94999999999997</v>
       </c>
       <c r="T4">
-        <v>0.3947551020408163</v>
+        <v>0.3922181818181819</v>
       </c>
       <c r="U4">
-        <v>0.366764705882353</v>
+        <v>0.3786607142857143</v>
       </c>
       <c r="V4">
-        <v>0.6018163265306123</v>
+        <v>0.6002727272727274</v>
       </c>
       <c r="W4">
-        <v>0.5807450980392155</v>
+        <v>0.5542321428571428</v>
       </c>
       <c r="X4">
-        <v>0.2889795918367346</v>
+        <v>0.2973272727272727</v>
       </c>
       <c r="Y4">
-        <v>0.3026274509803921</v>
+        <v>0.2914464285714285</v>
       </c>
       <c r="Z4">
-        <v>12.2530612244898</v>
+        <v>11.98363636363636</v>
       </c>
       <c r="AA4">
-        <v>13.15882352941177</v>
+        <v>13.99642857142857</v>
       </c>
       <c r="AB4">
-        <v>13.07959183673469</v>
+        <v>12.92909090909091</v>
       </c>
       <c r="AC4">
-        <v>12.06078431372549</v>
+        <v>11.4125</v>
       </c>
       <c r="AD4">
-        <v>0.2297857142857142</v>
+        <v>0.2315363636363636</v>
       </c>
       <c r="AE4">
-        <v>0.2248627450980392</v>
+        <v>0.2183303571428571</v>
       </c>
       <c r="AF4">
-        <v>1.004145966617821</v>
+        <v>0.9984888252604788</v>
       </c>
       <c r="AG4">
-        <v>0.9742110504446962</v>
+        <v>0.9633170853643295</v>
       </c>
       <c r="AH4">
-        <v>1.081331197722015</v>
+        <v>0.9317083532473049</v>
       </c>
       <c r="AI4">
-        <v>0.9977088473739867</v>
+        <v>1.038382527840848</v>
       </c>
       <c r="AJ4">
-        <v>11.68705503154184</v>
+        <v>12.08463268400981</v>
       </c>
       <c r="AK4">
-        <v>10.09531659470128</v>
+        <v>10.94414156952831</v>
       </c>
       <c r="AL4">
-        <v>0.6530612244897959</v>
+        <v>0.6545454545454545</v>
       </c>
       <c r="AM4">
-        <v>0.392156862745098</v>
+        <v>0.2321428571428572</v>
       </c>
       <c r="AN4">
         <v>50.5</v>
       </c>
       <c r="AO4">
-        <v>26.5</v>
+        <v>23.5</v>
       </c>
       <c r="AP4">
         <v>76.2</v>
       </c>
       <c r="AQ4">
-        <v>74.59999999999999</v>
+        <v>73.7</v>
       </c>
       <c r="AR4">
-        <v>0.6923076923076923</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="AS4">
-        <v>0.4615384615384616</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="AT4">
-        <v>0.4668807932495382</v>
+        <v>0.4708451456207227</v>
       </c>
       <c r="AU4">
-        <v>0.5144816496194571</v>
+        <v>0.5310040260184871</v>
       </c>
       <c r="AV4">
         <v>2.57</v>
       </c>
       <c r="AW4">
-        <v>-7.67</v>
+        <v>-8.26</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4">
+        <v>0</v>
       </c>
       <c r="AZ4">
         <v>0</v>
       </c>
       <c r="BA4">
-        <v>0.0320016339869281</v>
+        <v>0</v>
       </c>
       <c r="BB4">
-        <v>0.4988822868847246</v>
+        <v>0.5072247644815804</v>
       </c>
     </row>
     <row r="5" spans="1:54">
@@ -1206,145 +1254,157 @@
         <v>2023</v>
       </c>
       <c r="D5">
-        <v>226.5</v>
+        <v>238</v>
       </c>
       <c r="E5">
-        <v>-8.5</v>
+        <v>-1</v>
       </c>
       <c r="F5" t="s">
         <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="H5">
+        <v>0.5172413793103449</v>
+      </c>
+      <c r="I5">
+        <v>0.543859649122807</v>
       </c>
       <c r="J5">
-        <v>117.7647058823529</v>
+        <v>114.4137931034483</v>
       </c>
       <c r="K5">
-        <v>114.56</v>
+        <v>117.5862068965517</v>
       </c>
       <c r="L5">
-        <v>98.22941176470586</v>
+        <v>100.1448275862069</v>
       </c>
       <c r="M5">
-        <v>97.74400000000003</v>
+        <v>99.28793103448275</v>
       </c>
       <c r="N5">
-        <v>118.4470588235294</v>
+        <v>114.2224137931034</v>
       </c>
       <c r="O5">
-        <v>117.038</v>
+        <v>117.8103448275862</v>
       </c>
       <c r="P5">
-        <v>112.7666666666667</v>
+        <v>116.8551724137931</v>
       </c>
       <c r="Q5">
-        <v>113.862</v>
+        <v>117.6327586206897</v>
       </c>
       <c r="R5">
-        <v>78.54705882352941</v>
+        <v>72.43275862068967</v>
       </c>
       <c r="S5">
-        <v>73.85999999999997</v>
+        <v>74.52586206896548</v>
       </c>
       <c r="T5">
-        <v>0.4725882352941175</v>
+        <v>0.4279137931034481</v>
       </c>
       <c r="U5">
-        <v>0.37594</v>
+        <v>0.4385172413793104</v>
       </c>
       <c r="V5">
-        <v>0.6004901960784313</v>
+        <v>0.5747068965517242</v>
       </c>
       <c r="W5">
-        <v>0.6148200000000001</v>
+        <v>0.590655172413793</v>
       </c>
       <c r="X5">
-        <v>0.2602549019607844</v>
+        <v>0.2648448275862069</v>
       </c>
       <c r="Y5">
-        <v>0.24718</v>
+        <v>0.2716896551724138</v>
       </c>
       <c r="Z5">
-        <v>11.72352941176471</v>
+        <v>12.53275862068965</v>
       </c>
       <c r="AA5">
-        <v>12.754</v>
+        <v>12.71551724137932</v>
       </c>
       <c r="AB5">
-        <v>10.93725490196079</v>
+        <v>12.91724137931034</v>
       </c>
       <c r="AC5">
-        <v>11.748</v>
+        <v>11.30344827586207</v>
       </c>
       <c r="AD5">
-        <v>0.1979705882352942</v>
+        <v>0.2230258620689654</v>
       </c>
       <c r="AE5">
-        <v>0.20836</v>
+        <v>0.2126034482758621</v>
       </c>
       <c r="AF5">
-        <v>1.031214587411146</v>
+        <v>1.000995565209521</v>
       </c>
       <c r="AG5">
-        <v>1.003152364273205</v>
+        <v>1.028750716505265</v>
       </c>
       <c r="AH5">
-        <v>0.9538794538794538</v>
+        <v>0.955595740405867</v>
       </c>
       <c r="AI5">
-        <v>1.062034450651769</v>
+        <v>1.020527859237537</v>
       </c>
       <c r="AJ5">
-        <v>11.12247016451622</v>
+        <v>10.8723541890598</v>
       </c>
       <c r="AK5">
-        <v>11.32812429310343</v>
+        <v>9.892586013078649</v>
       </c>
       <c r="AL5">
-        <v>0.7058823529411765</v>
+        <v>0.4310344827586207</v>
       </c>
       <c r="AM5">
-        <v>0.62</v>
+        <v>0.4827586206896552</v>
       </c>
       <c r="AN5">
-        <v>54.5</v>
+        <v>24.5</v>
       </c>
       <c r="AO5">
-        <v>50.5</v>
+        <v>23.5</v>
       </c>
       <c r="AP5">
-        <v>78.59999999999999</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="AQ5">
-        <v>76.5</v>
+        <v>74.3</v>
       </c>
       <c r="AR5">
-        <v>0.5714285714285714</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="AS5">
-        <v>0.7142857142857143</v>
+        <v>0.4761904761904762</v>
       </c>
       <c r="AT5">
-        <v>0.4701593191895224</v>
+        <v>0.4786232524774695</v>
       </c>
       <c r="AU5">
-        <v>0.4971801412612292</v>
+        <v>0.5091581440274026</v>
       </c>
       <c r="AV5">
-        <v>7.02</v>
+        <v>-3.26</v>
       </c>
       <c r="AW5">
-        <v>0.82</v>
+        <v>5.67</v>
+      </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5">
+        <v>0</v>
       </c>
       <c r="AZ5">
-        <v>0.1086996187363834</v>
+        <v>0</v>
       </c>
       <c r="BA5">
-        <v>0.2389722222222222</v>
+        <v>0</v>
       </c>
       <c r="BB5">
-        <v>0.5376034404991255</v>
+        <v>0.4821010929620567</v>
       </c>
     </row>
     <row r="6" spans="1:54">
@@ -1355,145 +1415,157 @@
         <v>2023</v>
       </c>
       <c r="D6">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="E6">
-        <v>3.5</v>
+        <v>-2.5</v>
       </c>
       <c r="F6" t="s">
         <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="H6">
+        <v>0.5272727272727272</v>
+      </c>
+      <c r="I6">
+        <v>0.5272727272727272</v>
       </c>
       <c r="J6">
-        <v>115.0754716981132</v>
+        <v>114.2758620689655</v>
       </c>
       <c r="K6">
-        <v>118.1</v>
+        <v>114.125</v>
       </c>
       <c r="L6">
-        <v>100.5018867924528</v>
+        <v>95.83793103448276</v>
       </c>
       <c r="M6">
-        <v>101.72</v>
+        <v>97.74464285714289</v>
       </c>
       <c r="N6">
-        <v>114.1433962264151</v>
+        <v>117.4655172413793</v>
       </c>
       <c r="O6">
-        <v>115.244</v>
+        <v>116.5875</v>
       </c>
       <c r="P6">
-        <v>114.0113207547169</v>
+        <v>115.7172413793103</v>
       </c>
       <c r="Q6">
-        <v>115.212</v>
+        <v>114.6125</v>
       </c>
       <c r="R6">
-        <v>73.56792452830189</v>
+        <v>75.93965517241378</v>
       </c>
       <c r="S6">
-        <v>76.15799999999999</v>
+        <v>74.10892857142855</v>
       </c>
       <c r="T6">
-        <v>0.3821320754716982</v>
+        <v>0.3916896551724139</v>
       </c>
       <c r="U6">
-        <v>0.4824200000000001</v>
+        <v>0.37975</v>
       </c>
       <c r="V6">
-        <v>0.5966792452830189</v>
+        <v>0.567293103448276</v>
       </c>
       <c r="W6">
-        <v>0.5974199999999997</v>
+        <v>0.6101785714285716</v>
       </c>
       <c r="X6">
-        <v>0.2771509433962264</v>
+        <v>0.2887068965517242</v>
       </c>
       <c r="Y6">
-        <v>0.2279200000000001</v>
+        <v>0.2492857142857143</v>
       </c>
       <c r="Z6">
-        <v>13.6377358490566</v>
+        <v>10.59310344827586</v>
       </c>
       <c r="AA6">
-        <v>13.908</v>
+        <v>12.54464285714286</v>
       </c>
       <c r="AB6">
-        <v>13.26603773584905</v>
+        <v>10.82586206896552</v>
       </c>
       <c r="AC6">
-        <v>12.144</v>
+        <v>11.5875</v>
       </c>
       <c r="AD6">
-        <v>0.2184999999999999</v>
+        <v>0.2175689655172414</v>
       </c>
       <c r="AE6">
-        <v>0.20424</v>
+        <v>0.2118482142857143</v>
       </c>
       <c r="AF6">
-        <v>1.007666126953706</v>
+        <v>0.9997888195010107</v>
       </c>
       <c r="AG6">
-        <v>1.03415061295972</v>
+        <v>0.9984689413823272</v>
       </c>
       <c r="AH6">
-        <v>0.9819642564354812</v>
+        <v>0.980084490042245</v>
       </c>
       <c r="AI6">
-        <v>1.069714930849563</v>
+        <v>0.9521723256663016</v>
       </c>
       <c r="AJ6">
-        <v>10.26966416860802</v>
+        <v>11.04659895147679</v>
       </c>
       <c r="AK6">
-        <v>11.1610931364271</v>
+        <v>11.29485107092102</v>
       </c>
       <c r="AL6">
-        <v>0.5094339622641509</v>
+        <v>0.5344827586206896</v>
       </c>
       <c r="AM6">
-        <v>0.52</v>
+        <v>0.5892857142857143</v>
       </c>
       <c r="AN6">
-        <v>49.5</v>
+        <v>38.5</v>
       </c>
       <c r="AO6">
-        <v>52.5</v>
+        <v>50.5</v>
       </c>
       <c r="AP6">
-        <v>75.7</v>
+        <v>75.8</v>
       </c>
       <c r="AQ6">
-        <v>76.3</v>
+        <v>76.5</v>
       </c>
       <c r="AR6">
-        <v>0.4615384615384616</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="AS6">
-        <v>0.5</v>
+        <v>0.6470588235294118</v>
       </c>
       <c r="AT6">
-        <v>0.5006922459857107</v>
+        <v>0.5017457426789564</v>
       </c>
       <c r="AU6">
-        <v>0.4599134479728436</v>
+        <v>0.5040731123913106</v>
       </c>
       <c r="AV6">
-        <v>2.53</v>
+        <v>-0.01</v>
       </c>
       <c r="AW6">
-        <v>5.52</v>
+        <v>0.82</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6">
+        <v>0</v>
       </c>
       <c r="AZ6">
-        <v>0.07831105870020966</v>
+        <v>0.0734183429118774</v>
       </c>
       <c r="BA6">
-        <v>0.003536111111111111</v>
+        <v>0.06725074404761905</v>
       </c>
       <c r="BB6">
-        <v>0.473056474132357</v>
+        <v>0.5352555232354393</v>
       </c>
     </row>
     <row r="7" spans="1:54">
@@ -1504,145 +1576,157 @@
         <v>2023</v>
       </c>
       <c r="D7">
-        <v>232.5</v>
+        <v>220.5</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>-1.5</v>
       </c>
       <c r="F7" t="s">
         <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="H7">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="I7">
+        <v>0.5357142857142857</v>
       </c>
       <c r="J7">
-        <v>109.58</v>
+        <v>108.4035087719298</v>
       </c>
       <c r="K7">
-        <v>116.86</v>
+        <v>117.1578947368421</v>
       </c>
       <c r="L7">
-        <v>98.76799999999996</v>
+        <v>96.07894736842105</v>
       </c>
       <c r="M7">
-        <v>100.554</v>
+        <v>98.19824561403506</v>
       </c>
       <c r="N7">
-        <v>110.452</v>
+        <v>112.080701754386</v>
       </c>
       <c r="O7">
-        <v>114.848</v>
+        <v>118.9526315789474</v>
       </c>
       <c r="P7">
-        <v>118.108</v>
+        <v>111.8228070175439</v>
       </c>
       <c r="Q7">
-        <v>113.878</v>
+        <v>114.6842105263158</v>
       </c>
       <c r="R7">
-        <v>76.07799999999999</v>
+        <v>78.37543859649125</v>
       </c>
       <c r="S7">
-        <v>72.774</v>
+        <v>77.1368421052632</v>
       </c>
       <c r="T7">
-        <v>0.38766</v>
+        <v>0.4056140350877192</v>
       </c>
       <c r="U7">
-        <v>0.3582799999999999</v>
+        <v>0.357122807017544</v>
       </c>
       <c r="V7">
-        <v>0.5513600000000001</v>
+        <v>0.5641929824561404</v>
       </c>
       <c r="W7">
-        <v>0.5712399999999999</v>
+        <v>0.6092631578947367</v>
       </c>
       <c r="X7">
-        <v>0.2877999999999999</v>
+        <v>0.2632631578947368</v>
       </c>
       <c r="Y7">
-        <v>0.24724</v>
+        <v>0.2657543859649122</v>
       </c>
       <c r="Z7">
-        <v>14.056</v>
+        <v>11.74736842105264</v>
       </c>
       <c r="AA7">
-        <v>11.432</v>
+        <v>12.86666666666666</v>
       </c>
       <c r="AB7">
-        <v>11.66</v>
+        <v>14.61578947368421</v>
       </c>
       <c r="AC7">
-        <v>13.746</v>
+        <v>12.02982456140351</v>
       </c>
       <c r="AD7">
-        <v>0.2161399999999999</v>
+        <v>0.2098508771929825</v>
       </c>
       <c r="AE7">
-        <v>0.21313</v>
+        <v>0.2048245614035088</v>
       </c>
       <c r="AF7">
-        <v>0.9595446584938704</v>
+        <v>0.9484121502356065</v>
       </c>
       <c r="AG7">
-        <v>1.023292469352014</v>
+        <v>1.025003453515679</v>
       </c>
       <c r="AH7">
-        <v>0.9582040518342764</v>
+        <v>0.9839779899660139</v>
       </c>
       <c r="AI7">
-        <v>1.038279422671002</v>
+        <v>1.049865229110512</v>
       </c>
       <c r="AJ7">
-        <v>10.8850172255261</v>
+        <v>9.224033537778547</v>
       </c>
       <c r="AK7">
-        <v>11.83386665464843</v>
+        <v>10.85759411443585</v>
       </c>
       <c r="AL7">
-        <v>0.24</v>
+        <v>0.5614035087719298</v>
       </c>
       <c r="AM7">
-        <v>0.48</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="AN7">
-        <v>23.5</v>
+        <v>49.5</v>
       </c>
       <c r="AO7">
-        <v>23.5</v>
+        <v>51.5</v>
       </c>
       <c r="AP7">
-        <v>73.7</v>
+        <v>76.2</v>
       </c>
       <c r="AQ7">
-        <v>74.40000000000001</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="AR7">
-        <v>0.4444444444444444</v>
+        <v>0.6451612903225806</v>
       </c>
       <c r="AS7">
-        <v>0.3125</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="AT7">
-        <v>0.5336498073718861</v>
+        <v>0.497360457755521</v>
       </c>
       <c r="AU7">
-        <v>0.522953524768202</v>
+        <v>0.4886849411668416</v>
       </c>
       <c r="AV7">
-        <v>-8.26</v>
+        <v>4.23</v>
       </c>
       <c r="AW7">
-        <v>-7.9</v>
+        <v>2.16</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7">
+        <v>0</v>
       </c>
       <c r="AZ7">
-        <v>0.1383333333333333</v>
+        <v>0.2125828460038986</v>
       </c>
       <c r="BA7">
-        <v>0.2209361111111111</v>
+        <v>0.04266081871345029</v>
       </c>
       <c r="BB7">
-        <v>0.5349845143797591</v>
+        <v>0.5563048688766261</v>
       </c>
     </row>
     <row r="8" spans="1:54">
@@ -1653,145 +1737,157 @@
         <v>2023</v>
       </c>
       <c r="D8">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="E8">
-        <v>7.5</v>
+        <v>-5</v>
       </c>
       <c r="F8" t="s">
         <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="H8">
+        <v>0.5185185185185185</v>
+      </c>
+      <c r="I8">
+        <v>0.5714285714285714</v>
       </c>
       <c r="J8">
-        <v>112.5882352941177</v>
+        <v>113.7142857142857</v>
       </c>
       <c r="K8">
-        <v>119.5102040816327</v>
+        <v>111.0526315789474</v>
       </c>
       <c r="L8">
-        <v>100.4549019607843</v>
+        <v>99.07321428571427</v>
       </c>
       <c r="M8">
-        <v>100.5326530612245</v>
+        <v>98.14912280701758</v>
       </c>
       <c r="N8">
-        <v>111.8627450980393</v>
+        <v>113.8142857142857</v>
       </c>
       <c r="O8">
-        <v>118.3795918367347</v>
+        <v>112.5771929824561</v>
       </c>
       <c r="P8">
-        <v>121.4509803921569</v>
+        <v>113.6571428571429</v>
       </c>
       <c r="Q8">
-        <v>115.5836734693878</v>
+        <v>115.4596491228071</v>
       </c>
       <c r="R8">
-        <v>75.41372549019609</v>
+        <v>78.44821428571427</v>
       </c>
       <c r="S8">
-        <v>77.65510204081633</v>
+        <v>77.05964912280702</v>
       </c>
       <c r="T8">
-        <v>0.3397058823529411</v>
+        <v>0.3316428571428571</v>
       </c>
       <c r="U8">
-        <v>0.4187755102040815</v>
+        <v>0.361280701754386</v>
       </c>
       <c r="V8">
-        <v>0.5598823529411765</v>
+        <v>0.588375</v>
       </c>
       <c r="W8">
-        <v>0.6076530612244898</v>
+        <v>0.5773157894736841</v>
       </c>
       <c r="X8">
-        <v>0.2390392156862745</v>
+        <v>0.2592678571428572</v>
       </c>
       <c r="Y8">
-        <v>0.2873265306122449</v>
+        <v>0.3036491228070175</v>
       </c>
       <c r="Z8">
-        <v>12.87254901960784</v>
+        <v>12.15</v>
       </c>
       <c r="AA8">
-        <v>12.30408163265306</v>
+        <v>13.0140350877193</v>
       </c>
       <c r="AB8">
-        <v>11.7921568627451</v>
+        <v>12.42500000000001</v>
       </c>
       <c r="AC8">
-        <v>12.23673469387755</v>
+        <v>12.34736842105263</v>
       </c>
       <c r="AD8">
-        <v>0.1863137254901961</v>
+        <v>0.2073482142857143</v>
       </c>
       <c r="AE8">
-        <v>0.2159591836734694</v>
+        <v>0.2249122807017544</v>
       </c>
       <c r="AF8">
-        <v>0.9858864736787886</v>
+        <v>0.9948756405449318</v>
       </c>
       <c r="AG8">
-        <v>1.046499160084349</v>
+        <v>0.9715890776810794</v>
       </c>
       <c r="AH8">
-        <v>0.9592476489028213</v>
+        <v>0.8295644891122278</v>
       </c>
       <c r="AI8">
-        <v>0.9008993624772313</v>
+        <v>0.9484992101105845</v>
       </c>
       <c r="AJ8">
-        <v>10.83779962941656</v>
+        <v>11.83776385392209</v>
       </c>
       <c r="AK8">
-        <v>11.92000967158146</v>
+        <v>10.30996971532567</v>
       </c>
       <c r="AL8">
-        <v>0.2745098039215687</v>
+        <v>0.4642857142857143</v>
       </c>
       <c r="AM8">
-        <v>0.5714285714285714</v>
+        <v>0.4035087719298245</v>
       </c>
       <c r="AN8">
-        <v>22.5</v>
+        <v>41.5</v>
       </c>
       <c r="AO8">
-        <v>34.5</v>
+        <v>26.5</v>
       </c>
       <c r="AP8">
-        <v>73.2</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="AQ8">
-        <v>75.90000000000001</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="AR8">
-        <v>0.4545454545454545</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="AS8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AT8">
-        <v>0.5013878562811607</v>
+        <v>0.5014265243554643</v>
       </c>
       <c r="AU8">
-        <v>0.4809311494851381</v>
+        <v>0.5168364017216078</v>
       </c>
       <c r="AV8">
-        <v>0.02</v>
+        <v>-0.37</v>
       </c>
       <c r="AW8">
-        <v>-5.26</v>
+        <v>-7.67</v>
+      </c>
+      <c r="AX8">
+        <v>0</v>
+      </c>
+      <c r="AY8">
+        <v>0</v>
       </c>
       <c r="AZ8">
-        <v>0.0740686274509804</v>
+        <v>0.03342509920634921</v>
       </c>
       <c r="BA8">
-        <v>0</v>
+        <v>0.02835953878406708</v>
       </c>
       <c r="BB8">
-        <v>0.4691531170330834</v>
+        <v>0.4977675346567421</v>
       </c>
     </row>
     <row r="9" spans="1:54">
@@ -1802,7 +1898,7 @@
         <v>2023</v>
       </c>
       <c r="D9">
-        <v>230.5</v>
+        <v>237</v>
       </c>
       <c r="E9">
         <v>-3</v>
@@ -1811,136 +1907,148 @@
         <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="H9">
+        <v>0.6296296296296297</v>
+      </c>
+      <c r="I9">
+        <v>0.4821428571428572</v>
       </c>
       <c r="J9">
-        <v>117.5</v>
+        <v>117.9454545454546</v>
       </c>
       <c r="K9">
-        <v>112.7884615384615</v>
+        <v>115.3333333333333</v>
       </c>
       <c r="L9">
-        <v>99.29615384615384</v>
+        <v>100.6054545454545</v>
       </c>
       <c r="M9">
-        <v>96.38653846153846</v>
+        <v>98.9754385964912</v>
       </c>
       <c r="N9">
-        <v>117.6326923076923</v>
+        <v>115.9890909090909</v>
       </c>
       <c r="O9">
-        <v>116.2365384615385</v>
+        <v>115.3385964912281</v>
       </c>
       <c r="P9">
-        <v>116.6019230769231</v>
+        <v>114.9181818181818</v>
       </c>
       <c r="Q9">
-        <v>115.7346153846154</v>
+        <v>113.6421052631579</v>
       </c>
       <c r="R9">
-        <v>75.2576923076923</v>
+        <v>72.63272727272728</v>
       </c>
       <c r="S9">
-        <v>76.56923076923077</v>
+        <v>77.2842105263158</v>
       </c>
       <c r="T9">
-        <v>0.4435384615384615</v>
+        <v>0.3601454545454545</v>
       </c>
       <c r="U9">
-        <v>0.3589807692307693</v>
+        <v>0.34540350877193</v>
       </c>
       <c r="V9">
-        <v>0.5911923076923076</v>
+        <v>0.5756909090909088</v>
       </c>
       <c r="W9">
-        <v>0.5569038461538461</v>
+        <v>0.5812280701754386</v>
       </c>
       <c r="X9">
-        <v>0.2701730769230769</v>
+        <v>0.2487090909090909</v>
       </c>
       <c r="Y9">
-        <v>0.2793846153846153</v>
+        <v>0.2877017543859649</v>
       </c>
       <c r="Z9">
-        <v>12.84807692307693</v>
+        <v>11.20545454545455</v>
       </c>
       <c r="AA9">
-        <v>10.05192307692308</v>
+        <v>12.54561403508772</v>
       </c>
       <c r="AB9">
-        <v>11.64807692307692</v>
+        <v>13.84545454545455</v>
       </c>
       <c r="AC9">
-        <v>14.53653846153846</v>
+        <v>12.98421052631579</v>
       </c>
       <c r="AD9">
-        <v>0.2116346153846154</v>
+        <v>0.2140181818181818</v>
       </c>
       <c r="AE9">
-        <v>0.2239423076923077</v>
+        <v>0.218640350877193</v>
       </c>
       <c r="AF9">
-        <v>1.028896672504378</v>
+        <v>1.031893740555158</v>
       </c>
       <c r="AG9">
-        <v>0.9876397682877542</v>
+        <v>1.009040536599592</v>
       </c>
       <c r="AH9">
-        <v>0.9985815602836879</v>
+        <v>1.088073583063563</v>
       </c>
       <c r="AI9">
-        <v>1.022563228189827</v>
+        <v>1.03757225433526</v>
       </c>
       <c r="AJ9">
-        <v>10.12897595249164</v>
+        <v>12.84653215579022</v>
       </c>
       <c r="AK9">
-        <v>10.51982841784163</v>
+        <v>10.25693318504967</v>
       </c>
       <c r="AL9">
-        <v>0.5</v>
+        <v>0.4909090909090909</v>
       </c>
       <c r="AM9">
-        <v>0.4423076923076923</v>
+        <v>0.5087719298245614</v>
       </c>
       <c r="AN9">
         <v>23.5</v>
       </c>
       <c r="AO9">
-        <v>46.5</v>
+        <v>45.5</v>
       </c>
       <c r="AP9">
-        <v>74.3</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="AQ9">
-        <v>74.90000000000001</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="AR9">
-        <v>0.45</v>
+        <v>0.3529411764705883</v>
       </c>
       <c r="AS9">
-        <v>0.25</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AT9">
-        <v>0.5109802444072918</v>
+        <v>0.5109269500826601</v>
       </c>
       <c r="AU9">
-        <v>0.4632874520987874</v>
+        <v>0.522103121732861</v>
       </c>
       <c r="AV9">
-        <v>5.67</v>
+        <v>-7.9</v>
       </c>
       <c r="AW9">
-        <v>2.37</v>
+        <v>-0.84</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+      <c r="AY9">
+        <v>0</v>
       </c>
       <c r="AZ9">
-        <v>0</v>
+        <v>0.0513219696969697</v>
       </c>
       <c r="BA9">
-        <v>0.1291092414529914</v>
+        <v>0.06989278752436646</v>
       </c>
       <c r="BB9">
-        <v>0.4960854202449316</v>
+        <v>0.4854646746695784</v>
       </c>
     </row>
     <row r="10" spans="1:54">
@@ -1951,145 +2059,479 @@
         <v>2023</v>
       </c>
       <c r="D10">
-        <v>229.5</v>
+        <v>232.5</v>
       </c>
       <c r="E10">
-        <v>-1.5</v>
+        <v>-7.5</v>
       </c>
       <c r="F10" t="s">
         <v>61</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="H10">
+        <v>0.3818181818181818</v>
+      </c>
+      <c r="I10">
+        <v>0.4745762711864407</v>
       </c>
       <c r="J10">
-        <v>112.9230769230769</v>
+        <v>112.9310344827586</v>
       </c>
       <c r="K10">
-        <v>116.1764705882353</v>
+        <v>115.728813559322</v>
       </c>
       <c r="L10">
-        <v>97.08076923076919</v>
+        <v>95.01379310344829</v>
       </c>
       <c r="M10">
-        <v>99.83529411764708</v>
+        <v>100.7152542372881</v>
       </c>
       <c r="N10">
-        <v>115.3788461538461</v>
+        <v>117.1948275862069</v>
       </c>
       <c r="O10">
-        <v>115.2941176470588</v>
+        <v>114.4084745762712</v>
       </c>
       <c r="P10">
-        <v>114.0269230769231</v>
+        <v>116.4810344827586</v>
       </c>
       <c r="Q10">
-        <v>115.8960784313725</v>
+        <v>114.3101694915254</v>
       </c>
       <c r="R10">
-        <v>75.59038461538465</v>
+        <v>76.44827586206897</v>
       </c>
       <c r="S10">
-        <v>75.74705882352939</v>
+        <v>73.97457627118642</v>
       </c>
       <c r="T10">
-        <v>0.3688653846153845</v>
+        <v>0.4876034482758621</v>
       </c>
       <c r="U10">
-        <v>0.3343529411764705</v>
+        <v>0.3866440677966103</v>
       </c>
       <c r="V10">
-        <v>0.5693076923076925</v>
+        <v>0.5970000000000001</v>
       </c>
       <c r="W10">
-        <v>0.5748039215686276</v>
+        <v>0.5972203389830509</v>
       </c>
       <c r="X10">
-        <v>0.2390192307692307</v>
+        <v>0.3177758620689655</v>
       </c>
       <c r="Y10">
-        <v>0.2422745098039216</v>
+        <v>0.2729830508474576</v>
       </c>
       <c r="Z10">
-        <v>11.91538461538462</v>
+        <v>11.12931034482758</v>
       </c>
       <c r="AA10">
-        <v>10.87058823529412</v>
+        <v>13.51694915254237</v>
       </c>
       <c r="AB10">
-        <v>12.49615384615385</v>
+        <v>11.79137931034483</v>
       </c>
       <c r="AC10">
-        <v>12.14313725490196</v>
+        <v>13.23559322033898</v>
       </c>
       <c r="AD10">
-        <v>0.2111442307692308</v>
+        <v>0.2361810344827586</v>
       </c>
       <c r="AE10">
-        <v>0.2071764705882353</v>
+        <v>0.2185508474576271</v>
       </c>
       <c r="AF10">
-        <v>0.9888185369796577</v>
+        <v>0.9880230488430326</v>
       </c>
       <c r="AG10">
-        <v>1.017307097970537</v>
+        <v>1.012500556074559</v>
       </c>
       <c r="AH10">
-        <v>0.9947774750227066</v>
+        <v>1.062595419847328</v>
       </c>
       <c r="AI10">
-        <v>1.075949367088608</v>
+        <v>1.042667447764109</v>
       </c>
       <c r="AJ10">
-        <v>12.83901229403534</v>
+        <v>11.64986616611822</v>
       </c>
       <c r="AK10">
-        <v>10.78253104695492</v>
+        <v>10.59713825852643</v>
       </c>
       <c r="AL10">
-        <v>0.5192307692307693</v>
+        <v>0.5344827586206896</v>
       </c>
       <c r="AM10">
-        <v>0.4901960784313725</v>
+        <v>0.5084745762711864</v>
       </c>
       <c r="AN10">
+        <v>48.5</v>
+      </c>
+      <c r="AO10">
+        <v>49.5</v>
+      </c>
+      <c r="AP10">
+        <v>75.3</v>
+      </c>
+      <c r="AQ10">
+        <v>75.7</v>
+      </c>
+      <c r="AR10">
+        <v>0.6521739130434783</v>
+      </c>
+      <c r="AS10">
+        <v>0.5</v>
+      </c>
+      <c r="AT10">
+        <v>0.4948452023531681</v>
+      </c>
+      <c r="AU10">
+        <v>0.5072308985866205</v>
+      </c>
+      <c r="AV10">
+        <v>3.12</v>
+      </c>
+      <c r="AW10">
+        <v>2.53</v>
+      </c>
+      <c r="AX10">
+        <v>0</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+      <c r="AZ10">
+        <v>0.06642241379310346</v>
+      </c>
+      <c r="BA10">
+        <v>0.0500765065913371</v>
+      </c>
+      <c r="BB10">
+        <v>0.5045813821174125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2023</v>
+      </c>
+      <c r="D11">
+        <v>233.5</v>
+      </c>
+      <c r="E11">
+        <v>-4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11">
+        <v>0.4545454545454545</v>
+      </c>
+      <c r="I11">
+        <v>0.5</v>
+      </c>
+      <c r="J11">
+        <v>118.2321428571429</v>
+      </c>
+      <c r="K11">
+        <v>113.1818181818182</v>
+      </c>
+      <c r="L11">
+        <v>101.6875</v>
+      </c>
+      <c r="M11">
+        <v>98.25090909090913</v>
+      </c>
+      <c r="N11">
+        <v>115.3303571428571</v>
+      </c>
+      <c r="O11">
+        <v>114.9272727272727</v>
+      </c>
+      <c r="P11">
+        <v>115.2607142857143</v>
+      </c>
+      <c r="Q11">
+        <v>115.06</v>
+      </c>
+      <c r="R11">
+        <v>76.3517857142857</v>
+      </c>
+      <c r="S11">
+        <v>76.68545454545456</v>
+      </c>
+      <c r="T11">
+        <v>0.4796071428571428</v>
+      </c>
+      <c r="U11">
+        <v>0.3656909090909092</v>
+      </c>
+      <c r="V11">
+        <v>0.5983571428571427</v>
+      </c>
+      <c r="W11">
+        <v>0.585</v>
+      </c>
+      <c r="X11">
+        <v>0.2236785714285715</v>
+      </c>
+      <c r="Y11">
+        <v>0.2737454545454545</v>
+      </c>
+      <c r="Z11">
+        <v>13.83035714285714</v>
+      </c>
+      <c r="AA11">
+        <v>12.08727272727273</v>
+      </c>
+      <c r="AB11">
+        <v>12.14107142857143</v>
+      </c>
+      <c r="AC11">
+        <v>10.48909090909091</v>
+      </c>
+      <c r="AD11">
+        <v>0.2020535714285714</v>
+      </c>
+      <c r="AE11">
+        <v>0.2091</v>
+      </c>
+      <c r="AF11">
+        <v>1.034401949756281</v>
+      </c>
+      <c r="AG11">
+        <v>0.9902171319494155</v>
+      </c>
+      <c r="AH11">
+        <v>1.031868297840205</v>
+      </c>
+      <c r="AI11">
+        <v>0.9895582329317268</v>
+      </c>
+      <c r="AJ11">
+        <v>11.1915003963923</v>
+      </c>
+      <c r="AK11">
+        <v>10.80755780854879</v>
+      </c>
+      <c r="AL11">
+        <v>0.5</v>
+      </c>
+      <c r="AM11">
+        <v>0.4727272727272727</v>
+      </c>
+      <c r="AN11">
         <v>52.5</v>
       </c>
-      <c r="AO10">
-        <v>46.5</v>
-      </c>
-      <c r="AP10">
-        <v>77</v>
-      </c>
-      <c r="AQ10">
-        <v>76.8</v>
-      </c>
-      <c r="AR10">
-        <v>0.3888888888888889</v>
-      </c>
-      <c r="AS10">
-        <v>0.5625</v>
-      </c>
-      <c r="AT10">
-        <v>0.5201061141568565</v>
-      </c>
-      <c r="AU10">
-        <v>0.4867434903865058</v>
-      </c>
-      <c r="AV10">
-        <v>6.94</v>
-      </c>
-      <c r="AW10">
-        <v>1.55</v>
-      </c>
-      <c r="AZ10">
-        <v>0.1855128205128205</v>
-      </c>
-      <c r="BA10">
-        <v>0</v>
-      </c>
-      <c r="BB10">
-        <v>0.5081830790651193</v>
+      <c r="AO11">
+        <v>35.5</v>
+      </c>
+      <c r="AP11">
+        <v>76.3</v>
+      </c>
+      <c r="AQ11">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="AR11">
+        <v>0.4375</v>
+      </c>
+      <c r="AS11">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="AT11">
+        <v>0.4665778935925355</v>
+      </c>
+      <c r="AU11">
+        <v>0.4885297006723326</v>
+      </c>
+      <c r="AV11">
+        <v>5.52</v>
+      </c>
+      <c r="AW11">
+        <v>-3.23</v>
+      </c>
+      <c r="AX11">
+        <v>0</v>
+      </c>
+      <c r="AY11">
+        <v>0</v>
+      </c>
+      <c r="AZ11">
+        <v>0.1008246527777778</v>
+      </c>
+      <c r="BA11">
+        <v>0</v>
+      </c>
+      <c r="BB11">
+        <v>0.5080132763719982</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2023</v>
+      </c>
+      <c r="D12">
+        <v>238</v>
+      </c>
+      <c r="E12">
+        <v>-2.5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12">
+        <v>0.5178571428571429</v>
+      </c>
+      <c r="I12">
+        <v>0.4642857142857143</v>
+      </c>
+      <c r="J12">
+        <v>114.9107142857143</v>
+      </c>
+      <c r="K12">
+        <v>117</v>
+      </c>
+      <c r="L12">
+        <v>97.02142857142853</v>
+      </c>
+      <c r="M12">
+        <v>101.340350877193</v>
+      </c>
+      <c r="N12">
+        <v>118.0178571428571</v>
+      </c>
+      <c r="O12">
+        <v>114.2315789473684</v>
+      </c>
+      <c r="P12">
+        <v>118.0964285714285</v>
+      </c>
+      <c r="Q12">
+        <v>115.5350877192983</v>
+      </c>
+      <c r="R12">
+        <v>76.08392857142857</v>
+      </c>
+      <c r="S12">
+        <v>76.13859649122804</v>
+      </c>
+      <c r="T12">
+        <v>0.4093035714285714</v>
+      </c>
+      <c r="U12">
+        <v>0.3422982456140351</v>
+      </c>
+      <c r="V12">
+        <v>0.6018214285714286</v>
+      </c>
+      <c r="W12">
+        <v>0.5796140350877192</v>
+      </c>
+      <c r="X12">
+        <v>0.3046428571428572</v>
+      </c>
+      <c r="Y12">
+        <v>0.2905087719298247</v>
+      </c>
+      <c r="Z12">
+        <v>12.74464285714286</v>
+      </c>
+      <c r="AA12">
+        <v>11.76842105263158</v>
+      </c>
+      <c r="AB12">
+        <v>11.46785714285714</v>
+      </c>
+      <c r="AC12">
+        <v>10.62456140350877</v>
+      </c>
+      <c r="AD12">
+        <v>0.2318035714285715</v>
+      </c>
+      <c r="AE12">
+        <v>0.2049298245614035</v>
+      </c>
+      <c r="AF12">
+        <v>1.005343082114736</v>
+      </c>
+      <c r="AG12">
+        <v>1.023622047244094</v>
+      </c>
+      <c r="AH12">
+        <v>1.05009065009065</v>
+      </c>
+      <c r="AI12">
+        <v>0.9829059829059829</v>
+      </c>
+      <c r="AJ12">
+        <v>12.80105574010302</v>
+      </c>
+      <c r="AK12">
+        <v>11.03423699060847</v>
+      </c>
+      <c r="AL12">
+        <v>0.4821428571428572</v>
+      </c>
+      <c r="AM12">
+        <v>0.456140350877193</v>
+      </c>
+      <c r="AN12">
+        <v>39.5</v>
+      </c>
+      <c r="AO12">
+        <v>44.5</v>
+      </c>
+      <c r="AP12">
+        <v>75.09999999999999</v>
+      </c>
+      <c r="AQ12">
+        <v>75</v>
+      </c>
+      <c r="AR12">
+        <v>0.5</v>
+      </c>
+      <c r="AS12">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="AT12">
+        <v>0.4899900864789329</v>
+      </c>
+      <c r="AU12">
+        <v>0.5090334752681904</v>
+      </c>
+      <c r="AV12">
+        <v>-8.550000000000001</v>
+      </c>
+      <c r="AW12">
+        <v>-3.08</v>
+      </c>
+      <c r="AX12">
+        <v>0</v>
+      </c>
+      <c r="AY12">
+        <v>0</v>
+      </c>
+      <c r="AZ12">
+        <v>0.09126116071428569</v>
+      </c>
+      <c r="BA12">
+        <v>0</v>
+      </c>
+      <c r="BB12">
+        <v>0.5405309416319272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
script written for totals ml parameter search
</commit_message>
<xml_diff>
--- a/current_games_spread.xlsx
+++ b/current_games_spread.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>year</t>
   </si>
@@ -175,70 +175,58 @@
     <t>calc_home_prob</t>
   </si>
   <si>
-    <t>Charlotte</t>
+    <t>Indiana</t>
   </si>
   <si>
     <t>Cleveland</t>
   </si>
   <si>
+    <t>Orlando</t>
+  </si>
+  <si>
     <t>Philadelphia</t>
   </si>
   <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>NewYork</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>Chicago</t>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>LALakers</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>NewOrleans</t>
+  </si>
+  <si>
+    <t>SanAntonio</t>
   </si>
   <si>
     <t>OklahomaCity</t>
   </si>
   <si>
-    <t>Dallas</t>
-  </si>
-  <si>
     <t>GoldenState</t>
   </si>
   <si>
     <t>Portland</t>
-  </si>
-  <si>
-    <t>Atlanta</t>
-  </si>
-  <si>
-    <t>SanAntonio</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Brooklyn</t>
-  </si>
-  <si>
-    <t>Denver</t>
-  </si>
-  <si>
-    <t>Orlando</t>
-  </si>
-  <si>
-    <t>NewOrleans</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>LALakers</t>
   </si>
 </sst>
 </file>
@@ -596,7 +584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB12"/>
+  <dimension ref="A1:BB10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -771,142 +759,142 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>239.5</v>
+        <v>232.5</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H2">
-        <v>0.4107142857142857</v>
+        <v>0.5166666666666667</v>
       </c>
       <c r="I2">
-        <v>0.4642857142857143</v>
+        <v>0.559322033898305</v>
       </c>
       <c r="J2">
-        <v>111.8275862068966</v>
+        <v>114.5</v>
       </c>
       <c r="K2">
-        <v>116.280701754386</v>
+        <v>117.864406779661</v>
       </c>
       <c r="L2">
-        <v>100.4551724137931</v>
+        <v>100.1333333333333</v>
       </c>
       <c r="M2">
-        <v>99.8280701754386</v>
+        <v>97.97118644067795</v>
       </c>
       <c r="N2">
-        <v>110.2896551724138</v>
+        <v>114.3233333333333</v>
       </c>
       <c r="O2">
-        <v>115.5175438596491</v>
+        <v>118.8779661016949</v>
       </c>
       <c r="P2">
-        <v>117.1620689655172</v>
+        <v>116.9033333333334</v>
       </c>
       <c r="Q2">
-        <v>115.4035087719298</v>
+        <v>112.471186440678</v>
       </c>
       <c r="R2">
-        <v>75.48965517241383</v>
+        <v>72.58500000000001</v>
       </c>
       <c r="S2">
-        <v>75.6140350877193</v>
+        <v>79.24406779661018</v>
       </c>
       <c r="T2">
-        <v>0.3582413793103449</v>
+        <v>0.4286166666666665</v>
       </c>
       <c r="U2">
-        <v>0.3334210526315788</v>
+        <v>0.4795762711864405</v>
       </c>
       <c r="V2">
-        <v>0.5457068965517242</v>
+        <v>0.5759500000000001</v>
       </c>
       <c r="W2">
-        <v>0.5747368421052632</v>
+        <v>0.6039322033898304</v>
       </c>
       <c r="X2">
-        <v>0.259</v>
+        <v>0.2641500000000001</v>
       </c>
       <c r="Y2">
-        <v>0.2397894736842106</v>
+        <v>0.2538474576271187</v>
       </c>
       <c r="Z2">
-        <v>11.41379310344828</v>
+        <v>12.54</v>
       </c>
       <c r="AA2">
-        <v>10.86842105263158</v>
+        <v>11.67966101694916</v>
       </c>
       <c r="AB2">
-        <v>12.62413793103448</v>
+        <v>12.95333333333333</v>
       </c>
       <c r="AC2">
-        <v>12.10350877192983</v>
+        <v>10.70677966101695</v>
       </c>
       <c r="AD2">
-        <v>0.2059137931034482</v>
+        <v>0.2227499999999999</v>
       </c>
       <c r="AE2">
-        <v>0.2047280701754386</v>
+        <v>0.194906779661017</v>
       </c>
       <c r="AF2">
-        <v>0.978369083174948</v>
+        <v>1.00174978127734</v>
       </c>
       <c r="AG2">
-        <v>1.017328974229099</v>
+        <v>1.031184661239379</v>
       </c>
       <c r="AH2">
-        <v>0.9687532120464589</v>
+        <v>1.01018922852984</v>
       </c>
       <c r="AI2">
-        <v>0.9975859987929995</v>
+        <v>1.04922826191161</v>
       </c>
       <c r="AJ2">
-        <v>10.75453061069434</v>
+        <v>10.69968846898513</v>
       </c>
       <c r="AK2">
-        <v>10.60412760742525</v>
+        <v>11.44842173582498</v>
       </c>
       <c r="AL2">
-        <v>0.2586206896551724</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="AM2">
-        <v>0.5087719298245614</v>
+        <v>0.711864406779661</v>
       </c>
       <c r="AN2">
-        <v>34.5</v>
+        <v>24.5</v>
       </c>
       <c r="AO2">
-        <v>46.5</v>
+        <v>54.5</v>
       </c>
       <c r="AP2">
-        <v>75.59999999999999</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="AQ2">
-        <v>76.8</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="AR2">
-        <v>0.4285714285714285</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="AS2">
-        <v>0.5625</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="AT2">
-        <v>0.5142371785085557</v>
+        <v>0.4783174602543346</v>
       </c>
       <c r="AU2">
-        <v>0.4884157127775369</v>
+        <v>0.4722330995958968</v>
       </c>
       <c r="AV2">
-        <v>0.53</v>
+        <v>-3.26</v>
       </c>
       <c r="AW2">
-        <v>1.55</v>
+        <v>7.02</v>
       </c>
       <c r="AX2">
         <v>0</v>
@@ -915,13 +903,13 @@
         <v>0</v>
       </c>
       <c r="AZ2">
-        <v>0.009606082375478928</v>
+        <v>0</v>
       </c>
       <c r="BA2">
         <v>0</v>
       </c>
       <c r="BB2">
-        <v>0.4927525502177201</v>
+        <v>0.5261400917355202</v>
       </c>
     </row>
     <row r="3" spans="1:54">
@@ -932,142 +920,142 @@
         <v>2023</v>
       </c>
       <c r="D3">
-        <v>224.5</v>
+        <v>222.5</v>
       </c>
       <c r="E3">
-        <v>-14.5</v>
+        <v>-2.5</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H3">
-        <v>0.5714285714285714</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="I3">
-        <v>0.4035087719298245</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="J3">
-        <v>111.6610169491525</v>
+        <v>111.7540983606557</v>
       </c>
       <c r="K3">
-        <v>112.5438596491228</v>
+        <v>117.0847457627119</v>
       </c>
       <c r="L3">
-        <v>94.69322033898304</v>
+        <v>94.58360655737704</v>
       </c>
       <c r="M3">
-        <v>100.5964912280702</v>
+        <v>98.04576271186437</v>
       </c>
       <c r="N3">
-        <v>116.4915254237288</v>
+        <v>116.7819672131148</v>
       </c>
       <c r="O3">
-        <v>111.3105263157895</v>
+        <v>119.0813559322034</v>
       </c>
       <c r="P3">
-        <v>110.457627118644</v>
+        <v>110.9147540983606</v>
       </c>
       <c r="Q3">
-        <v>121.3385964912281</v>
+        <v>114.7254237288136</v>
       </c>
       <c r="R3">
-        <v>78.12881355932201</v>
+        <v>77.94754098360653</v>
       </c>
       <c r="S3">
-        <v>75.28421052631577</v>
+        <v>77.3118644067797</v>
       </c>
       <c r="T3">
-        <v>0.3742711864406779</v>
+        <v>0.3738852459016392</v>
       </c>
       <c r="U3">
-        <v>0.3382105263157894</v>
+        <v>0.3575084745762713</v>
       </c>
       <c r="V3">
-        <v>0.5925254237288136</v>
+        <v>0.5937377049180327</v>
       </c>
       <c r="W3">
-        <v>0.5595438596491228</v>
+        <v>0.6111355932203389</v>
       </c>
       <c r="X3">
-        <v>0.2726440677966102</v>
+        <v>0.2739672131147541</v>
       </c>
       <c r="Y3">
-        <v>0.2357543859649123</v>
+        <v>0.2631186440677966</v>
       </c>
       <c r="Z3">
-        <v>12.12033898305085</v>
+        <v>12.07540983606557</v>
       </c>
       <c r="AA3">
-        <v>13.03859649122807</v>
+        <v>12.8728813559322</v>
       </c>
       <c r="AB3">
-        <v>13.32881355932203</v>
+        <v>13.30819672131148</v>
       </c>
       <c r="AC3">
-        <v>11.62631578947368</v>
+        <v>11.94576271186441</v>
       </c>
       <c r="AD3">
-        <v>0.2082203389830509</v>
+        <v>0.2097704918032787</v>
       </c>
       <c r="AE3">
-        <v>0.1885964912280702</v>
+        <v>0.203864406779661</v>
       </c>
       <c r="AF3">
-        <v>0.9769117843320433</v>
+        <v>0.9777261448876268</v>
       </c>
       <c r="AG3">
-        <v>0.9846356924682661</v>
+        <v>1.02436347998873</v>
       </c>
       <c r="AH3">
-        <v>0.9791540174053835</v>
+        <v>0.9723729890958879</v>
       </c>
       <c r="AI3">
-        <v>0.9922057677318784</v>
+        <v>0.993582320015441</v>
       </c>
       <c r="AJ3">
-        <v>11.28462306015944</v>
+        <v>11.11881544832595</v>
       </c>
       <c r="AK3">
-        <v>10.94334721467812</v>
+        <v>10.6933975124416</v>
       </c>
       <c r="AL3">
-        <v>0.6271186440677966</v>
+        <v>0.6229508196721312</v>
       </c>
       <c r="AM3">
-        <v>0.2456140350877193</v>
+        <v>0.6949152542372882</v>
       </c>
       <c r="AN3">
         <v>46.5</v>
       </c>
       <c r="AO3">
-        <v>22.5</v>
+        <v>51.5</v>
       </c>
       <c r="AP3">
         <v>77.2</v>
       </c>
       <c r="AQ3">
-        <v>73.2</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="AR3">
         <v>0.3076923076923077</v>
       </c>
       <c r="AS3">
-        <v>0.4545454545454545</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="AT3">
-        <v>0.4861200277815768</v>
+        <v>0.4850395075395907</v>
       </c>
       <c r="AU3">
-        <v>0.4997811215277623</v>
+        <v>0.4905401505778892</v>
       </c>
       <c r="AV3">
         <v>2.04</v>
       </c>
       <c r="AW3">
-        <v>0.02</v>
+        <v>2.16</v>
       </c>
       <c r="AX3">
         <v>0</v>
@@ -1076,13 +1064,13 @@
         <v>0</v>
       </c>
       <c r="AZ3">
-        <v>0</v>
+        <v>0.01605874316939891</v>
       </c>
       <c r="BA3">
-        <v>0.224900097465887</v>
+        <v>0.1459345574387947</v>
       </c>
       <c r="BB3">
-        <v>0.4571758231346628</v>
+        <v>0.5469661432241609</v>
       </c>
     </row>
     <row r="4" spans="1:54">
@@ -1093,142 +1081,142 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>225.5</v>
+        <v>227</v>
       </c>
       <c r="E4">
-        <v>-14.5</v>
+        <v>-7</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H4">
-        <v>0.5740740740740741</v>
+        <v>0.5689655172413793</v>
       </c>
       <c r="I4">
-        <v>0.4259259259259259</v>
+        <v>0.4464285714285715</v>
       </c>
       <c r="J4">
-        <v>114.1272727272727</v>
+        <v>110.8983050847458</v>
       </c>
       <c r="K4">
-        <v>110.1071428571429</v>
+        <v>112.271186440678</v>
       </c>
       <c r="L4">
-        <v>96.72727272727275</v>
+        <v>98.11525423728817</v>
       </c>
       <c r="M4">
-        <v>98.74464285714282</v>
+        <v>99.21525423728815</v>
       </c>
       <c r="N4">
-        <v>116.98</v>
+        <v>112.4779661016949</v>
       </c>
       <c r="O4">
-        <v>111.0571428571429</v>
+        <v>112.1745762711864</v>
       </c>
       <c r="P4">
-        <v>113.4072727272728</v>
+        <v>115.2813559322034</v>
       </c>
       <c r="Q4">
-        <v>118.8785714285714</v>
+        <v>119.757627118644</v>
       </c>
       <c r="R4">
-        <v>77.26363636363635</v>
+        <v>76.79322033898305</v>
       </c>
       <c r="S4">
-        <v>75.94999999999997</v>
+        <v>74.21016949152541</v>
       </c>
       <c r="T4">
-        <v>0.3922181818181819</v>
+        <v>0.3609322033898305</v>
       </c>
       <c r="U4">
-        <v>0.3786607142857143</v>
+        <v>0.3809491525423727</v>
       </c>
       <c r="V4">
-        <v>0.6002727272727274</v>
+        <v>0.5776610169491525</v>
       </c>
       <c r="W4">
-        <v>0.5542321428571428</v>
+        <v>0.5650677966101695</v>
       </c>
       <c r="X4">
-        <v>0.2973272727272727</v>
+        <v>0.3009661016949152</v>
       </c>
       <c r="Y4">
-        <v>0.2914464285714285</v>
+        <v>0.3114237288135593</v>
       </c>
       <c r="Z4">
-        <v>11.98363636363636</v>
+        <v>13.12203389830508</v>
       </c>
       <c r="AA4">
-        <v>13.99642857142857</v>
+        <v>12.61864406779661</v>
       </c>
       <c r="AB4">
-        <v>12.92909090909091</v>
+        <v>12.45254237288135</v>
       </c>
       <c r="AC4">
-        <v>11.4125</v>
+        <v>11.91016949152543</v>
       </c>
       <c r="AD4">
-        <v>0.2315363636363636</v>
+        <v>0.2236864406779661</v>
       </c>
       <c r="AE4">
-        <v>0.2183303571428571</v>
+        <v>0.2359152542372881</v>
       </c>
       <c r="AF4">
-        <v>0.9984888252604788</v>
+        <v>0.9702388896303216</v>
       </c>
       <c r="AG4">
-        <v>0.9633170853643295</v>
+        <v>0.9822501000934205</v>
       </c>
       <c r="AH4">
-        <v>0.9317083532473049</v>
+        <v>0.9498191451423914</v>
       </c>
       <c r="AI4">
-        <v>1.038382527840848</v>
+        <v>1.083685587761675</v>
       </c>
       <c r="AJ4">
-        <v>12.08463268400981</v>
+        <v>10.23734425846104</v>
       </c>
       <c r="AK4">
-        <v>10.94414156952831</v>
+        <v>12.15134854547899</v>
       </c>
       <c r="AL4">
-        <v>0.6545454545454545</v>
+        <v>0.4067796610169492</v>
       </c>
       <c r="AM4">
-        <v>0.2321428571428572</v>
+        <v>0.2542372881355932</v>
       </c>
       <c r="AN4">
-        <v>50.5</v>
+        <v>26.5</v>
       </c>
       <c r="AO4">
-        <v>23.5</v>
+        <v>29.5</v>
       </c>
       <c r="AP4">
-        <v>76.2</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="AQ4">
-        <v>73.7</v>
+        <v>74.2</v>
       </c>
       <c r="AR4">
-        <v>0.7142857142857143</v>
+        <v>0.4</v>
       </c>
       <c r="AS4">
-        <v>0.3636363636363636</v>
+        <v>0.3</v>
       </c>
       <c r="AT4">
-        <v>0.4708451456207227</v>
+        <v>0.5150758958270623</v>
       </c>
       <c r="AU4">
-        <v>0.5310040260184871</v>
+        <v>0.5230943868025552</v>
       </c>
       <c r="AV4">
-        <v>2.57</v>
+        <v>-7.67</v>
       </c>
       <c r="AW4">
-        <v>-8.26</v>
+        <v>-7.35</v>
       </c>
       <c r="AX4">
         <v>0</v>
@@ -1240,10 +1228,10 @@
         <v>0</v>
       </c>
       <c r="BA4">
-        <v>0</v>
+        <v>0.01070503766478343</v>
       </c>
       <c r="BB4">
-        <v>0.5072247644815804</v>
+        <v>0.4946058788780239</v>
       </c>
     </row>
     <row r="5" spans="1:54">
@@ -1254,142 +1242,142 @@
         <v>2023</v>
       </c>
       <c r="D5">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E5">
-        <v>-1</v>
+        <v>-3.5</v>
       </c>
       <c r="F5" t="s">
         <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H5">
-        <v>0.5172413793103449</v>
+        <v>0.5892857142857143</v>
       </c>
       <c r="I5">
-        <v>0.543859649122807</v>
+        <v>0.4727272727272727</v>
       </c>
       <c r="J5">
-        <v>114.4137931034483</v>
+        <v>114.3508771929825</v>
       </c>
       <c r="K5">
-        <v>117.5862068965517</v>
+        <v>116.1228070175439</v>
       </c>
       <c r="L5">
-        <v>100.1448275862069</v>
+        <v>96.61403508771932</v>
       </c>
       <c r="M5">
-        <v>99.28793103448275</v>
+        <v>100.8456140350877</v>
       </c>
       <c r="N5">
-        <v>114.2224137931034</v>
+        <v>117.4017543859649</v>
       </c>
       <c r="O5">
-        <v>117.8103448275862</v>
+        <v>114.8263157894737</v>
       </c>
       <c r="P5">
-        <v>116.8551724137931</v>
+        <v>113.4947368421053</v>
       </c>
       <c r="Q5">
-        <v>117.6327586206897</v>
+        <v>110.9526315789474</v>
       </c>
       <c r="R5">
-        <v>72.43275862068967</v>
+        <v>77.05087719298244</v>
       </c>
       <c r="S5">
-        <v>74.52586206896548</v>
+        <v>75.8315789473684</v>
       </c>
       <c r="T5">
-        <v>0.4279137931034481</v>
+        <v>0.3918070175438597</v>
       </c>
       <c r="U5">
-        <v>0.4385172413793104</v>
+        <v>0.3555087719298246</v>
       </c>
       <c r="V5">
-        <v>0.5747068965517242</v>
+        <v>0.6026666666666667</v>
       </c>
       <c r="W5">
-        <v>0.590655172413793</v>
+        <v>0.5628596491228071</v>
       </c>
       <c r="X5">
-        <v>0.2648448275862069</v>
+        <v>0.2970526315789473</v>
       </c>
       <c r="Y5">
-        <v>0.2716896551724138</v>
+        <v>0.274017543859649</v>
       </c>
       <c r="Z5">
-        <v>12.53275862068965</v>
+        <v>12.01929824561403</v>
       </c>
       <c r="AA5">
-        <v>12.71551724137932</v>
+        <v>11.6</v>
       </c>
       <c r="AB5">
-        <v>12.91724137931034</v>
+        <v>12.87017543859649</v>
       </c>
       <c r="AC5">
-        <v>11.30344827586207</v>
+        <v>12.76315789473684</v>
       </c>
       <c r="AD5">
-        <v>0.2230258620689654</v>
+        <v>0.2331578947368421</v>
       </c>
       <c r="AE5">
-        <v>0.2126034482758621</v>
+        <v>0.2004649122807017</v>
       </c>
       <c r="AF5">
-        <v>1.000995565209521</v>
+        <v>1.000445119798622</v>
       </c>
       <c r="AG5">
-        <v>1.028750716505265</v>
+        <v>1.015947567957514</v>
       </c>
       <c r="AH5">
-        <v>0.955595740405867</v>
+        <v>0.9969315741024855</v>
       </c>
       <c r="AI5">
-        <v>1.020527859237537</v>
+        <v>1.016165583925064</v>
       </c>
       <c r="AJ5">
-        <v>10.8723541890598</v>
+        <v>11.93769090497879</v>
       </c>
       <c r="AK5">
-        <v>9.892586013078649</v>
+        <v>11.55470615056548</v>
       </c>
       <c r="AL5">
-        <v>0.4310344827586207</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AM5">
-        <v>0.4827586206896552</v>
+        <v>0.6140350877192983</v>
       </c>
       <c r="AN5">
-        <v>24.5</v>
+        <v>50.5</v>
       </c>
       <c r="AO5">
-        <v>23.5</v>
+        <v>49.5</v>
       </c>
       <c r="AP5">
-        <v>75.90000000000001</v>
+        <v>76.2</v>
       </c>
       <c r="AQ5">
-        <v>74.3</v>
+        <v>75.2</v>
       </c>
       <c r="AR5">
-        <v>0.4444444444444444</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="AS5">
-        <v>0.4761904761904762</v>
+        <v>0.4615384615384616</v>
       </c>
       <c r="AT5">
-        <v>0.4786232524774695</v>
+        <v>0.4695080561336129</v>
       </c>
       <c r="AU5">
-        <v>0.5091581440274026</v>
+        <v>0.4703024102169868</v>
       </c>
       <c r="AV5">
-        <v>-3.26</v>
+        <v>2.57</v>
       </c>
       <c r="AW5">
-        <v>5.67</v>
+        <v>5.37</v>
       </c>
       <c r="AX5">
         <v>0</v>
@@ -1401,10 +1389,10 @@
         <v>0</v>
       </c>
       <c r="BA5">
-        <v>0</v>
+        <v>0.1417312378167641</v>
       </c>
       <c r="BB5">
-        <v>0.4821010929620567</v>
+        <v>0.558836618517463</v>
       </c>
     </row>
     <row r="6" spans="1:54">
@@ -1415,142 +1403,142 @@
         <v>2023</v>
       </c>
       <c r="D6">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="E6">
-        <v>-2.5</v>
+        <v>-6</v>
       </c>
       <c r="F6" t="s">
         <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H6">
-        <v>0.5272727272727272</v>
+        <v>0.4915254237288136</v>
       </c>
       <c r="I6">
-        <v>0.5272727272727272</v>
+        <v>0.4827586206896552</v>
       </c>
       <c r="J6">
-        <v>114.2758620689655</v>
+        <v>113.3220338983051</v>
       </c>
       <c r="K6">
-        <v>114.125</v>
+        <v>114.8983050847458</v>
       </c>
       <c r="L6">
-        <v>95.83793103448276</v>
+        <v>96.78305084745764</v>
       </c>
       <c r="M6">
-        <v>97.74464285714289</v>
+        <v>98.93389830508472</v>
       </c>
       <c r="N6">
-        <v>117.4655172413793</v>
+        <v>116.4254237288136</v>
       </c>
       <c r="O6">
-        <v>116.5875</v>
+        <v>114.9881355932204</v>
       </c>
       <c r="P6">
-        <v>115.7172413793103</v>
+        <v>115.5474576271186</v>
       </c>
       <c r="Q6">
-        <v>114.6125</v>
+        <v>113.5966101694916</v>
       </c>
       <c r="R6">
-        <v>75.93965517241378</v>
+        <v>76.81186440677965</v>
       </c>
       <c r="S6">
-        <v>74.10892857142855</v>
+        <v>77.26440677966103</v>
       </c>
       <c r="T6">
-        <v>0.3916896551724139</v>
+        <v>0.3557796610169492</v>
       </c>
       <c r="U6">
-        <v>0.37975</v>
+        <v>0.3453220338983052</v>
       </c>
       <c r="V6">
-        <v>0.567293103448276</v>
+        <v>0.5583220338983051</v>
       </c>
       <c r="W6">
-        <v>0.6101785714285716</v>
+        <v>0.580864406779661</v>
       </c>
       <c r="X6">
-        <v>0.2887068965517242</v>
+        <v>0.2780847457627119</v>
       </c>
       <c r="Y6">
-        <v>0.2492857142857143</v>
+        <v>0.2866440677966102</v>
       </c>
       <c r="Z6">
-        <v>10.59310344827586</v>
+        <v>10.07627118644068</v>
       </c>
       <c r="AA6">
-        <v>12.54464285714286</v>
+        <v>12.64745762711864</v>
       </c>
       <c r="AB6">
-        <v>10.82586206896552</v>
+        <v>14.53050847457627</v>
       </c>
       <c r="AC6">
-        <v>11.5875</v>
+        <v>12.93728813559322</v>
       </c>
       <c r="AD6">
-        <v>0.2175689655172414</v>
+        <v>0.2238220338983051</v>
       </c>
       <c r="AE6">
-        <v>0.2118482142857143</v>
+        <v>0.2183389830508474</v>
       </c>
       <c r="AF6">
-        <v>0.9997888195010107</v>
+        <v>0.9914438661269036</v>
       </c>
       <c r="AG6">
-        <v>0.9984689413823272</v>
+        <v>1.005234515177128</v>
       </c>
       <c r="AH6">
-        <v>0.980084490042245</v>
+        <v>1.053046166118257</v>
       </c>
       <c r="AI6">
-        <v>0.9521723256663016</v>
+        <v>0.9051482519545656</v>
       </c>
       <c r="AJ6">
-        <v>11.04659895147679</v>
+        <v>10.2402341703331</v>
       </c>
       <c r="AK6">
-        <v>11.29485107092102</v>
+        <v>10.34603815969372</v>
       </c>
       <c r="AL6">
-        <v>0.5344827586206896</v>
+        <v>0.4745762711864407</v>
       </c>
       <c r="AM6">
-        <v>0.5892857142857143</v>
+        <v>0.5084745762711864</v>
       </c>
       <c r="AN6">
-        <v>38.5</v>
+        <v>46.5</v>
       </c>
       <c r="AO6">
-        <v>50.5</v>
+        <v>45.5</v>
       </c>
       <c r="AP6">
-        <v>75.8</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="AQ6">
-        <v>76.5</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="AR6">
-        <v>0.6111111111111112</v>
+        <v>0.3157894736842105</v>
       </c>
       <c r="AS6">
-        <v>0.6470588235294118</v>
+        <v>0.5</v>
       </c>
       <c r="AT6">
-        <v>0.5017457426789564</v>
+        <v>0.4555862237270019</v>
       </c>
       <c r="AU6">
-        <v>0.5040731123913106</v>
+        <v>0.5203230998601887</v>
       </c>
       <c r="AV6">
-        <v>-0.01</v>
+        <v>2.37</v>
       </c>
       <c r="AW6">
-        <v>0.82</v>
+        <v>-0.84</v>
       </c>
       <c r="AX6">
         <v>0</v>
@@ -1559,13 +1547,13 @@
         <v>0</v>
       </c>
       <c r="AZ6">
-        <v>0.0734183429118774</v>
+        <v>0</v>
       </c>
       <c r="BA6">
-        <v>0.06725074404761905</v>
+        <v>0.06752354048964218</v>
       </c>
       <c r="BB6">
-        <v>0.5352555232354393</v>
+        <v>0.5232730061438239</v>
       </c>
     </row>
     <row r="7" spans="1:54">
@@ -1576,142 +1564,142 @@
         <v>2023</v>
       </c>
       <c r="D7">
-        <v>220.5</v>
+        <v>237.5</v>
       </c>
       <c r="E7">
-        <v>-1.5</v>
+        <v>-14.5</v>
       </c>
       <c r="F7" t="s">
         <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H7">
-        <v>0.3888888888888889</v>
+        <v>0.3684210526315789</v>
       </c>
       <c r="I7">
-        <v>0.5357142857142857</v>
+        <v>0.4067796610169492</v>
       </c>
       <c r="J7">
-        <v>108.4035087719298</v>
+        <v>113</v>
       </c>
       <c r="K7">
-        <v>117.1578947368421</v>
+        <v>112.4406779661017</v>
       </c>
       <c r="L7">
-        <v>96.07894736842105</v>
+        <v>95.02500000000002</v>
       </c>
       <c r="M7">
-        <v>98.19824561403506</v>
+        <v>100.5762711864407</v>
       </c>
       <c r="N7">
-        <v>112.080701754386</v>
+        <v>117.3116666666667</v>
       </c>
       <c r="O7">
-        <v>118.9526315789474</v>
+        <v>111.2661016949153</v>
       </c>
       <c r="P7">
-        <v>111.8228070175439</v>
+        <v>116.83</v>
       </c>
       <c r="Q7">
-        <v>114.6842105263158</v>
+        <v>121.2593220338983</v>
       </c>
       <c r="R7">
-        <v>78.37543859649125</v>
+        <v>76.42000000000002</v>
       </c>
       <c r="S7">
-        <v>77.1368421052632</v>
+        <v>75.11016949152541</v>
       </c>
       <c r="T7">
-        <v>0.4056140350877192</v>
+        <v>0.4868166666666666</v>
       </c>
       <c r="U7">
-        <v>0.357122807017544</v>
+        <v>0.3369491525423728</v>
       </c>
       <c r="V7">
-        <v>0.5641929824561404</v>
+        <v>0.5973000000000002</v>
       </c>
       <c r="W7">
-        <v>0.6092631578947367</v>
+        <v>0.5584745762711865</v>
       </c>
       <c r="X7">
-        <v>0.2632631578947368</v>
+        <v>0.3168999999999999</v>
       </c>
       <c r="Y7">
-        <v>0.2657543859649122</v>
+        <v>0.2349152542372881</v>
       </c>
       <c r="Z7">
-        <v>11.74736842105264</v>
+        <v>11.09166666666667</v>
       </c>
       <c r="AA7">
-        <v>12.86666666666666</v>
+        <v>13.03898305084745</v>
       </c>
       <c r="AB7">
-        <v>14.61578947368421</v>
+        <v>11.795</v>
       </c>
       <c r="AC7">
-        <v>12.02982456140351</v>
+        <v>11.66779661016949</v>
       </c>
       <c r="AD7">
-        <v>0.2098508771929825</v>
+        <v>0.235175</v>
       </c>
       <c r="AE7">
-        <v>0.2048245614035088</v>
+        <v>0.1888135593220338</v>
       </c>
       <c r="AF7">
-        <v>0.9484121502356065</v>
+        <v>0.9886264216972879</v>
       </c>
       <c r="AG7">
-        <v>1.025003453515679</v>
+        <v>0.983732965582692</v>
       </c>
       <c r="AH7">
-        <v>0.9839779899660139</v>
+        <v>1.056047197640118</v>
       </c>
       <c r="AI7">
-        <v>1.049865229110512</v>
+        <v>0.9634710079389006</v>
       </c>
       <c r="AJ7">
-        <v>9.224033537778547</v>
+        <v>11.5123122496453</v>
       </c>
       <c r="AK7">
-        <v>10.85759411443585</v>
+        <v>10.7707563690161</v>
       </c>
       <c r="AL7">
-        <v>0.5614035087719298</v>
+        <v>0.5166666666666667</v>
       </c>
       <c r="AM7">
-        <v>0.6842105263157895</v>
+        <v>0.2372881355932203</v>
       </c>
       <c r="AN7">
-        <v>49.5</v>
+        <v>48.5</v>
       </c>
       <c r="AO7">
-        <v>51.5</v>
+        <v>22.5</v>
       </c>
       <c r="AP7">
-        <v>76.2</v>
+        <v>75.3</v>
       </c>
       <c r="AQ7">
-        <v>75.09999999999999</v>
+        <v>73.2</v>
       </c>
       <c r="AR7">
-        <v>0.6451612903225806</v>
+        <v>0.625</v>
       </c>
       <c r="AS7">
-        <v>0.7222222222222222</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="AT7">
-        <v>0.497360457755521</v>
+        <v>0.4983191914194789</v>
       </c>
       <c r="AU7">
-        <v>0.4886849411668416</v>
+        <v>0.4980648985055629</v>
       </c>
       <c r="AV7">
-        <v>4.23</v>
+        <v>3.12</v>
       </c>
       <c r="AW7">
-        <v>2.16</v>
+        <v>0.02</v>
       </c>
       <c r="AX7">
         <v>0</v>
@@ -1720,13 +1708,13 @@
         <v>0</v>
       </c>
       <c r="AZ7">
-        <v>0.2125828460038986</v>
+        <v>0.06420833333333334</v>
       </c>
       <c r="BA7">
-        <v>0.04266081871345029</v>
+        <v>0.1430767419962335</v>
       </c>
       <c r="BB7">
-        <v>0.5563048688766261</v>
+        <v>0.4274377413206152</v>
       </c>
     </row>
     <row r="8" spans="1:54">
@@ -1737,142 +1725,142 @@
         <v>2023</v>
       </c>
       <c r="D8">
-        <v>226</v>
+        <v>240.5</v>
       </c>
       <c r="E8">
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="F8" t="s">
         <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H8">
-        <v>0.5185185185185185</v>
+        <v>0.559322033898305</v>
       </c>
       <c r="I8">
-        <v>0.5714285714285714</v>
+        <v>0.625</v>
       </c>
       <c r="J8">
-        <v>113.7142857142857</v>
+        <v>117.5666666666667</v>
       </c>
       <c r="K8">
-        <v>111.0526315789474</v>
+        <v>117.8947368421053</v>
       </c>
       <c r="L8">
-        <v>99.07321428571427</v>
+        <v>99.36333333333333</v>
       </c>
       <c r="M8">
-        <v>98.14912280701758</v>
+        <v>100.5754385964912</v>
       </c>
       <c r="N8">
-        <v>113.8142857142857</v>
+        <v>117.7283333333333</v>
       </c>
       <c r="O8">
-        <v>112.5771929824561</v>
+        <v>116</v>
       </c>
       <c r="P8">
-        <v>113.6571428571429</v>
+        <v>117.5533333333333</v>
       </c>
       <c r="Q8">
-        <v>115.4596491228071</v>
+        <v>114.4017543859649</v>
       </c>
       <c r="R8">
-        <v>78.44821428571427</v>
+        <v>74.61499999999997</v>
       </c>
       <c r="S8">
-        <v>77.05964912280702</v>
+        <v>72.91754385964914</v>
       </c>
       <c r="T8">
-        <v>0.3316428571428571</v>
+        <v>0.4369666666666667</v>
       </c>
       <c r="U8">
-        <v>0.361280701754386</v>
+        <v>0.3608070175438597</v>
       </c>
       <c r="V8">
-        <v>0.588375</v>
+        <v>0.5909666666666664</v>
       </c>
       <c r="W8">
-        <v>0.5773157894736841</v>
+        <v>0.5752982456140349</v>
       </c>
       <c r="X8">
-        <v>0.2592678571428572</v>
+        <v>0.2710166666666666</v>
       </c>
       <c r="Y8">
-        <v>0.3036491228070175</v>
+        <v>0.2529649122807018</v>
       </c>
       <c r="Z8">
-        <v>12.15</v>
+        <v>12.86833333333334</v>
       </c>
       <c r="AA8">
-        <v>13.0140350877193</v>
+        <v>11.20701754385965</v>
       </c>
       <c r="AB8">
-        <v>12.42500000000001</v>
+        <v>11.14666666666667</v>
       </c>
       <c r="AC8">
-        <v>12.34736842105263</v>
+        <v>13.91929824561404</v>
       </c>
       <c r="AD8">
-        <v>0.2073482142857143</v>
+        <v>0.2116583333333334</v>
       </c>
       <c r="AE8">
-        <v>0.2249122807017544</v>
+        <v>0.2164649122807017</v>
       </c>
       <c r="AF8">
-        <v>0.9948756405449318</v>
+        <v>1.028579760863225</v>
       </c>
       <c r="AG8">
-        <v>0.9715890776810794</v>
+        <v>1.031450016116406</v>
       </c>
       <c r="AH8">
-        <v>0.8295644891122278</v>
+        <v>1.003685851998866</v>
       </c>
       <c r="AI8">
-        <v>0.9484992101105845</v>
+        <v>1.048958333333333</v>
       </c>
       <c r="AJ8">
-        <v>11.83776385392209</v>
+        <v>9.788371786064435</v>
       </c>
       <c r="AK8">
-        <v>10.30996971532567</v>
+        <v>12.99484946623262</v>
       </c>
       <c r="AL8">
-        <v>0.4642857142857143</v>
+        <v>0.4833333333333333</v>
       </c>
       <c r="AM8">
-        <v>0.4035087719298245</v>
+        <v>0.4912280701754386</v>
       </c>
       <c r="AN8">
-        <v>41.5</v>
+        <v>23.5</v>
       </c>
       <c r="AO8">
-        <v>26.5</v>
+        <v>23.5</v>
       </c>
       <c r="AP8">
-        <v>76.40000000000001</v>
+        <v>74.3</v>
       </c>
       <c r="AQ8">
-        <v>74.59999999999999</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="AR8">
-        <v>0.2666666666666667</v>
+        <v>0.4761904761904762</v>
       </c>
       <c r="AS8">
-        <v>0.4</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AT8">
-        <v>0.5014265243554643</v>
+        <v>0.5094891615581804</v>
       </c>
       <c r="AU8">
-        <v>0.5168364017216078</v>
+        <v>0.505926743154552</v>
       </c>
       <c r="AV8">
-        <v>-0.37</v>
+        <v>5.67</v>
       </c>
       <c r="AW8">
-        <v>-7.67</v>
+        <v>-7.9</v>
       </c>
       <c r="AX8">
         <v>0</v>
@@ -1881,13 +1869,13 @@
         <v>0</v>
       </c>
       <c r="AZ8">
-        <v>0.03342509920634921</v>
+        <v>0.07842939814814817</v>
       </c>
       <c r="BA8">
-        <v>0.02835953878406708</v>
+        <v>0.04952119883040936</v>
       </c>
       <c r="BB8">
-        <v>0.4977675346567421</v>
+        <v>0.4755294624178618</v>
       </c>
     </row>
     <row r="9" spans="1:54">
@@ -1898,142 +1886,142 @@
         <v>2023</v>
       </c>
       <c r="D9">
-        <v>237</v>
+        <v>238.5</v>
       </c>
       <c r="E9">
-        <v>-3</v>
+        <v>-6</v>
       </c>
       <c r="F9" t="s">
         <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H9">
-        <v>0.6296296296296297</v>
+        <v>0.4655172413793103</v>
       </c>
       <c r="I9">
-        <v>0.4821428571428572</v>
+        <v>0.456140350877193</v>
       </c>
       <c r="J9">
-        <v>117.9454545454546</v>
+        <v>117.0169491525424</v>
       </c>
       <c r="K9">
-        <v>115.3333333333333</v>
+        <v>118.6206896551724</v>
       </c>
       <c r="L9">
-        <v>100.6054545454545</v>
+        <v>101.3084745762712</v>
       </c>
       <c r="M9">
-        <v>98.9754385964912</v>
+        <v>101.4827586206897</v>
       </c>
       <c r="N9">
-        <v>115.9890909090909</v>
+        <v>114.3254237288136</v>
       </c>
       <c r="O9">
-        <v>115.3385964912281</v>
+        <v>116.0172413793103</v>
       </c>
       <c r="P9">
-        <v>114.9181818181818</v>
+        <v>115.4864406779661</v>
       </c>
       <c r="Q9">
-        <v>113.6421052631579</v>
+        <v>115.9689655172414</v>
       </c>
       <c r="R9">
-        <v>72.63272727272728</v>
+        <v>76.23559322033896</v>
       </c>
       <c r="S9">
-        <v>77.2842105263158</v>
+        <v>76.16551724137929</v>
       </c>
       <c r="T9">
-        <v>0.3601454545454545</v>
+        <v>0.3448474576271187</v>
       </c>
       <c r="U9">
-        <v>0.34540350877193</v>
+        <v>0.4778793103448276</v>
       </c>
       <c r="V9">
-        <v>0.5756909090909088</v>
+        <v>0.5796101694915253</v>
       </c>
       <c r="W9">
-        <v>0.5812280701754386</v>
+        <v>0.6011551724137929</v>
       </c>
       <c r="X9">
-        <v>0.2487090909090909</v>
+        <v>0.2917627118644069</v>
       </c>
       <c r="Y9">
-        <v>0.2877017543859649</v>
+        <v>0.2244827586206897</v>
       </c>
       <c r="Z9">
-        <v>11.20545454545455</v>
+        <v>11.7135593220339</v>
       </c>
       <c r="AA9">
-        <v>12.54561403508772</v>
+        <v>13.76724137931034</v>
       </c>
       <c r="AB9">
-        <v>13.84545454545455</v>
+        <v>10.59491525423729</v>
       </c>
       <c r="AC9">
-        <v>12.98421052631579</v>
+        <v>12.12413793103449</v>
       </c>
       <c r="AD9">
-        <v>0.2140181818181818</v>
+        <v>0.2045932203389831</v>
       </c>
       <c r="AE9">
-        <v>0.218640350877193</v>
+        <v>0.2018534482758621</v>
       </c>
       <c r="AF9">
-        <v>1.031893740555158</v>
+        <v>1.023770333793022</v>
       </c>
       <c r="AG9">
-        <v>1.009040536599592</v>
+        <v>1.037801309319094</v>
       </c>
       <c r="AH9">
-        <v>1.088073583063563</v>
+        <v>0.9799150251062188</v>
       </c>
       <c r="AI9">
-        <v>1.03757225433526</v>
+        <v>1.017248062015504</v>
       </c>
       <c r="AJ9">
-        <v>12.84653215579022</v>
+        <v>10.85574365731555</v>
       </c>
       <c r="AK9">
-        <v>10.25693318504967</v>
+        <v>11.23391967429506</v>
       </c>
       <c r="AL9">
-        <v>0.4909090909090909</v>
+        <v>0.4576271186440678</v>
       </c>
       <c r="AM9">
-        <v>0.5087719298245614</v>
+        <v>0.5</v>
       </c>
       <c r="AN9">
-        <v>23.5</v>
+        <v>44.5</v>
       </c>
       <c r="AO9">
-        <v>45.5</v>
+        <v>52.5</v>
       </c>
       <c r="AP9">
-        <v>74.40000000000001</v>
+        <v>75</v>
       </c>
       <c r="AQ9">
-        <v>77.40000000000001</v>
+        <v>76.3</v>
       </c>
       <c r="AR9">
-        <v>0.3529411764705883</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="AS9">
-        <v>0.4666666666666667</v>
+        <v>0.4375</v>
       </c>
       <c r="AT9">
-        <v>0.5109269500826601</v>
+        <v>0.5087168190972892</v>
       </c>
       <c r="AU9">
-        <v>0.522103121732861</v>
+        <v>0.4676985007366004</v>
       </c>
       <c r="AV9">
-        <v>-7.9</v>
+        <v>-3.08</v>
       </c>
       <c r="AW9">
-        <v>-0.84</v>
+        <v>5.52</v>
       </c>
       <c r="AX9">
         <v>0</v>
@@ -2042,13 +2030,13 @@
         <v>0</v>
       </c>
       <c r="AZ9">
-        <v>0.0513219696969697</v>
+        <v>0</v>
       </c>
       <c r="BA9">
-        <v>0.06989278752436646</v>
+        <v>0.1828556034482759</v>
       </c>
       <c r="BB9">
-        <v>0.4854646746695784</v>
+        <v>0.457110219249547</v>
       </c>
     </row>
     <row r="10" spans="1:54">
@@ -2059,142 +2047,142 @@
         <v>2023</v>
       </c>
       <c r="D10">
-        <v>232.5</v>
+        <v>240.5</v>
       </c>
       <c r="E10">
-        <v>-7.5</v>
+        <v>-6</v>
       </c>
       <c r="F10" t="s">
         <v>61</v>
       </c>
       <c r="G10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H10">
-        <v>0.3818181818181818</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="I10">
-        <v>0.4745762711864407</v>
+        <v>0.5172413793103449</v>
       </c>
       <c r="J10">
-        <v>112.9310344827586</v>
+        <v>119.4561403508772</v>
       </c>
       <c r="K10">
-        <v>115.728813559322</v>
+        <v>114.8793103448276</v>
       </c>
       <c r="L10">
-        <v>95.01379310344829</v>
+        <v>100.0842105263158</v>
       </c>
       <c r="M10">
-        <v>100.7152542372881</v>
+        <v>97.04827586206892</v>
       </c>
       <c r="N10">
-        <v>117.1948275862069</v>
+        <v>118.7192982456141</v>
       </c>
       <c r="O10">
-        <v>114.4084745762712</v>
+        <v>117.9603448275862</v>
       </c>
       <c r="P10">
-        <v>116.4810344827586</v>
+        <v>116.6491228070176</v>
       </c>
       <c r="Q10">
-        <v>114.3101694915254</v>
+        <v>118.2810344827586</v>
       </c>
       <c r="R10">
-        <v>76.44827586206897</v>
+        <v>77.19298245614037</v>
       </c>
       <c r="S10">
-        <v>73.97457627118642</v>
+        <v>76.11724137931034</v>
       </c>
       <c r="T10">
-        <v>0.4876034482758621</v>
+        <v>0.4160350877192981</v>
       </c>
       <c r="U10">
-        <v>0.3866440677966103</v>
+        <v>0.4119655172413793</v>
       </c>
       <c r="V10">
-        <v>0.5970000000000001</v>
+        <v>0.6081929824561403</v>
       </c>
       <c r="W10">
-        <v>0.5972203389830509</v>
+        <v>0.600741379310345</v>
       </c>
       <c r="X10">
-        <v>0.3177758620689655</v>
+        <v>0.2870701754385966</v>
       </c>
       <c r="Y10">
-        <v>0.2729830508474576</v>
+        <v>0.3012586206896552</v>
       </c>
       <c r="Z10">
-        <v>11.12931034482758</v>
+        <v>12.18245614035087</v>
       </c>
       <c r="AA10">
-        <v>13.51694915254237</v>
+        <v>12.60689655172414</v>
       </c>
       <c r="AB10">
-        <v>11.79137931034483</v>
+        <v>12.3</v>
       </c>
       <c r="AC10">
-        <v>13.23559322033898</v>
+        <v>11.49827586206897</v>
       </c>
       <c r="AD10">
-        <v>0.2361810344827586</v>
+        <v>0.2159385964912281</v>
       </c>
       <c r="AE10">
-        <v>0.2185508474576271</v>
+        <v>0.2303879310344828</v>
       </c>
       <c r="AF10">
-        <v>0.9880230488430326</v>
+        <v>1.04511058924652</v>
       </c>
       <c r="AG10">
-        <v>1.012500556074559</v>
+        <v>1.005068331975745</v>
       </c>
       <c r="AH10">
-        <v>1.062595419847328</v>
+        <v>0.9933911000146864</v>
       </c>
       <c r="AI10">
-        <v>1.042667447764109</v>
+        <v>1.035869728350593</v>
       </c>
       <c r="AJ10">
-        <v>11.64986616611822</v>
+        <v>12.06425803542074</v>
       </c>
       <c r="AK10">
-        <v>10.59713825852643</v>
+        <v>12.8090452768224</v>
       </c>
       <c r="AL10">
-        <v>0.5344827586206896</v>
+        <v>0.5614035087719298</v>
       </c>
       <c r="AM10">
-        <v>0.5084745762711864</v>
+        <v>0.4827586206896552</v>
       </c>
       <c r="AN10">
-        <v>48.5</v>
+        <v>34.5</v>
       </c>
       <c r="AO10">
-        <v>49.5</v>
+        <v>39.5</v>
       </c>
       <c r="AP10">
-        <v>75.3</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="AQ10">
-        <v>75.7</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="AR10">
-        <v>0.6521739130434783</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="AS10">
         <v>0.5</v>
       </c>
       <c r="AT10">
-        <v>0.4948452023531681</v>
+        <v>0.4718078380778777</v>
       </c>
       <c r="AU10">
-        <v>0.5072308985866205</v>
+        <v>0.4889632915169508</v>
       </c>
       <c r="AV10">
-        <v>3.12</v>
+        <v>-5.26</v>
       </c>
       <c r="AW10">
-        <v>2.53</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="AX10">
         <v>0</v>
@@ -2203,335 +2191,13 @@
         <v>0</v>
       </c>
       <c r="AZ10">
-        <v>0.06642241379310346</v>
+        <v>0.01811525341130604</v>
       </c>
       <c r="BA10">
-        <v>0.0500765065913371</v>
+        <v>0.2868235153256705</v>
       </c>
       <c r="BB10">
-        <v>0.5045813821174125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:54">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>2023</v>
-      </c>
-      <c r="D11">
-        <v>233.5</v>
-      </c>
-      <c r="E11">
-        <v>-4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11">
-        <v>0.4545454545454545</v>
-      </c>
-      <c r="I11">
-        <v>0.5</v>
-      </c>
-      <c r="J11">
-        <v>118.2321428571429</v>
-      </c>
-      <c r="K11">
-        <v>113.1818181818182</v>
-      </c>
-      <c r="L11">
-        <v>101.6875</v>
-      </c>
-      <c r="M11">
-        <v>98.25090909090913</v>
-      </c>
-      <c r="N11">
-        <v>115.3303571428571</v>
-      </c>
-      <c r="O11">
-        <v>114.9272727272727</v>
-      </c>
-      <c r="P11">
-        <v>115.2607142857143</v>
-      </c>
-      <c r="Q11">
-        <v>115.06</v>
-      </c>
-      <c r="R11">
-        <v>76.3517857142857</v>
-      </c>
-      <c r="S11">
-        <v>76.68545454545456</v>
-      </c>
-      <c r="T11">
-        <v>0.4796071428571428</v>
-      </c>
-      <c r="U11">
-        <v>0.3656909090909092</v>
-      </c>
-      <c r="V11">
-        <v>0.5983571428571427</v>
-      </c>
-      <c r="W11">
-        <v>0.585</v>
-      </c>
-      <c r="X11">
-        <v>0.2236785714285715</v>
-      </c>
-      <c r="Y11">
-        <v>0.2737454545454545</v>
-      </c>
-      <c r="Z11">
-        <v>13.83035714285714</v>
-      </c>
-      <c r="AA11">
-        <v>12.08727272727273</v>
-      </c>
-      <c r="AB11">
-        <v>12.14107142857143</v>
-      </c>
-      <c r="AC11">
-        <v>10.48909090909091</v>
-      </c>
-      <c r="AD11">
-        <v>0.2020535714285714</v>
-      </c>
-      <c r="AE11">
-        <v>0.2091</v>
-      </c>
-      <c r="AF11">
-        <v>1.034401949756281</v>
-      </c>
-      <c r="AG11">
-        <v>0.9902171319494155</v>
-      </c>
-      <c r="AH11">
-        <v>1.031868297840205</v>
-      </c>
-      <c r="AI11">
-        <v>0.9895582329317268</v>
-      </c>
-      <c r="AJ11">
-        <v>11.1915003963923</v>
-      </c>
-      <c r="AK11">
-        <v>10.80755780854879</v>
-      </c>
-      <c r="AL11">
-        <v>0.5</v>
-      </c>
-      <c r="AM11">
-        <v>0.4727272727272727</v>
-      </c>
-      <c r="AN11">
-        <v>52.5</v>
-      </c>
-      <c r="AO11">
-        <v>35.5</v>
-      </c>
-      <c r="AP11">
-        <v>76.3</v>
-      </c>
-      <c r="AQ11">
-        <v>76.09999999999999</v>
-      </c>
-      <c r="AR11">
-        <v>0.4375</v>
-      </c>
-      <c r="AS11">
-        <v>0.5333333333333333</v>
-      </c>
-      <c r="AT11">
-        <v>0.4665778935925355</v>
-      </c>
-      <c r="AU11">
-        <v>0.4885297006723326</v>
-      </c>
-      <c r="AV11">
-        <v>5.52</v>
-      </c>
-      <c r="AW11">
-        <v>-3.23</v>
-      </c>
-      <c r="AX11">
-        <v>0</v>
-      </c>
-      <c r="AY11">
-        <v>0</v>
-      </c>
-      <c r="AZ11">
-        <v>0.1008246527777778</v>
-      </c>
-      <c r="BA11">
-        <v>0</v>
-      </c>
-      <c r="BB11">
-        <v>0.5080132763719982</v>
-      </c>
-    </row>
-    <row r="12" spans="1:54">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>2023</v>
-      </c>
-      <c r="D12">
-        <v>238</v>
-      </c>
-      <c r="E12">
-        <v>-2.5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12">
-        <v>0.5178571428571429</v>
-      </c>
-      <c r="I12">
-        <v>0.4642857142857143</v>
-      </c>
-      <c r="J12">
-        <v>114.9107142857143</v>
-      </c>
-      <c r="K12">
-        <v>117</v>
-      </c>
-      <c r="L12">
-        <v>97.02142857142853</v>
-      </c>
-      <c r="M12">
-        <v>101.340350877193</v>
-      </c>
-      <c r="N12">
-        <v>118.0178571428571</v>
-      </c>
-      <c r="O12">
-        <v>114.2315789473684</v>
-      </c>
-      <c r="P12">
-        <v>118.0964285714285</v>
-      </c>
-      <c r="Q12">
-        <v>115.5350877192983</v>
-      </c>
-      <c r="R12">
-        <v>76.08392857142857</v>
-      </c>
-      <c r="S12">
-        <v>76.13859649122804</v>
-      </c>
-      <c r="T12">
-        <v>0.4093035714285714</v>
-      </c>
-      <c r="U12">
-        <v>0.3422982456140351</v>
-      </c>
-      <c r="V12">
-        <v>0.6018214285714286</v>
-      </c>
-      <c r="W12">
-        <v>0.5796140350877192</v>
-      </c>
-      <c r="X12">
-        <v>0.3046428571428572</v>
-      </c>
-      <c r="Y12">
-        <v>0.2905087719298247</v>
-      </c>
-      <c r="Z12">
-        <v>12.74464285714286</v>
-      </c>
-      <c r="AA12">
-        <v>11.76842105263158</v>
-      </c>
-      <c r="AB12">
-        <v>11.46785714285714</v>
-      </c>
-      <c r="AC12">
-        <v>10.62456140350877</v>
-      </c>
-      <c r="AD12">
-        <v>0.2318035714285715</v>
-      </c>
-      <c r="AE12">
-        <v>0.2049298245614035</v>
-      </c>
-      <c r="AF12">
-        <v>1.005343082114736</v>
-      </c>
-      <c r="AG12">
-        <v>1.023622047244094</v>
-      </c>
-      <c r="AH12">
-        <v>1.05009065009065</v>
-      </c>
-      <c r="AI12">
-        <v>0.9829059829059829</v>
-      </c>
-      <c r="AJ12">
-        <v>12.80105574010302</v>
-      </c>
-      <c r="AK12">
-        <v>11.03423699060847</v>
-      </c>
-      <c r="AL12">
-        <v>0.4821428571428572</v>
-      </c>
-      <c r="AM12">
-        <v>0.456140350877193</v>
-      </c>
-      <c r="AN12">
-        <v>39.5</v>
-      </c>
-      <c r="AO12">
-        <v>44.5</v>
-      </c>
-      <c r="AP12">
-        <v>75.09999999999999</v>
-      </c>
-      <c r="AQ12">
-        <v>75</v>
-      </c>
-      <c r="AR12">
-        <v>0.5</v>
-      </c>
-      <c r="AS12">
-        <v>0.4444444444444444</v>
-      </c>
-      <c r="AT12">
-        <v>0.4899900864789329</v>
-      </c>
-      <c r="AU12">
-        <v>0.5090334752681904</v>
-      </c>
-      <c r="AV12">
-        <v>-8.550000000000001</v>
-      </c>
-      <c r="AW12">
-        <v>-3.08</v>
-      </c>
-      <c r="AX12">
-        <v>0</v>
-      </c>
-      <c r="AY12">
-        <v>0</v>
-      </c>
-      <c r="AZ12">
-        <v>0.09126116071428569</v>
-      </c>
-      <c r="BA12">
-        <v>0</v>
-      </c>
-      <c r="BB12">
-        <v>0.5405309416319272</v>
+        <v>0.5219576120000876</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
totals machine learning model v1 done!
</commit_message>
<xml_diff>
--- a/current_games_spread.xlsx
+++ b/current_games_spread.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>year</t>
   </si>
@@ -175,58 +175,40 @@
     <t>calc_home_prob</t>
   </si>
   <si>
-    <t>Indiana</t>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>SanAntonio</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>LALakers</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Denver</t>
   </si>
   <si>
     <t>Cleveland</t>
   </si>
   <si>
-    <t>Orlando</t>
-  </si>
-  <si>
-    <t>Philadelphia</t>
-  </si>
-  <si>
     <t>Toronto</t>
-  </si>
-  <si>
-    <t>Dallas</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>LALakers</t>
-  </si>
-  <si>
-    <t>Sacramento</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>Denver</t>
-  </si>
-  <si>
-    <t>Detroit</t>
-  </si>
-  <si>
-    <t>Memphis</t>
-  </si>
-  <si>
-    <t>NewOrleans</t>
-  </si>
-  <si>
-    <t>SanAntonio</t>
-  </si>
-  <si>
-    <t>OklahomaCity</t>
-  </si>
-  <si>
-    <t>GoldenState</t>
-  </si>
-  <si>
-    <t>Portland</t>
   </si>
 </sst>
 </file>
@@ -584,7 +566,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB10"/>
+  <dimension ref="A1:BB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -759,142 +741,142 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>232.5</v>
+        <v>238</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>1.5</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H2">
-        <v>0.5166666666666667</v>
+        <v>0.492063492063492</v>
       </c>
       <c r="I2">
-        <v>0.559322033898305</v>
+        <v>0.4461538461538462</v>
       </c>
       <c r="J2">
-        <v>114.5</v>
+        <v>113.3181818181818</v>
       </c>
       <c r="K2">
-        <v>117.864406779661</v>
+        <v>117.2121212121212</v>
       </c>
       <c r="L2">
-        <v>100.1333333333333</v>
+        <v>97.73484848484851</v>
       </c>
       <c r="M2">
-        <v>97.97118644067795</v>
+        <v>99.81363636363636</v>
       </c>
       <c r="N2">
-        <v>114.3233333333333</v>
+        <v>115.5484848484848</v>
       </c>
       <c r="O2">
-        <v>118.8779661016949</v>
+        <v>116.5969696969697</v>
       </c>
       <c r="P2">
-        <v>116.9033333333334</v>
+        <v>115.7136363636364</v>
       </c>
       <c r="Q2">
-        <v>112.471186440678</v>
+        <v>116.5227272727273</v>
       </c>
       <c r="R2">
-        <v>72.58500000000001</v>
+        <v>76.3878787878788</v>
       </c>
       <c r="S2">
-        <v>79.24406779661018</v>
+        <v>75.90303030303029</v>
       </c>
       <c r="T2">
-        <v>0.4286166666666665</v>
+        <v>0.3638181818181819</v>
       </c>
       <c r="U2">
-        <v>0.4795762711864405</v>
+        <v>0.3316969696969697</v>
       </c>
       <c r="V2">
-        <v>0.5759500000000001</v>
+        <v>0.5898484848484846</v>
       </c>
       <c r="W2">
-        <v>0.6039322033898304</v>
+        <v>0.5795454545454549</v>
       </c>
       <c r="X2">
-        <v>0.2641500000000001</v>
+        <v>0.2657878787878787</v>
       </c>
       <c r="Y2">
-        <v>0.2538474576271187</v>
+        <v>0.2420606060606061</v>
       </c>
       <c r="Z2">
-        <v>12.54</v>
+        <v>12.4030303030303</v>
       </c>
       <c r="AA2">
-        <v>11.67966101694916</v>
+        <v>10.83181818181818</v>
       </c>
       <c r="AB2">
-        <v>12.95333333333333</v>
+        <v>10.62121212121212</v>
       </c>
       <c r="AC2">
-        <v>10.70677966101695</v>
+        <v>12.06666666666666</v>
       </c>
       <c r="AD2">
-        <v>0.2227499999999999</v>
+        <v>0.2044924242424242</v>
       </c>
       <c r="AE2">
-        <v>0.194906779661017</v>
+        <v>0.2080909090909091</v>
       </c>
       <c r="AF2">
-        <v>1.00174978127734</v>
+        <v>0.9896784438269154</v>
       </c>
       <c r="AG2">
-        <v>1.031184661239379</v>
+        <v>1.023686648140797</v>
       </c>
       <c r="AH2">
-        <v>1.01018922852984</v>
+        <v>1.029549405000669</v>
       </c>
       <c r="AI2">
-        <v>1.04922826191161</v>
+        <v>1.020941054808687</v>
       </c>
       <c r="AJ2">
-        <v>10.69968846898513</v>
+        <v>10.94913735485252</v>
       </c>
       <c r="AK2">
-        <v>11.44842173582498</v>
+        <v>11.00484074136847</v>
       </c>
       <c r="AL2">
-        <v>0.4333333333333333</v>
+        <v>0.4696969696969697</v>
       </c>
       <c r="AM2">
-        <v>0.711864406779661</v>
+        <v>0.5</v>
       </c>
       <c r="AN2">
-        <v>24.5</v>
+        <v>35.5</v>
       </c>
       <c r="AO2">
-        <v>54.5</v>
+        <v>46.5</v>
       </c>
       <c r="AP2">
-        <v>75.90000000000001</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="AQ2">
-        <v>78.59999999999999</v>
+        <v>76.8</v>
       </c>
       <c r="AR2">
-        <v>0.4736842105263158</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="AS2">
-        <v>0.5714285714285714</v>
+        <v>0.55</v>
       </c>
       <c r="AT2">
-        <v>0.4783174602543346</v>
+        <v>0.4893791837054243</v>
       </c>
       <c r="AU2">
-        <v>0.4722330995958968</v>
+        <v>0.4890893517231572</v>
       </c>
       <c r="AV2">
-        <v>-3.26</v>
+        <v>-3.23</v>
       </c>
       <c r="AW2">
-        <v>7.02</v>
+        <v>1.55</v>
       </c>
       <c r="AX2">
         <v>0</v>
@@ -909,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="BB2">
-        <v>0.5261400917355202</v>
+        <v>0.4928241638494351</v>
       </c>
     </row>
     <row r="3" spans="1:54">
@@ -920,157 +902,157 @@
         <v>2023</v>
       </c>
       <c r="D3">
-        <v>222.5</v>
+        <v>232.5</v>
       </c>
       <c r="E3">
-        <v>-2.5</v>
+        <v>-9.5</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H3">
-        <v>0.5517241379310345</v>
+        <v>0.578125</v>
       </c>
       <c r="I3">
-        <v>0.5517241379310345</v>
+        <v>0.5</v>
       </c>
       <c r="J3">
-        <v>111.7540983606557</v>
+        <v>115.0153846153846</v>
       </c>
       <c r="K3">
-        <v>117.0847457627119</v>
+        <v>114.5606060606061</v>
       </c>
       <c r="L3">
-        <v>94.58360655737704</v>
+        <v>96.50153846153847</v>
       </c>
       <c r="M3">
-        <v>98.04576271186437</v>
+        <v>97.25909090909089</v>
       </c>
       <c r="N3">
-        <v>116.7819672131148</v>
+        <v>118.3292307692308</v>
       </c>
       <c r="O3">
-        <v>119.0813559322034</v>
+        <v>117.4484848484848</v>
       </c>
       <c r="P3">
-        <v>110.9147540983606</v>
+        <v>114.1584615384616</v>
       </c>
       <c r="Q3">
-        <v>114.7254237288136</v>
+        <v>118.6378787878787</v>
       </c>
       <c r="R3">
-        <v>77.94754098360653</v>
+        <v>77.40153846153845</v>
       </c>
       <c r="S3">
-        <v>77.3118644067797</v>
+        <v>75.72424242424243</v>
       </c>
       <c r="T3">
-        <v>0.3738852459016392</v>
+        <v>0.3916615384615385</v>
       </c>
       <c r="U3">
-        <v>0.3575084745762713</v>
+        <v>0.4188484848484847</v>
       </c>
       <c r="V3">
-        <v>0.5937377049180327</v>
+        <v>0.6068000000000001</v>
       </c>
       <c r="W3">
-        <v>0.6111355932203389</v>
+        <v>0.5997727272727275</v>
       </c>
       <c r="X3">
-        <v>0.2739672131147541</v>
+        <v>0.3079692307692308</v>
       </c>
       <c r="Y3">
-        <v>0.2631186440677966</v>
+        <v>0.3028939393939394</v>
       </c>
       <c r="Z3">
-        <v>12.07540983606557</v>
+        <v>11.86769230769231</v>
       </c>
       <c r="AA3">
-        <v>12.8728813559322</v>
+        <v>12.63636363636364</v>
       </c>
       <c r="AB3">
-        <v>13.30819672131148</v>
+        <v>12.62</v>
       </c>
       <c r="AC3">
-        <v>11.94576271186441</v>
+        <v>11.5560606060606</v>
       </c>
       <c r="AD3">
-        <v>0.2097704918032787</v>
+        <v>0.2393153846153846</v>
       </c>
       <c r="AE3">
-        <v>0.203864406779661</v>
+        <v>0.2301969696969697</v>
       </c>
       <c r="AF3">
-        <v>0.9777261448876268</v>
+        <v>1.004501175680215</v>
       </c>
       <c r="AG3">
-        <v>1.02436347998873</v>
+        <v>1.000529310572979</v>
       </c>
       <c r="AH3">
-        <v>0.9723729890958879</v>
+        <v>1.150570715177457</v>
       </c>
       <c r="AI3">
-        <v>0.993582320015441</v>
+        <v>0.9456421108319005</v>
       </c>
       <c r="AJ3">
-        <v>11.11881544832595</v>
+        <v>12.39167500652982</v>
       </c>
       <c r="AK3">
-        <v>10.6933975124416</v>
+        <v>12.58923155509668</v>
       </c>
       <c r="AL3">
-        <v>0.6229508196721312</v>
+        <v>0.6615384615384615</v>
       </c>
       <c r="AM3">
-        <v>0.6949152542372882</v>
+        <v>0.4696969696969697</v>
       </c>
       <c r="AN3">
-        <v>46.5</v>
+        <v>50.5</v>
       </c>
       <c r="AO3">
-        <v>51.5</v>
+        <v>39.5</v>
       </c>
       <c r="AP3">
-        <v>77.2</v>
+        <v>76.2</v>
       </c>
       <c r="AQ3">
         <v>75.09999999999999</v>
       </c>
       <c r="AR3">
-        <v>0.3076923076923077</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="AS3">
-        <v>0.7368421052631579</v>
+        <v>0.5294117647058824</v>
       </c>
       <c r="AT3">
-        <v>0.4850395075395907</v>
+        <v>0.4822239615893419</v>
       </c>
       <c r="AU3">
-        <v>0.4905401505778892</v>
+        <v>0.4844204434951139</v>
       </c>
       <c r="AV3">
-        <v>2.04</v>
+        <v>2.57</v>
       </c>
       <c r="AW3">
-        <v>2.16</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="AX3">
         <v>0</v>
       </c>
       <c r="AY3">
+        <v>0.03982123427330137</v>
+      </c>
+      <c r="AZ3">
         <v>0</v>
       </c>
-      <c r="AZ3">
-        <v>0.01605874316939891</v>
-      </c>
       <c r="BA3">
-        <v>0.1459345574387947</v>
+        <v>0.06537773569023568</v>
       </c>
       <c r="BB3">
-        <v>0.5469661432241609</v>
+        <v>0.5107431656442085</v>
       </c>
     </row>
     <row r="4" spans="1:54">
@@ -1081,157 +1063,157 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>227</v>
+        <v>226.5</v>
       </c>
       <c r="E4">
-        <v>-7</v>
+        <v>-4.5</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H4">
-        <v>0.5689655172413793</v>
+        <v>0.4776119402985075</v>
       </c>
       <c r="I4">
-        <v>0.4464285714285715</v>
+        <v>0.5384615384615384</v>
       </c>
       <c r="J4">
-        <v>110.8983050847458</v>
+        <v>115.2985074626866</v>
       </c>
       <c r="K4">
-        <v>112.271186440678</v>
+        <v>113.5909090909091</v>
       </c>
       <c r="L4">
-        <v>98.11525423728817</v>
+        <v>100.6149253731343</v>
       </c>
       <c r="M4">
-        <v>99.21525423728815</v>
+        <v>97.95909090909095</v>
       </c>
       <c r="N4">
-        <v>112.4779661016949</v>
+        <v>114.189552238806</v>
       </c>
       <c r="O4">
-        <v>112.1745762711864</v>
+        <v>115.8575757575758</v>
       </c>
       <c r="P4">
-        <v>115.2813559322034</v>
+        <v>114.4283582089552</v>
       </c>
       <c r="Q4">
-        <v>119.757627118644</v>
+        <v>114.8954545454545</v>
       </c>
       <c r="R4">
-        <v>76.79322033898305</v>
+        <v>74.17462686567166</v>
       </c>
       <c r="S4">
-        <v>74.21016949152541</v>
+        <v>74.19242424242422</v>
       </c>
       <c r="T4">
-        <v>0.3609322033898305</v>
+        <v>0.3865522388059703</v>
       </c>
       <c r="U4">
-        <v>0.3809491525423727</v>
+        <v>0.3904848484848485</v>
       </c>
       <c r="V4">
-        <v>0.5776610169491525</v>
+        <v>0.5945223880597016</v>
       </c>
       <c r="W4">
-        <v>0.5650677966101695</v>
+        <v>0.6041060606060608</v>
       </c>
       <c r="X4">
-        <v>0.3009661016949152</v>
+        <v>0.2703283582089552</v>
       </c>
       <c r="Y4">
-        <v>0.3114237288135593</v>
+        <v>0.2540606060606061</v>
       </c>
       <c r="Z4">
-        <v>13.12203389830508</v>
+        <v>13.4</v>
       </c>
       <c r="AA4">
-        <v>12.61864406779661</v>
+        <v>12.23181818181818</v>
       </c>
       <c r="AB4">
-        <v>12.45254237288135</v>
+        <v>13.11641791044775</v>
       </c>
       <c r="AC4">
-        <v>11.91016949152543</v>
+        <v>11.65757575757576</v>
       </c>
       <c r="AD4">
-        <v>0.2236864406779661</v>
+        <v>0.2166716417910447</v>
       </c>
       <c r="AE4">
-        <v>0.2359152542372881</v>
+        <v>0.2108636363636363</v>
       </c>
       <c r="AF4">
-        <v>0.9702388896303216</v>
+        <v>1.00697386430294</v>
       </c>
       <c r="AG4">
-        <v>0.9822501000934205</v>
+        <v>0.9920603414053196</v>
       </c>
       <c r="AH4">
-        <v>0.9498191451423914</v>
+        <v>0.9887378640776698</v>
       </c>
       <c r="AI4">
-        <v>1.083685587761675</v>
+        <v>0.9771908763505401</v>
       </c>
       <c r="AJ4">
-        <v>10.23734425846104</v>
+        <v>10.91488771777957</v>
       </c>
       <c r="AK4">
-        <v>12.15134854547899</v>
+        <v>11.26670782589838</v>
       </c>
       <c r="AL4">
-        <v>0.4067796610169492</v>
+        <v>0.5074626865671642</v>
       </c>
       <c r="AM4">
-        <v>0.2542372881355932</v>
+        <v>0.5606060606060606</v>
       </c>
       <c r="AN4">
-        <v>26.5</v>
+        <v>49.5</v>
       </c>
       <c r="AO4">
-        <v>29.5</v>
+        <v>50.5</v>
       </c>
       <c r="AP4">
-        <v>74.59999999999999</v>
+        <v>75.7</v>
       </c>
       <c r="AQ4">
-        <v>74.2</v>
+        <v>76.5</v>
       </c>
       <c r="AR4">
-        <v>0.4</v>
+        <v>0.5294117647058824</v>
       </c>
       <c r="AS4">
-        <v>0.3</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="AT4">
-        <v>0.5150758958270623</v>
+        <v>0.5070320524274528</v>
       </c>
       <c r="AU4">
-        <v>0.5230943868025552</v>
+        <v>0.5079167324199545</v>
       </c>
       <c r="AV4">
-        <v>-7.67</v>
+        <v>2.53</v>
       </c>
       <c r="AW4">
-        <v>-7.35</v>
+        <v>0.82</v>
       </c>
       <c r="AX4">
-        <v>0</v>
+        <v>0.1505738476011289</v>
       </c>
       <c r="AY4">
-        <v>0</v>
+        <v>0.08827504853653123</v>
       </c>
       <c r="AZ4">
-        <v>0</v>
+        <v>0.1191625207296849</v>
       </c>
       <c r="BA4">
-        <v>0.01070503766478343</v>
+        <v>0.06975694444444445</v>
       </c>
       <c r="BB4">
-        <v>0.4946058788780239</v>
+        <v>0.5013452762916569</v>
       </c>
     </row>
     <row r="5" spans="1:54">
@@ -1242,157 +1224,157 @@
         <v>2023</v>
       </c>
       <c r="D5">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="E5">
-        <v>-3.5</v>
+        <v>12.5</v>
       </c>
       <c r="F5" t="s">
         <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H5">
-        <v>0.5892857142857143</v>
+        <v>0.4</v>
       </c>
       <c r="I5">
-        <v>0.4727272727272727</v>
+        <v>0.5538461538461539</v>
       </c>
       <c r="J5">
-        <v>114.3508771929825</v>
+        <v>112.0615384615385</v>
       </c>
       <c r="K5">
-        <v>116.1228070175439</v>
+        <v>116.8333333333333</v>
       </c>
       <c r="L5">
-        <v>96.61403508771932</v>
+        <v>100.5692307692308</v>
       </c>
       <c r="M5">
-        <v>100.8456140350877</v>
+        <v>97.80303030303025</v>
       </c>
       <c r="N5">
-        <v>117.4017543859649</v>
+        <v>110.96</v>
       </c>
       <c r="O5">
-        <v>114.8263157894737</v>
+        <v>118.9530303030303</v>
       </c>
       <c r="P5">
-        <v>113.4947368421053</v>
+        <v>121.0630769230769</v>
       </c>
       <c r="Q5">
-        <v>110.9526315789474</v>
+        <v>114.7833333333334</v>
       </c>
       <c r="R5">
-        <v>77.05087719298244</v>
+        <v>75.31846153846153</v>
       </c>
       <c r="S5">
-        <v>75.8315789473684</v>
+        <v>77.29545454545459</v>
       </c>
       <c r="T5">
-        <v>0.3918070175438597</v>
+        <v>0.3374</v>
       </c>
       <c r="U5">
-        <v>0.3555087719298246</v>
+        <v>0.3627424242424243</v>
       </c>
       <c r="V5">
-        <v>0.6026666666666667</v>
+        <v>0.5566307692307692</v>
       </c>
       <c r="W5">
-        <v>0.5628596491228071</v>
+        <v>0.6079696969696967</v>
       </c>
       <c r="X5">
-        <v>0.2970526315789473</v>
+        <v>0.234</v>
       </c>
       <c r="Y5">
-        <v>0.274017543859649</v>
+        <v>0.2612878787878788</v>
       </c>
       <c r="Z5">
-        <v>12.01929824561403</v>
+        <v>12.92615384615384</v>
       </c>
       <c r="AA5">
-        <v>11.6</v>
+        <v>12.7060606060606</v>
       </c>
       <c r="AB5">
-        <v>12.87017543859649</v>
+        <v>11.67692307692308</v>
       </c>
       <c r="AC5">
-        <v>12.76315789473684</v>
+        <v>11.77727272727273</v>
       </c>
       <c r="AD5">
-        <v>0.2331578947368421</v>
+        <v>0.1901538461538461</v>
       </c>
       <c r="AE5">
-        <v>0.2004649122807017</v>
+        <v>0.2019242424242425</v>
       </c>
       <c r="AF5">
-        <v>1.000445119798622</v>
+        <v>0.9787033926771918</v>
       </c>
       <c r="AG5">
-        <v>1.015947567957514</v>
+        <v>1.02037845705968</v>
       </c>
       <c r="AH5">
-        <v>0.9969315741024855</v>
+        <v>0.9816035145524438</v>
       </c>
       <c r="AI5">
-        <v>1.016165583925064</v>
+        <v>0.9329529243937232</v>
       </c>
       <c r="AJ5">
-        <v>11.93769090497879</v>
+        <v>10.43938831552725</v>
       </c>
       <c r="AK5">
-        <v>11.55470615056548</v>
+        <v>11.2014383996977</v>
       </c>
       <c r="AL5">
-        <v>0.6666666666666666</v>
+        <v>0.2461538461538462</v>
       </c>
       <c r="AM5">
-        <v>0.6140350877192983</v>
+        <v>0.696969696969697</v>
       </c>
       <c r="AN5">
-        <v>50.5</v>
+        <v>22.5</v>
       </c>
       <c r="AO5">
-        <v>49.5</v>
+        <v>51.5</v>
       </c>
       <c r="AP5">
-        <v>76.2</v>
+        <v>73.2</v>
       </c>
       <c r="AQ5">
-        <v>75.2</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="AR5">
-        <v>0.7142857142857143</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="AS5">
-        <v>0.4615384615384616</v>
+        <v>0.75</v>
       </c>
       <c r="AT5">
-        <v>0.4695080561336129</v>
+        <v>0.4887791237416139</v>
       </c>
       <c r="AU5">
-        <v>0.4703024102169868</v>
+        <v>0.4921000768022141</v>
       </c>
       <c r="AV5">
-        <v>2.57</v>
+        <v>0.02</v>
       </c>
       <c r="AW5">
-        <v>5.37</v>
+        <v>2.16</v>
       </c>
       <c r="AX5">
         <v>0</v>
       </c>
       <c r="AY5">
-        <v>0</v>
+        <v>0.02967047393987132</v>
       </c>
       <c r="AZ5">
         <v>0</v>
       </c>
       <c r="BA5">
-        <v>0.1417312378167641</v>
+        <v>0.03684343434343434</v>
       </c>
       <c r="BB5">
-        <v>0.558836618517463</v>
+        <v>0.5194559870106303</v>
       </c>
     </row>
     <row r="6" spans="1:54">
@@ -1403,157 +1385,157 @@
         <v>2023</v>
       </c>
       <c r="D6">
-        <v>226</v>
+        <v>212.5</v>
       </c>
       <c r="E6">
-        <v>-6</v>
+        <v>-2</v>
       </c>
       <c r="F6" t="s">
         <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H6">
-        <v>0.4915254237288136</v>
+        <v>0.359375</v>
       </c>
       <c r="I6">
-        <v>0.4827586206896552</v>
+        <v>0.5538461538461539</v>
       </c>
       <c r="J6">
-        <v>113.3220338983051</v>
+        <v>108.3283582089552</v>
       </c>
       <c r="K6">
-        <v>114.8983050847458</v>
+        <v>111.9411764705882</v>
       </c>
       <c r="L6">
-        <v>96.78305084745764</v>
+        <v>95.81343283582088</v>
       </c>
       <c r="M6">
-        <v>98.93389830508472</v>
+        <v>94.6941176470588</v>
       </c>
       <c r="N6">
-        <v>116.4254237288136</v>
+        <v>112.4701492537313</v>
       </c>
       <c r="O6">
-        <v>114.9881355932204</v>
+        <v>116.8117647058824</v>
       </c>
       <c r="P6">
-        <v>115.5474576271186</v>
+        <v>113.2731343283582</v>
       </c>
       <c r="Q6">
-        <v>113.5966101694916</v>
+        <v>111.1</v>
       </c>
       <c r="R6">
-        <v>76.81186440677965</v>
+        <v>78.22388059701495</v>
       </c>
       <c r="S6">
-        <v>77.26440677966103</v>
+        <v>77.50294117647056</v>
       </c>
       <c r="T6">
-        <v>0.3557796610169492</v>
+        <v>0.4042686567164178</v>
       </c>
       <c r="U6">
-        <v>0.3453220338983052</v>
+        <v>0.3727794117647058</v>
       </c>
       <c r="V6">
-        <v>0.5583220338983051</v>
+        <v>0.5663283582089553</v>
       </c>
       <c r="W6">
-        <v>0.580864406779661</v>
+        <v>0.5924852941176471</v>
       </c>
       <c r="X6">
-        <v>0.2780847457627119</v>
+        <v>0.2747910447761194</v>
       </c>
       <c r="Y6">
-        <v>0.2866440677966102</v>
+        <v>0.2699264705882354</v>
       </c>
       <c r="Z6">
-        <v>10.07627118644068</v>
+        <v>11.81194029850747</v>
       </c>
       <c r="AA6">
-        <v>12.64745762711864</v>
+        <v>11.92058823529412</v>
       </c>
       <c r="AB6">
-        <v>14.53050847457627</v>
+        <v>14.24477611940299</v>
       </c>
       <c r="AC6">
-        <v>12.93728813559322</v>
+        <v>13.43970588235294</v>
       </c>
       <c r="AD6">
-        <v>0.2238220338983051</v>
+        <v>0.2163955223880598</v>
       </c>
       <c r="AE6">
-        <v>0.2183389830508474</v>
+        <v>0.209375</v>
       </c>
       <c r="AF6">
-        <v>0.9914438661269036</v>
+        <v>0.9460991983314867</v>
       </c>
       <c r="AG6">
-        <v>1.005234515177128</v>
+        <v>0.9776521962496789</v>
       </c>
       <c r="AH6">
-        <v>1.053046166118257</v>
+        <v>1.067741342886011</v>
       </c>
       <c r="AI6">
-        <v>0.9051482519545656</v>
+        <v>1.000525486074619</v>
       </c>
       <c r="AJ6">
-        <v>10.2402341703331</v>
+        <v>9.410042364650762</v>
       </c>
       <c r="AK6">
-        <v>10.34603815969372</v>
+        <v>10.67140537762314</v>
       </c>
       <c r="AL6">
-        <v>0.4745762711864407</v>
+        <v>0.5223880597014925</v>
       </c>
       <c r="AM6">
-        <v>0.5084745762711864</v>
+        <v>0.6176470588235294</v>
       </c>
       <c r="AN6">
+        <v>49.5</v>
+      </c>
+      <c r="AO6">
         <v>46.5</v>
       </c>
-      <c r="AO6">
-        <v>45.5</v>
-      </c>
       <c r="AP6">
-        <v>74.90000000000001</v>
+        <v>76.2</v>
       </c>
       <c r="AQ6">
-        <v>77.40000000000001</v>
+        <v>77.2</v>
       </c>
       <c r="AR6">
-        <v>0.3157894736842105</v>
+        <v>0.5945945945945946</v>
       </c>
       <c r="AS6">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="AT6">
-        <v>0.4555862237270019</v>
+        <v>0.5093089740497807</v>
       </c>
       <c r="AU6">
-        <v>0.5203230998601887</v>
+        <v>0.491706430832801</v>
       </c>
       <c r="AV6">
-        <v>2.37</v>
+        <v>4.23</v>
       </c>
       <c r="AW6">
-        <v>-0.84</v>
+        <v>2.04</v>
       </c>
       <c r="AX6">
-        <v>0</v>
+        <v>0.1040707645094322</v>
       </c>
       <c r="AY6">
         <v>0</v>
       </c>
       <c r="AZ6">
+        <v>0.1266272802653399</v>
+      </c>
+      <c r="BA6">
         <v>0</v>
       </c>
-      <c r="BA6">
-        <v>0.06752354048964218</v>
-      </c>
       <c r="BB6">
-        <v>0.5232730061438239</v>
+        <v>0.5714803477360895</v>
       </c>
     </row>
     <row r="7" spans="1:54">
@@ -1564,640 +1546,157 @@
         <v>2023</v>
       </c>
       <c r="D7">
-        <v>237.5</v>
+        <v>224.5</v>
       </c>
       <c r="E7">
-        <v>-14.5</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
         <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H7">
-        <v>0.3684210526315789</v>
+        <v>0.4923076923076923</v>
       </c>
       <c r="I7">
-        <v>0.4067796610169492</v>
+        <v>0.4925373134328358</v>
       </c>
       <c r="J7">
-        <v>113</v>
+        <v>116.6363636363636</v>
       </c>
       <c r="K7">
-        <v>112.4406779661017</v>
+        <v>112.3880597014925</v>
       </c>
       <c r="L7">
-        <v>95.02500000000002</v>
+        <v>101.3469696969697</v>
       </c>
       <c r="M7">
-        <v>100.5762711864407</v>
+        <v>96.52388059701495</v>
       </c>
       <c r="N7">
-        <v>117.3116666666667</v>
+        <v>114.0469696969697</v>
       </c>
       <c r="O7">
-        <v>111.2661016949153</v>
+        <v>115.6746268656716</v>
       </c>
       <c r="P7">
-        <v>116.83</v>
+        <v>114.8</v>
       </c>
       <c r="Q7">
-        <v>121.2593220338983</v>
+        <v>115.3223880597015</v>
       </c>
       <c r="R7">
-        <v>76.42000000000002</v>
+        <v>76.43636363636362</v>
       </c>
       <c r="S7">
-        <v>75.11016949152541</v>
+        <v>76.75223880597012</v>
       </c>
       <c r="T7">
-        <v>0.4868166666666666</v>
+        <v>0.3468636363636364</v>
       </c>
       <c r="U7">
-        <v>0.3369491525423728</v>
+        <v>0.3534029850746268</v>
       </c>
       <c r="V7">
-        <v>0.5973000000000002</v>
+        <v>0.5776818181818182</v>
       </c>
       <c r="W7">
-        <v>0.5584745762711865</v>
+        <v>0.5547164179104477</v>
       </c>
       <c r="X7">
-        <v>0.3168999999999999</v>
+        <v>0.2951969696969697</v>
       </c>
       <c r="Y7">
-        <v>0.2349152542372881</v>
+        <v>0.270865671641791</v>
       </c>
       <c r="Z7">
-        <v>11.09166666666667</v>
+        <v>11.75151515151515</v>
       </c>
       <c r="AA7">
-        <v>13.03898305084745</v>
+        <v>10.18656716417911</v>
       </c>
       <c r="AB7">
-        <v>11.795</v>
+        <v>10.46212121212121</v>
       </c>
       <c r="AC7">
-        <v>11.66779661016949</v>
+        <v>14.57462686567164</v>
       </c>
       <c r="AD7">
-        <v>0.235175</v>
+        <v>0.2049545454545454</v>
       </c>
       <c r="AE7">
-        <v>0.1888135593220338</v>
+        <v>0.219955223880597</v>
       </c>
       <c r="AF7">
-        <v>0.9886264216972879</v>
+        <v>1.018658197697499</v>
       </c>
       <c r="AG7">
-        <v>0.983732965582692</v>
+        <v>0.9815551065632536</v>
       </c>
       <c r="AH7">
-        <v>1.056047197640118</v>
+        <v>0.9345284489477786</v>
       </c>
       <c r="AI7">
-        <v>0.9634710079389006</v>
+        <v>0.9757857459052679</v>
       </c>
       <c r="AJ7">
-        <v>11.5123122496453</v>
+        <v>10.58534774000644</v>
       </c>
       <c r="AK7">
-        <v>10.7707563690161</v>
+        <v>10.3519487297754</v>
       </c>
       <c r="AL7">
-        <v>0.5166666666666667</v>
+        <v>0.4848484848484849</v>
       </c>
       <c r="AM7">
-        <v>0.2372881355932203</v>
+        <v>0.4776119402985075</v>
       </c>
       <c r="AN7">
-        <v>48.5</v>
+        <v>44.5</v>
       </c>
       <c r="AO7">
-        <v>22.5</v>
+        <v>46.5</v>
       </c>
       <c r="AP7">
-        <v>75.3</v>
+        <v>75</v>
       </c>
       <c r="AQ7">
-        <v>73.2</v>
+        <v>74.90000000000001</v>
       </c>
       <c r="AR7">
-        <v>0.625</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="AS7">
-        <v>0.4545454545454545</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="AT7">
-        <v>0.4983191914194789</v>
+        <v>0.5112498936184414</v>
       </c>
       <c r="AU7">
-        <v>0.4980648985055629</v>
+        <v>0.4607480785545702</v>
       </c>
       <c r="AV7">
-        <v>3.12</v>
+        <v>-3.08</v>
       </c>
       <c r="AW7">
-        <v>0.02</v>
+        <v>2.37</v>
       </c>
       <c r="AX7">
-        <v>0</v>
+        <v>0.2661314137544454</v>
       </c>
       <c r="AY7">
         <v>0</v>
       </c>
       <c r="AZ7">
-        <v>0.06420833333333334</v>
+        <v>0.1375957491582491</v>
       </c>
       <c r="BA7">
-        <v>0.1430767419962335</v>
+        <v>0</v>
       </c>
       <c r="BB7">
-        <v>0.4274377413206152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:54">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>2023</v>
-      </c>
-      <c r="D8">
-        <v>240.5</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8">
-        <v>0.559322033898305</v>
-      </c>
-      <c r="I8">
-        <v>0.625</v>
-      </c>
-      <c r="J8">
-        <v>117.5666666666667</v>
-      </c>
-      <c r="K8">
-        <v>117.8947368421053</v>
-      </c>
-      <c r="L8">
-        <v>99.36333333333333</v>
-      </c>
-      <c r="M8">
-        <v>100.5754385964912</v>
-      </c>
-      <c r="N8">
-        <v>117.7283333333333</v>
-      </c>
-      <c r="O8">
-        <v>116</v>
-      </c>
-      <c r="P8">
-        <v>117.5533333333333</v>
-      </c>
-      <c r="Q8">
-        <v>114.4017543859649</v>
-      </c>
-      <c r="R8">
-        <v>74.61499999999997</v>
-      </c>
-      <c r="S8">
-        <v>72.91754385964914</v>
-      </c>
-      <c r="T8">
-        <v>0.4369666666666667</v>
-      </c>
-      <c r="U8">
-        <v>0.3608070175438597</v>
-      </c>
-      <c r="V8">
-        <v>0.5909666666666664</v>
-      </c>
-      <c r="W8">
-        <v>0.5752982456140349</v>
-      </c>
-      <c r="X8">
-        <v>0.2710166666666666</v>
-      </c>
-      <c r="Y8">
-        <v>0.2529649122807018</v>
-      </c>
-      <c r="Z8">
-        <v>12.86833333333334</v>
-      </c>
-      <c r="AA8">
-        <v>11.20701754385965</v>
-      </c>
-      <c r="AB8">
-        <v>11.14666666666667</v>
-      </c>
-      <c r="AC8">
-        <v>13.91929824561404</v>
-      </c>
-      <c r="AD8">
-        <v>0.2116583333333334</v>
-      </c>
-      <c r="AE8">
-        <v>0.2164649122807017</v>
-      </c>
-      <c r="AF8">
-        <v>1.028579760863225</v>
-      </c>
-      <c r="AG8">
-        <v>1.031450016116406</v>
-      </c>
-      <c r="AH8">
-        <v>1.003685851998866</v>
-      </c>
-      <c r="AI8">
-        <v>1.048958333333333</v>
-      </c>
-      <c r="AJ8">
-        <v>9.788371786064435</v>
-      </c>
-      <c r="AK8">
-        <v>12.99484946623262</v>
-      </c>
-      <c r="AL8">
-        <v>0.4833333333333333</v>
-      </c>
-      <c r="AM8">
-        <v>0.4912280701754386</v>
-      </c>
-      <c r="AN8">
-        <v>23.5</v>
-      </c>
-      <c r="AO8">
-        <v>23.5</v>
-      </c>
-      <c r="AP8">
-        <v>74.3</v>
-      </c>
-      <c r="AQ8">
-        <v>74.40000000000001</v>
-      </c>
-      <c r="AR8">
-        <v>0.4761904761904762</v>
-      </c>
-      <c r="AS8">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="AT8">
-        <v>0.5094891615581804</v>
-      </c>
-      <c r="AU8">
-        <v>0.505926743154552</v>
-      </c>
-      <c r="AV8">
-        <v>5.67</v>
-      </c>
-      <c r="AW8">
-        <v>-7.9</v>
-      </c>
-      <c r="AX8">
-        <v>0</v>
-      </c>
-      <c r="AY8">
-        <v>0</v>
-      </c>
-      <c r="AZ8">
-        <v>0.07842939814814817</v>
-      </c>
-      <c r="BA8">
-        <v>0.04952119883040936</v>
-      </c>
-      <c r="BB8">
-        <v>0.4755294624178618</v>
-      </c>
-    </row>
-    <row r="9" spans="1:54">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>2023</v>
-      </c>
-      <c r="D9">
-        <v>238.5</v>
-      </c>
-      <c r="E9">
-        <v>-6</v>
-      </c>
-      <c r="F9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9">
-        <v>0.4655172413793103</v>
-      </c>
-      <c r="I9">
-        <v>0.456140350877193</v>
-      </c>
-      <c r="J9">
-        <v>117.0169491525424</v>
-      </c>
-      <c r="K9">
-        <v>118.6206896551724</v>
-      </c>
-      <c r="L9">
-        <v>101.3084745762712</v>
-      </c>
-      <c r="M9">
-        <v>101.4827586206897</v>
-      </c>
-      <c r="N9">
-        <v>114.3254237288136</v>
-      </c>
-      <c r="O9">
-        <v>116.0172413793103</v>
-      </c>
-      <c r="P9">
-        <v>115.4864406779661</v>
-      </c>
-      <c r="Q9">
-        <v>115.9689655172414</v>
-      </c>
-      <c r="R9">
-        <v>76.23559322033896</v>
-      </c>
-      <c r="S9">
-        <v>76.16551724137929</v>
-      </c>
-      <c r="T9">
-        <v>0.3448474576271187</v>
-      </c>
-      <c r="U9">
-        <v>0.4778793103448276</v>
-      </c>
-      <c r="V9">
-        <v>0.5796101694915253</v>
-      </c>
-      <c r="W9">
-        <v>0.6011551724137929</v>
-      </c>
-      <c r="X9">
-        <v>0.2917627118644069</v>
-      </c>
-      <c r="Y9">
-        <v>0.2244827586206897</v>
-      </c>
-      <c r="Z9">
-        <v>11.7135593220339</v>
-      </c>
-      <c r="AA9">
-        <v>13.76724137931034</v>
-      </c>
-      <c r="AB9">
-        <v>10.59491525423729</v>
-      </c>
-      <c r="AC9">
-        <v>12.12413793103449</v>
-      </c>
-      <c r="AD9">
-        <v>0.2045932203389831</v>
-      </c>
-      <c r="AE9">
-        <v>0.2018534482758621</v>
-      </c>
-      <c r="AF9">
-        <v>1.023770333793022</v>
-      </c>
-      <c r="AG9">
-        <v>1.037801309319094</v>
-      </c>
-      <c r="AH9">
-        <v>0.9799150251062188</v>
-      </c>
-      <c r="AI9">
-        <v>1.017248062015504</v>
-      </c>
-      <c r="AJ9">
-        <v>10.85574365731555</v>
-      </c>
-      <c r="AK9">
-        <v>11.23391967429506</v>
-      </c>
-      <c r="AL9">
-        <v>0.4576271186440678</v>
-      </c>
-      <c r="AM9">
-        <v>0.5</v>
-      </c>
-      <c r="AN9">
-        <v>44.5</v>
-      </c>
-      <c r="AO9">
-        <v>52.5</v>
-      </c>
-      <c r="AP9">
-        <v>75</v>
-      </c>
-      <c r="AQ9">
-        <v>76.3</v>
-      </c>
-      <c r="AR9">
-        <v>0.4444444444444444</v>
-      </c>
-      <c r="AS9">
-        <v>0.4375</v>
-      </c>
-      <c r="AT9">
-        <v>0.5087168190972892</v>
-      </c>
-      <c r="AU9">
-        <v>0.4676985007366004</v>
-      </c>
-      <c r="AV9">
-        <v>-3.08</v>
-      </c>
-      <c r="AW9">
-        <v>5.52</v>
-      </c>
-      <c r="AX9">
-        <v>0</v>
-      </c>
-      <c r="AY9">
-        <v>0</v>
-      </c>
-      <c r="AZ9">
-        <v>0</v>
-      </c>
-      <c r="BA9">
-        <v>0.1828556034482759</v>
-      </c>
-      <c r="BB9">
-        <v>0.457110219249547</v>
-      </c>
-    </row>
-    <row r="10" spans="1:54">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>2023</v>
-      </c>
-      <c r="D10">
-        <v>240.5</v>
-      </c>
-      <c r="E10">
-        <v>-6</v>
-      </c>
-      <c r="F10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" t="s">
-        <v>70</v>
-      </c>
-      <c r="H10">
-        <v>0.5357142857142857</v>
-      </c>
-      <c r="I10">
-        <v>0.5172413793103449</v>
-      </c>
-      <c r="J10">
-        <v>119.4561403508772</v>
-      </c>
-      <c r="K10">
-        <v>114.8793103448276</v>
-      </c>
-      <c r="L10">
-        <v>100.0842105263158</v>
-      </c>
-      <c r="M10">
-        <v>97.04827586206892</v>
-      </c>
-      <c r="N10">
-        <v>118.7192982456141</v>
-      </c>
-      <c r="O10">
-        <v>117.9603448275862</v>
-      </c>
-      <c r="P10">
-        <v>116.6491228070176</v>
-      </c>
-      <c r="Q10">
-        <v>118.2810344827586</v>
-      </c>
-      <c r="R10">
-        <v>77.19298245614037</v>
-      </c>
-      <c r="S10">
-        <v>76.11724137931034</v>
-      </c>
-      <c r="T10">
-        <v>0.4160350877192981</v>
-      </c>
-      <c r="U10">
-        <v>0.4119655172413793</v>
-      </c>
-      <c r="V10">
-        <v>0.6081929824561403</v>
-      </c>
-      <c r="W10">
-        <v>0.600741379310345</v>
-      </c>
-      <c r="X10">
-        <v>0.2870701754385966</v>
-      </c>
-      <c r="Y10">
-        <v>0.3012586206896552</v>
-      </c>
-      <c r="Z10">
-        <v>12.18245614035087</v>
-      </c>
-      <c r="AA10">
-        <v>12.60689655172414</v>
-      </c>
-      <c r="AB10">
-        <v>12.3</v>
-      </c>
-      <c r="AC10">
-        <v>11.49827586206897</v>
-      </c>
-      <c r="AD10">
-        <v>0.2159385964912281</v>
-      </c>
-      <c r="AE10">
-        <v>0.2303879310344828</v>
-      </c>
-      <c r="AF10">
-        <v>1.04511058924652</v>
-      </c>
-      <c r="AG10">
-        <v>1.005068331975745</v>
-      </c>
-      <c r="AH10">
-        <v>0.9933911000146864</v>
-      </c>
-      <c r="AI10">
-        <v>1.035869728350593</v>
-      </c>
-      <c r="AJ10">
-        <v>12.06425803542074</v>
-      </c>
-      <c r="AK10">
-        <v>12.8090452768224</v>
-      </c>
-      <c r="AL10">
-        <v>0.5614035087719298</v>
-      </c>
-      <c r="AM10">
-        <v>0.4827586206896552</v>
-      </c>
-      <c r="AN10">
-        <v>34.5</v>
-      </c>
-      <c r="AO10">
-        <v>39.5</v>
-      </c>
-      <c r="AP10">
-        <v>75.90000000000001</v>
-      </c>
-      <c r="AQ10">
-        <v>75.09999999999999</v>
-      </c>
-      <c r="AR10">
-        <v>0.5263157894736842</v>
-      </c>
-      <c r="AS10">
-        <v>0.5</v>
-      </c>
-      <c r="AT10">
-        <v>0.4718078380778777</v>
-      </c>
-      <c r="AU10">
-        <v>0.4889632915169508</v>
-      </c>
-      <c r="AV10">
-        <v>-5.26</v>
-      </c>
-      <c r="AW10">
-        <v>-8.550000000000001</v>
-      </c>
-      <c r="AX10">
-        <v>0</v>
-      </c>
-      <c r="AY10">
-        <v>0</v>
-      </c>
-      <c r="AZ10">
-        <v>0.01811525341130604</v>
-      </c>
-      <c r="BA10">
-        <v>0.2868235153256705</v>
-      </c>
-      <c r="BB10">
-        <v>0.5219576120000876</v>
+        <v>0.4706578153960231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MAJOR RELEASE: MACHINE LEARNING MODEL V1.0
</commit_message>
<xml_diff>
--- a/current_games_spread.xlsx
+++ b/current_games_spread.xlsx
@@ -175,40 +175,40 @@
     <t>calc_home_prob</t>
   </si>
   <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>NewOrleans</t>
+  </si>
+  <si>
+    <t>SanAntonio</t>
+  </si>
+  <si>
+    <t>LALakers</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
     <t>Washington</t>
   </si>
   <si>
-    <t>Philadelphia</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>SanAntonio</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>LALakers</t>
-  </si>
-  <si>
-    <t>Atlanta</t>
-  </si>
-  <si>
     <t>Portland</t>
   </si>
   <si>
-    <t>Brooklyn</t>
-  </si>
-  <si>
-    <t>Denver</t>
-  </si>
-  <si>
-    <t>Cleveland</t>
-  </si>
-  <si>
-    <t>Toronto</t>
+    <t>OklahomaCity</t>
+  </si>
+  <si>
+    <t>NewYork</t>
   </si>
 </sst>
 </file>
@@ -741,10 +741,10 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>238</v>
+        <v>230.5</v>
       </c>
       <c r="E2">
-        <v>1.5</v>
+        <v>-9</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
@@ -753,145 +753,145 @@
         <v>59</v>
       </c>
       <c r="H2">
-        <v>0.492063492063492</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="I2">
-        <v>0.4461538461538462</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="J2">
-        <v>113.3181818181818</v>
+        <v>116.8805970149254</v>
       </c>
       <c r="K2">
-        <v>117.2121212121212</v>
+        <v>113.7462686567164</v>
       </c>
       <c r="L2">
-        <v>97.73484848484851</v>
+        <v>97.88358208955219</v>
       </c>
       <c r="M2">
-        <v>99.81363636363636</v>
+        <v>97.95074626865674</v>
       </c>
       <c r="N2">
-        <v>115.5484848484848</v>
+        <v>118.9134328358209</v>
       </c>
       <c r="O2">
-        <v>116.5969696969697</v>
+        <v>115.8492537313433</v>
       </c>
       <c r="P2">
-        <v>115.7136363636364</v>
+        <v>114.9223880597015</v>
       </c>
       <c r="Q2">
-        <v>116.5227272727273</v>
+        <v>114.8880597014925</v>
       </c>
       <c r="R2">
-        <v>76.3878787878788</v>
+        <v>77.12388059701497</v>
       </c>
       <c r="S2">
-        <v>75.90303030303029</v>
+        <v>74.20447761194028</v>
       </c>
       <c r="T2">
-        <v>0.3638181818181819</v>
+        <v>0.363134328358209</v>
       </c>
       <c r="U2">
-        <v>0.3316969696969697</v>
+        <v>0.3902388059701493</v>
       </c>
       <c r="V2">
-        <v>0.5898484848484846</v>
+        <v>0.6079552238805968</v>
       </c>
       <c r="W2">
-        <v>0.5795454545454549</v>
+        <v>0.6038656716417912</v>
       </c>
       <c r="X2">
-        <v>0.2657878787878787</v>
+        <v>0.2607014925373135</v>
       </c>
       <c r="Y2">
-        <v>0.2420606060606061</v>
+        <v>0.2556865671641791</v>
       </c>
       <c r="Z2">
-        <v>12.4030303030303</v>
+        <v>12.70149253731343</v>
       </c>
       <c r="AA2">
-        <v>10.83181818181818</v>
+        <v>12.22388059701493</v>
       </c>
       <c r="AB2">
-        <v>10.62121212121212</v>
+        <v>11.82686567164179</v>
       </c>
       <c r="AC2">
-        <v>12.06666666666666</v>
+        <v>11.65074626865672</v>
       </c>
       <c r="AD2">
-        <v>0.2044924242424242</v>
+        <v>0.2015149253731344</v>
       </c>
       <c r="AE2">
-        <v>0.2080909090909091</v>
+        <v>0.2110597014925373</v>
       </c>
       <c r="AF2">
-        <v>0.9896784438269154</v>
+        <v>1.020791240305025</v>
       </c>
       <c r="AG2">
-        <v>1.023686648140797</v>
+        <v>0.9934171935084404</v>
       </c>
       <c r="AH2">
-        <v>1.029549405000669</v>
+        <v>0.9525390541863533</v>
       </c>
       <c r="AI2">
-        <v>1.020941054808687</v>
+        <v>1.04032716616367</v>
       </c>
       <c r="AJ2">
-        <v>10.94913735485252</v>
+        <v>11.12416005624721</v>
       </c>
       <c r="AK2">
-        <v>11.00484074136847</v>
+        <v>11.25331564218959</v>
       </c>
       <c r="AL2">
-        <v>0.4696969696969697</v>
+        <v>0.6865671641791045</v>
       </c>
       <c r="AM2">
-        <v>0.5</v>
+        <v>0.5671641791044776</v>
       </c>
       <c r="AN2">
-        <v>35.5</v>
+        <v>51.5</v>
       </c>
       <c r="AO2">
-        <v>46.5</v>
+        <v>50.5</v>
       </c>
       <c r="AP2">
-        <v>76.09999999999999</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="AQ2">
-        <v>76.8</v>
+        <v>76.5</v>
       </c>
       <c r="AR2">
-        <v>0.5555555555555556</v>
+        <v>0.75</v>
       </c>
       <c r="AS2">
-        <v>0.55</v>
+        <v>0.6</v>
       </c>
       <c r="AT2">
-        <v>0.4893791837054243</v>
+        <v>0.4884292375388056</v>
       </c>
       <c r="AU2">
-        <v>0.4890893517231572</v>
+        <v>0.5079099556161815</v>
       </c>
       <c r="AV2">
-        <v>-3.23</v>
+        <v>2.16</v>
       </c>
       <c r="AW2">
-        <v>1.55</v>
+        <v>0.82</v>
       </c>
       <c r="AX2">
-        <v>0</v>
+        <v>0.02916223103971095</v>
       </c>
       <c r="AY2">
         <v>0</v>
       </c>
       <c r="AZ2">
-        <v>0</v>
+        <v>0.03629353233830845</v>
       </c>
       <c r="BA2">
         <v>0</v>
       </c>
       <c r="BB2">
-        <v>0.4928241638494351</v>
+        <v>0.5279092519844266</v>
       </c>
     </row>
     <row r="3" spans="1:54">
@@ -902,10 +902,10 @@
         <v>2023</v>
       </c>
       <c r="D3">
-        <v>232.5</v>
+        <v>220</v>
       </c>
       <c r="E3">
-        <v>-9.5</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
@@ -914,145 +914,145 @@
         <v>60</v>
       </c>
       <c r="H3">
-        <v>0.578125</v>
+        <v>0.4477611940298508</v>
       </c>
       <c r="I3">
-        <v>0.5</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="J3">
-        <v>115.0153846153846</v>
+        <v>111.8235294117647</v>
       </c>
       <c r="K3">
-        <v>114.5606060606061</v>
+        <v>111.9855072463768</v>
       </c>
       <c r="L3">
-        <v>96.50153846153847</v>
+        <v>100.4867647058824</v>
       </c>
       <c r="M3">
-        <v>97.25909090909089</v>
+        <v>94.70434782608693</v>
       </c>
       <c r="N3">
-        <v>118.3292307692308</v>
+        <v>110.375</v>
       </c>
       <c r="O3">
-        <v>117.4484848484848</v>
+        <v>116.8666666666667</v>
       </c>
       <c r="P3">
-        <v>114.1584615384616</v>
+        <v>116.0191176470588</v>
       </c>
       <c r="Q3">
-        <v>118.6378787878787</v>
+        <v>111.2985507246377</v>
       </c>
       <c r="R3">
-        <v>77.40153846153845</v>
+        <v>75.62352941176475</v>
       </c>
       <c r="S3">
-        <v>75.72424242424243</v>
+        <v>77.39855072463766</v>
       </c>
       <c r="T3">
-        <v>0.3916615384615385</v>
+        <v>0.3563382352941177</v>
       </c>
       <c r="U3">
-        <v>0.4188484848484847</v>
+        <v>0.374623188405797</v>
       </c>
       <c r="V3">
-        <v>0.6068000000000001</v>
+        <v>0.5497647058823528</v>
       </c>
       <c r="W3">
-        <v>0.5997727272727275</v>
+        <v>0.5926521739130435</v>
       </c>
       <c r="X3">
-        <v>0.3079692307692308</v>
+        <v>0.2632647058823531</v>
       </c>
       <c r="Y3">
-        <v>0.3028939393939394</v>
+        <v>0.2695507246376813</v>
       </c>
       <c r="Z3">
-        <v>11.86769230769231</v>
+        <v>11.5764705882353</v>
       </c>
       <c r="AA3">
-        <v>12.63636363636364</v>
+        <v>11.89855072463768</v>
       </c>
       <c r="AB3">
-        <v>12.62</v>
+        <v>12.41176470588235</v>
       </c>
       <c r="AC3">
-        <v>11.5560606060606</v>
+        <v>13.45942028985507</v>
       </c>
       <c r="AD3">
-        <v>0.2393153846153846</v>
+        <v>0.2055294117647059</v>
       </c>
       <c r="AE3">
-        <v>0.2301969696969697</v>
+        <v>0.2096304347826087</v>
       </c>
       <c r="AF3">
-        <v>1.004501175680215</v>
+        <v>0.9766247110197791</v>
       </c>
       <c r="AG3">
-        <v>1.000529310572979</v>
+        <v>0.9780393645971774</v>
       </c>
       <c r="AH3">
-        <v>1.150570715177457</v>
+        <v>0.9270559354725583</v>
       </c>
       <c r="AI3">
-        <v>0.9456421108319005</v>
+        <v>1.003105991976187</v>
       </c>
       <c r="AJ3">
-        <v>12.39167500652982</v>
+        <v>11.55032616864459</v>
       </c>
       <c r="AK3">
-        <v>12.58923155509668</v>
+        <v>10.60009947126309</v>
       </c>
       <c r="AL3">
-        <v>0.6615384615384615</v>
+        <v>0.3235294117647059</v>
       </c>
       <c r="AM3">
-        <v>0.4696969696969697</v>
+        <v>0.6086956521739131</v>
       </c>
       <c r="AN3">
-        <v>50.5</v>
+        <v>34.5</v>
       </c>
       <c r="AO3">
-        <v>39.5</v>
+        <v>46.5</v>
       </c>
       <c r="AP3">
-        <v>76.2</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="AQ3">
-        <v>75.09999999999999</v>
+        <v>77.2</v>
       </c>
       <c r="AR3">
-        <v>0.6842105263157895</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AS3">
-        <v>0.5294117647058824</v>
+        <v>0.3529411764705883</v>
       </c>
       <c r="AT3">
-        <v>0.4822239615893419</v>
+        <v>0.5026769579206853</v>
       </c>
       <c r="AU3">
-        <v>0.4844204434951139</v>
+        <v>0.492151092120753</v>
       </c>
       <c r="AV3">
-        <v>2.57</v>
+        <v>0.53</v>
       </c>
       <c r="AW3">
-        <v>-8.550000000000001</v>
+        <v>2.04</v>
       </c>
       <c r="AX3">
         <v>0</v>
       </c>
       <c r="AY3">
-        <v>0.03982123427330137</v>
+        <v>0</v>
       </c>
       <c r="AZ3">
         <v>0</v>
       </c>
       <c r="BA3">
-        <v>0.06537773569023568</v>
+        <v>0</v>
       </c>
       <c r="BB3">
-        <v>0.5107431656442085</v>
+        <v>0.5706285307576093</v>
       </c>
     </row>
     <row r="4" spans="1:54">
@@ -1063,10 +1063,10 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>226.5</v>
+        <v>227.5</v>
       </c>
       <c r="E4">
-        <v>-4.5</v>
+        <v>-7.5</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
@@ -1075,145 +1075,145 @@
         <v>61</v>
       </c>
       <c r="H4">
-        <v>0.4776119402985075</v>
+        <v>0.5692307692307692</v>
       </c>
       <c r="I4">
-        <v>0.5384615384615384</v>
+        <v>0.484375</v>
       </c>
       <c r="J4">
-        <v>115.2985074626866</v>
+        <v>115.0909090909091</v>
       </c>
       <c r="K4">
-        <v>113.5909090909091</v>
+        <v>113.2238805970149</v>
       </c>
       <c r="L4">
-        <v>100.6149253731343</v>
+        <v>96.45454545454545</v>
       </c>
       <c r="M4">
-        <v>97.95909090909095</v>
+        <v>97.78656716417913</v>
       </c>
       <c r="N4">
-        <v>114.189552238806</v>
+        <v>118.4818181818182</v>
       </c>
       <c r="O4">
-        <v>115.8575757575758</v>
+        <v>115.4029850746269</v>
       </c>
       <c r="P4">
-        <v>114.4283582089552</v>
+        <v>114.359090909091</v>
       </c>
       <c r="Q4">
-        <v>114.8954545454545</v>
+        <v>115.6686567164179</v>
       </c>
       <c r="R4">
-        <v>74.17462686567166</v>
+        <v>77.52727272727272</v>
       </c>
       <c r="S4">
-        <v>74.19242424242422</v>
+        <v>76.34477611940301</v>
       </c>
       <c r="T4">
-        <v>0.3865522388059703</v>
+        <v>0.3911969696969697</v>
       </c>
       <c r="U4">
-        <v>0.3904848484848485</v>
+        <v>0.3629701492537314</v>
       </c>
       <c r="V4">
-        <v>0.5945223880597016</v>
+        <v>0.6071060606060608</v>
       </c>
       <c r="W4">
-        <v>0.6041060606060608</v>
+        <v>0.589373134328358</v>
       </c>
       <c r="X4">
-        <v>0.2703283582089552</v>
+        <v>0.3085909090909091</v>
       </c>
       <c r="Y4">
-        <v>0.2540606060606061</v>
+        <v>0.2648805970149253</v>
       </c>
       <c r="Z4">
-        <v>13.4</v>
+        <v>11.81818181818182</v>
       </c>
       <c r="AA4">
-        <v>12.23181818181818</v>
+        <v>12.40746268656716</v>
       </c>
       <c r="AB4">
-        <v>13.11641791044775</v>
+        <v>12.56212121212121</v>
       </c>
       <c r="AC4">
-        <v>11.65757575757576</v>
+        <v>10.64029850746269</v>
       </c>
       <c r="AD4">
-        <v>0.2166716417910447</v>
+        <v>0.2396818181818181</v>
       </c>
       <c r="AE4">
-        <v>0.2108636363636363</v>
+        <v>0.2038059701492537</v>
       </c>
       <c r="AF4">
-        <v>1.00697386430294</v>
+        <v>1.005160778086542</v>
       </c>
       <c r="AG4">
-        <v>0.9920603414053196</v>
+        <v>0.9888548523756762</v>
       </c>
       <c r="AH4">
-        <v>0.9887378640776698</v>
+        <v>1.11216429699842</v>
       </c>
       <c r="AI4">
-        <v>0.9771908763505401</v>
+        <v>1.018630811143334</v>
       </c>
       <c r="AJ4">
-        <v>10.91488771777957</v>
+        <v>12.31250568094288</v>
       </c>
       <c r="AK4">
-        <v>11.26670782589838</v>
+        <v>10.8940910938849</v>
       </c>
       <c r="AL4">
-        <v>0.5074626865671642</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AM4">
-        <v>0.5606060606060606</v>
+        <v>0.4626865671641791</v>
       </c>
       <c r="AN4">
-        <v>49.5</v>
+        <v>50.5</v>
       </c>
       <c r="AO4">
-        <v>50.5</v>
+        <v>35.5</v>
       </c>
       <c r="AP4">
-        <v>75.7</v>
+        <v>76.2</v>
       </c>
       <c r="AQ4">
-        <v>76.5</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="AR4">
-        <v>0.5294117647058824</v>
+        <v>0.7</v>
       </c>
       <c r="AS4">
-        <v>0.5789473684210527</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="AT4">
-        <v>0.5070320524274528</v>
+        <v>0.4820341586818817</v>
       </c>
       <c r="AU4">
-        <v>0.5079167324199545</v>
+        <v>0.489537703351612</v>
       </c>
       <c r="AV4">
-        <v>2.53</v>
+        <v>2.57</v>
       </c>
       <c r="AW4">
-        <v>0.82</v>
+        <v>-3.23</v>
       </c>
       <c r="AX4">
-        <v>0.1505738476011289</v>
+        <v>0</v>
       </c>
       <c r="AY4">
-        <v>0.08827504853653123</v>
+        <v>0</v>
       </c>
       <c r="AZ4">
-        <v>0.1191625207296849</v>
+        <v>0</v>
       </c>
       <c r="BA4">
-        <v>0.06975694444444445</v>
+        <v>0</v>
       </c>
       <c r="BB4">
-        <v>0.5013452762916569</v>
+        <v>0.5007639899963852</v>
       </c>
     </row>
     <row r="5" spans="1:54">
@@ -1224,10 +1224,10 @@
         <v>2023</v>
       </c>
       <c r="D5">
-        <v>236</v>
+        <v>230.5</v>
       </c>
       <c r="E5">
-        <v>12.5</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>56</v>
@@ -1236,145 +1236,145 @@
         <v>62</v>
       </c>
       <c r="H5">
-        <v>0.4</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="I5">
-        <v>0.5538461538461539</v>
+        <v>0.5074626865671642</v>
       </c>
       <c r="J5">
-        <v>112.0615384615385</v>
+        <v>114.0757575757576</v>
       </c>
       <c r="K5">
-        <v>116.8333333333333</v>
+        <v>114.6268656716418</v>
       </c>
       <c r="L5">
-        <v>100.5692307692308</v>
+        <v>98.60303030303029</v>
       </c>
       <c r="M5">
-        <v>97.80303030303025</v>
+        <v>97.2014925373134</v>
       </c>
       <c r="N5">
-        <v>110.96</v>
+        <v>114.6636363636364</v>
       </c>
       <c r="O5">
-        <v>118.9530303030303</v>
+        <v>117.5970149253731</v>
       </c>
       <c r="P5">
-        <v>121.0630769230769</v>
+        <v>114.0530303030303</v>
       </c>
       <c r="Q5">
-        <v>114.7833333333334</v>
+        <v>118.7835820895522</v>
       </c>
       <c r="R5">
-        <v>75.31846153846153</v>
+        <v>77.1878787878788</v>
       </c>
       <c r="S5">
-        <v>77.29545454545459</v>
+        <v>75.67014925373135</v>
       </c>
       <c r="T5">
-        <v>0.3374</v>
+        <v>0.3455303030303031</v>
       </c>
       <c r="U5">
-        <v>0.3627424242424243</v>
+        <v>0.4193134328358208</v>
       </c>
       <c r="V5">
-        <v>0.5566307692307692</v>
+        <v>0.5800151515151516</v>
       </c>
       <c r="W5">
-        <v>0.6079696969696967</v>
+        <v>0.6003432835820898</v>
       </c>
       <c r="X5">
-        <v>0.234</v>
+        <v>0.2836363636363636</v>
       </c>
       <c r="Y5">
-        <v>0.2612878787878788</v>
+        <v>0.3039701492537314</v>
       </c>
       <c r="Z5">
-        <v>12.92615384615384</v>
+        <v>12.56060606060606</v>
       </c>
       <c r="AA5">
-        <v>12.7060606060606</v>
+        <v>12.57910447761194</v>
       </c>
       <c r="AB5">
-        <v>11.67692307692308</v>
+        <v>12.90606060606061</v>
       </c>
       <c r="AC5">
-        <v>11.77727272727273</v>
+        <v>11.51194029850746</v>
       </c>
       <c r="AD5">
-        <v>0.1901538461538461</v>
+        <v>0.2182651515151515</v>
       </c>
       <c r="AE5">
-        <v>0.2019242424242425</v>
+        <v>0.2306940298507463</v>
       </c>
       <c r="AF5">
-        <v>0.9787033926771918</v>
+        <v>0.9962948259891492</v>
       </c>
       <c r="AG5">
-        <v>1.02037845705968</v>
+        <v>1.001107997132243</v>
       </c>
       <c r="AH5">
-        <v>0.9816035145524438</v>
+        <v>0.9350511356089787</v>
       </c>
       <c r="AI5">
-        <v>0.9329529243937232</v>
+        <v>0.9363715277777777</v>
       </c>
       <c r="AJ5">
-        <v>10.43938831552725</v>
+        <v>10.44075726683016</v>
       </c>
       <c r="AK5">
-        <v>11.2014383996977</v>
+        <v>12.50651868342949</v>
       </c>
       <c r="AL5">
-        <v>0.2461538461538462</v>
+        <v>0.4848484848484849</v>
       </c>
       <c r="AM5">
-        <v>0.696969696969697</v>
+        <v>0.4626865671641791</v>
       </c>
       <c r="AN5">
-        <v>22.5</v>
+        <v>45.5</v>
       </c>
       <c r="AO5">
-        <v>51.5</v>
+        <v>39.5</v>
       </c>
       <c r="AP5">
-        <v>73.2</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="AQ5">
         <v>75.09999999999999</v>
       </c>
       <c r="AR5">
-        <v>0.4545454545454545</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="AS5">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="AT5">
-        <v>0.4887791237416139</v>
+        <v>0.5188261324245436</v>
       </c>
       <c r="AU5">
-        <v>0.4921000768022141</v>
+        <v>0.4870639960032235</v>
       </c>
       <c r="AV5">
-        <v>0.02</v>
+        <v>-0.84</v>
       </c>
       <c r="AW5">
-        <v>2.16</v>
+        <v>-8.550000000000001</v>
       </c>
       <c r="AX5">
-        <v>0</v>
+        <v>0.2500043071515946</v>
       </c>
       <c r="AY5">
-        <v>0.02967047393987132</v>
+        <v>0.03251883489450622</v>
       </c>
       <c r="AZ5">
-        <v>0</v>
+        <v>0.2133217592592592</v>
       </c>
       <c r="BA5">
-        <v>0.03684343434343434</v>
+        <v>0.04824523217247097</v>
       </c>
       <c r="BB5">
-        <v>0.5194559870106303</v>
+        <v>0.5179657086019411</v>
       </c>
     </row>
     <row r="6" spans="1:54">
@@ -1385,10 +1385,10 @@
         <v>2023</v>
       </c>
       <c r="D6">
-        <v>212.5</v>
+        <v>237.5</v>
       </c>
       <c r="E6">
-        <v>-2</v>
+        <v>3.5</v>
       </c>
       <c r="F6" t="s">
         <v>57</v>
@@ -1397,145 +1397,145 @@
         <v>63</v>
       </c>
       <c r="H6">
-        <v>0.359375</v>
+        <v>0.4090909090909091</v>
       </c>
       <c r="I6">
-        <v>0.5538461538461539</v>
+        <v>0.609375</v>
       </c>
       <c r="J6">
-        <v>108.3283582089552</v>
+        <v>112.3030303030303</v>
       </c>
       <c r="K6">
-        <v>111.9411764705882</v>
+        <v>118.1818181818182</v>
       </c>
       <c r="L6">
-        <v>95.81343283582088</v>
+        <v>100.6090909090909</v>
       </c>
       <c r="M6">
-        <v>94.6941176470588</v>
+        <v>100.6257575757576</v>
       </c>
       <c r="N6">
-        <v>112.4701492537313</v>
+        <v>111.1590909090909</v>
       </c>
       <c r="O6">
-        <v>116.8117647058824</v>
+        <v>116.2181818181818</v>
       </c>
       <c r="P6">
-        <v>113.2731343283582</v>
+        <v>120.9909090909091</v>
       </c>
       <c r="Q6">
-        <v>111.1</v>
+        <v>115.0924242424242</v>
       </c>
       <c r="R6">
-        <v>78.22388059701495</v>
+        <v>75.42272727272727</v>
       </c>
       <c r="S6">
-        <v>77.50294117647056</v>
+        <v>72.85151515151516</v>
       </c>
       <c r="T6">
-        <v>0.4042686567164178</v>
+        <v>0.3376060606060606</v>
       </c>
       <c r="U6">
-        <v>0.3727794117647058</v>
+        <v>0.3678636363636363</v>
       </c>
       <c r="V6">
-        <v>0.5663283582089553</v>
+        <v>0.5577575757575757</v>
       </c>
       <c r="W6">
-        <v>0.5924852941176471</v>
+        <v>0.574681818181818</v>
       </c>
       <c r="X6">
-        <v>0.2747910447761194</v>
+        <v>0.2331969696969697</v>
       </c>
       <c r="Y6">
-        <v>0.2699264705882354</v>
+        <v>0.2529848484848485</v>
       </c>
       <c r="Z6">
-        <v>11.81194029850747</v>
+        <v>12.95909090909091</v>
       </c>
       <c r="AA6">
-        <v>11.92058823529412</v>
+        <v>11.03484848484849</v>
       </c>
       <c r="AB6">
-        <v>14.24477611940299</v>
+        <v>11.68787878787879</v>
       </c>
       <c r="AC6">
-        <v>13.43970588235294</v>
+        <v>14.08787878787879</v>
       </c>
       <c r="AD6">
-        <v>0.2163955223880598</v>
+        <v>0.1899166666666667</v>
       </c>
       <c r="AE6">
-        <v>0.209375</v>
+        <v>0.2169772727272727</v>
       </c>
       <c r="AF6">
-        <v>0.9460991983314867</v>
+        <v>0.9808124917295222</v>
       </c>
       <c r="AG6">
-        <v>0.9776521962496789</v>
+        <v>1.032155617308456</v>
       </c>
       <c r="AH6">
-        <v>1.067741342886011</v>
+        <v>1.03291958985429</v>
       </c>
       <c r="AI6">
-        <v>1.000525486074619</v>
+        <v>1.035128205128205</v>
       </c>
       <c r="AJ6">
-        <v>9.410042364650762</v>
+        <v>10.54136110033076</v>
       </c>
       <c r="AK6">
-        <v>10.67140537762314</v>
+        <v>12.64900174634597</v>
       </c>
       <c r="AL6">
-        <v>0.5223880597014925</v>
+        <v>0.2575757575757576</v>
       </c>
       <c r="AM6">
-        <v>0.6176470588235294</v>
+        <v>0.4696969696969697</v>
       </c>
       <c r="AN6">
-        <v>49.5</v>
+        <v>22.5</v>
       </c>
       <c r="AO6">
-        <v>46.5</v>
+        <v>23.5</v>
       </c>
       <c r="AP6">
-        <v>76.2</v>
+        <v>73.2</v>
       </c>
       <c r="AQ6">
-        <v>77.2</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="AR6">
-        <v>0.5945945945945946</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="AS6">
-        <v>0.375</v>
+        <v>0.3157894736842105</v>
       </c>
       <c r="AT6">
-        <v>0.5093089740497807</v>
+        <v>0.4919335263662818</v>
       </c>
       <c r="AU6">
-        <v>0.491706430832801</v>
+        <v>0.5081090765260694</v>
       </c>
       <c r="AV6">
-        <v>4.23</v>
+        <v>0.02</v>
       </c>
       <c r="AW6">
-        <v>2.04</v>
+        <v>-7.9</v>
       </c>
       <c r="AX6">
-        <v>0.1040707645094322</v>
+        <v>0</v>
       </c>
       <c r="AY6">
+        <v>0.04072586953120923</v>
+      </c>
+      <c r="AZ6">
         <v>0</v>
       </c>
-      <c r="AZ6">
-        <v>0.1266272802653399</v>
-      </c>
       <c r="BA6">
-        <v>0</v>
+        <v>0.04276830808080808</v>
       </c>
       <c r="BB6">
-        <v>0.5714803477360895</v>
+        <v>0.4828193237373674</v>
       </c>
     </row>
     <row r="7" spans="1:54">
@@ -1546,10 +1546,10 @@
         <v>2023</v>
       </c>
       <c r="D7">
-        <v>224.5</v>
+        <v>225.5</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>-2.5</v>
       </c>
       <c r="F7" t="s">
         <v>58</v>
@@ -1558,145 +1558,145 @@
         <v>64</v>
       </c>
       <c r="H7">
-        <v>0.4923076923076923</v>
+        <v>0.5</v>
       </c>
       <c r="I7">
+        <v>0.5606060606060606</v>
+      </c>
+      <c r="J7">
+        <v>116.7164179104478</v>
+      </c>
+      <c r="K7">
+        <v>115.3382352941177</v>
+      </c>
+      <c r="L7">
+        <v>101.3238805970149</v>
+      </c>
+      <c r="M7">
+        <v>96.04117647058824</v>
+      </c>
+      <c r="N7">
+        <v>114.1686567164179</v>
+      </c>
+      <c r="O7">
+        <v>118.2220588235294</v>
+      </c>
+      <c r="P7">
+        <v>114.7611940298508</v>
+      </c>
+      <c r="Q7">
+        <v>115.2808823529411</v>
+      </c>
+      <c r="R7">
+        <v>76.41492537313432</v>
+      </c>
+      <c r="S7">
+        <v>76.61176470588234</v>
+      </c>
+      <c r="T7">
+        <v>0.3472835820895522</v>
+      </c>
+      <c r="U7">
+        <v>0.3987205882352943</v>
+      </c>
+      <c r="V7">
+        <v>0.5793582089552238</v>
+      </c>
+      <c r="W7">
+        <v>0.5737058823529413</v>
+      </c>
+      <c r="X7">
+        <v>0.2943432835820896</v>
+      </c>
+      <c r="Y7">
+        <v>0.2870882352941176</v>
+      </c>
+      <c r="Z7">
+        <v>11.85223880597015</v>
+      </c>
+      <c r="AA7">
+        <v>10.66470588235294</v>
+      </c>
+      <c r="AB7">
+        <v>10.48059701492537</v>
+      </c>
+      <c r="AC7">
+        <v>10.72352941176471</v>
+      </c>
+      <c r="AD7">
+        <v>0.2044850746268657</v>
+      </c>
+      <c r="AE7">
+        <v>0.2163529411764706</v>
+      </c>
+      <c r="AF7">
+        <v>1.019357361663299</v>
+      </c>
+      <c r="AG7">
+        <v>1.007320832263036</v>
+      </c>
+      <c r="AH7">
+        <v>0.9910059676044332</v>
+      </c>
+      <c r="AI7">
+        <v>1.020187853287432</v>
+      </c>
+      <c r="AJ7">
+        <v>10.52616635881319</v>
+      </c>
+      <c r="AK7">
+        <v>11.22839139665168</v>
+      </c>
+      <c r="AL7">
         <v>0.4925373134328358</v>
       </c>
-      <c r="J7">
-        <v>116.6363636363636</v>
-      </c>
-      <c r="K7">
-        <v>112.3880597014925</v>
-      </c>
-      <c r="L7">
-        <v>101.3469696969697</v>
-      </c>
-      <c r="M7">
-        <v>96.52388059701495</v>
-      </c>
-      <c r="N7">
-        <v>114.0469696969697</v>
-      </c>
-      <c r="O7">
-        <v>115.6746268656716</v>
-      </c>
-      <c r="P7">
-        <v>114.8</v>
-      </c>
-      <c r="Q7">
-        <v>115.3223880597015</v>
-      </c>
-      <c r="R7">
-        <v>76.43636363636362</v>
-      </c>
-      <c r="S7">
-        <v>76.75223880597012</v>
-      </c>
-      <c r="T7">
-        <v>0.3468636363636364</v>
-      </c>
-      <c r="U7">
-        <v>0.3534029850746268</v>
-      </c>
-      <c r="V7">
-        <v>0.5776818181818182</v>
-      </c>
-      <c r="W7">
-        <v>0.5547164179104477</v>
-      </c>
-      <c r="X7">
-        <v>0.2951969696969697</v>
-      </c>
-      <c r="Y7">
-        <v>0.270865671641791</v>
-      </c>
-      <c r="Z7">
-        <v>11.75151515151515</v>
-      </c>
-      <c r="AA7">
-        <v>10.18656716417911</v>
-      </c>
-      <c r="AB7">
-        <v>10.46212121212121</v>
-      </c>
-      <c r="AC7">
-        <v>14.57462686567164</v>
-      </c>
-      <c r="AD7">
-        <v>0.2049545454545454</v>
-      </c>
-      <c r="AE7">
-        <v>0.219955223880597</v>
-      </c>
-      <c r="AF7">
-        <v>1.018658197697499</v>
-      </c>
-      <c r="AG7">
-        <v>0.9815551065632536</v>
-      </c>
-      <c r="AH7">
-        <v>0.9345284489477786</v>
-      </c>
-      <c r="AI7">
-        <v>0.9757857459052679</v>
-      </c>
-      <c r="AJ7">
-        <v>10.58534774000644</v>
-      </c>
-      <c r="AK7">
-        <v>10.3519487297754</v>
-      </c>
-      <c r="AL7">
-        <v>0.4848484848484849</v>
-      </c>
       <c r="AM7">
-        <v>0.4776119402985075</v>
+        <v>0.5735294117647058</v>
       </c>
       <c r="AN7">
         <v>44.5</v>
       </c>
       <c r="AO7">
-        <v>46.5</v>
+        <v>38.5</v>
       </c>
       <c r="AP7">
         <v>75</v>
       </c>
       <c r="AQ7">
-        <v>74.90000000000001</v>
+        <v>75.8</v>
       </c>
       <c r="AR7">
         <v>0.4736842105263158</v>
       </c>
       <c r="AS7">
-        <v>0.3636363636363636</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="AT7">
-        <v>0.5112498936184414</v>
+        <v>0.5107478346136662</v>
       </c>
       <c r="AU7">
-        <v>0.4607480785545702</v>
+        <v>0.5084661876733064</v>
       </c>
       <c r="AV7">
         <v>-3.08</v>
       </c>
       <c r="AW7">
-        <v>2.37</v>
+        <v>-0.01</v>
       </c>
       <c r="AX7">
-        <v>0.2661314137544454</v>
+        <v>0.2579974119485635</v>
       </c>
       <c r="AY7">
         <v>0</v>
       </c>
       <c r="AZ7">
-        <v>0.1375957491582491</v>
+        <v>0.1334501105583195</v>
       </c>
       <c r="BA7">
         <v>0</v>
       </c>
       <c r="BB7">
-        <v>0.4706578153960231</v>
+        <v>0.4371395398434437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Housekeeping changes: improve directory structure, make names more consistent, and delete unnecessary files
</commit_message>
<xml_diff>
--- a/current_games_spread.xlsx
+++ b/current_games_spread.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>year</t>
   </si>
@@ -175,40 +175,46 @@
     <t>calc_home_prob</t>
   </si>
   <si>
-    <t>Denver</t>
-  </si>
-  <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
-    <t>Philadelphia</t>
-  </si>
-  <si>
-    <t>NewOrleans</t>
-  </si>
-  <si>
-    <t>SanAntonio</t>
-  </si>
-  <si>
-    <t>LALakers</t>
-  </si>
-  <si>
-    <t>Brooklyn</t>
-  </si>
-  <si>
-    <t>Cleveland</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>Portland</t>
-  </si>
-  <si>
-    <t>OklahomaCity</t>
-  </si>
-  <si>
-    <t>NewYork</t>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>GoldenState</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Milwaukee</t>
   </si>
 </sst>
 </file>
@@ -566,7 +572,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB7"/>
+  <dimension ref="A1:BB8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -741,157 +747,157 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>230.5</v>
+        <v>226.5</v>
       </c>
       <c r="E2">
-        <v>-9</v>
+        <v>3.5</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H2">
-        <v>0.5454545454545454</v>
+        <v>0.4461538461538462</v>
       </c>
       <c r="I2">
-        <v>0.5454545454545454</v>
+        <v>0.5441176470588235</v>
       </c>
       <c r="J2">
-        <v>116.8805970149254</v>
+        <v>111.3382352941177</v>
       </c>
       <c r="K2">
-        <v>113.7462686567164</v>
+        <v>115.8088235294118</v>
       </c>
       <c r="L2">
-        <v>97.88358208955219</v>
+        <v>99.05588235294118</v>
       </c>
       <c r="M2">
-        <v>97.95074626865674</v>
+        <v>100.0455882352941</v>
       </c>
       <c r="N2">
-        <v>118.9134328358209</v>
+        <v>111.5573529411765</v>
       </c>
       <c r="O2">
-        <v>115.8492537313433</v>
+        <v>115.3838235294117</v>
       </c>
       <c r="P2">
-        <v>114.9223880597015</v>
+        <v>119.135294117647</v>
       </c>
       <c r="Q2">
-        <v>114.8880597014925</v>
+        <v>117.4573529411765</v>
       </c>
       <c r="R2">
-        <v>77.12388059701497</v>
+        <v>74.49999999999999</v>
       </c>
       <c r="S2">
-        <v>74.20447761194028</v>
+        <v>72.68529411764706</v>
       </c>
       <c r="T2">
-        <v>0.363134328358209</v>
+        <v>0.3750882352941175</v>
       </c>
       <c r="U2">
-        <v>0.3902388059701493</v>
+        <v>0.4259117647058823</v>
       </c>
       <c r="V2">
-        <v>0.6079552238805968</v>
+        <v>0.5627205882352941</v>
       </c>
       <c r="W2">
-        <v>0.6038656716417912</v>
+        <v>0.5801617647058823</v>
       </c>
       <c r="X2">
-        <v>0.2607014925373135</v>
+        <v>0.3047941176470588</v>
       </c>
       <c r="Y2">
-        <v>0.2556865671641791</v>
+        <v>0.2639558823529413</v>
       </c>
       <c r="Z2">
-        <v>12.70149253731343</v>
+        <v>12.76323529411765</v>
       </c>
       <c r="AA2">
-        <v>12.22388059701493</v>
+        <v>12.18823529411765</v>
       </c>
       <c r="AB2">
-        <v>11.82686567164179</v>
+        <v>11.83676470588236</v>
       </c>
       <c r="AC2">
-        <v>11.65074626865672</v>
+        <v>12.72205882352941</v>
       </c>
       <c r="AD2">
-        <v>0.2015149253731344</v>
+        <v>0.231860294117647</v>
       </c>
       <c r="AE2">
-        <v>0.2110597014925373</v>
+        <v>0.2233088235294117</v>
       </c>
       <c r="AF2">
-        <v>1.020791240305025</v>
+        <v>0.9723863344464424</v>
       </c>
       <c r="AG2">
-        <v>0.9934171935084404</v>
+        <v>1.011430773182636</v>
       </c>
       <c r="AH2">
-        <v>0.9525390541863533</v>
+        <v>1.002949852507375</v>
       </c>
       <c r="AI2">
-        <v>1.04032716616367</v>
+        <v>1.145566137566137</v>
       </c>
       <c r="AJ2">
-        <v>11.12416005624721</v>
+        <v>12.04844424191435</v>
       </c>
       <c r="AK2">
-        <v>11.25331564218959</v>
+        <v>11.51885583694785</v>
       </c>
       <c r="AL2">
-        <v>0.6865671641791045</v>
+        <v>0.2205882352941176</v>
       </c>
       <c r="AM2">
-        <v>0.5671641791044776</v>
+        <v>0.4558823529411765</v>
       </c>
       <c r="AN2">
-        <v>51.5</v>
+        <v>29.5</v>
       </c>
       <c r="AO2">
-        <v>50.5</v>
+        <v>24.5</v>
       </c>
       <c r="AP2">
-        <v>75.09999999999999</v>
+        <v>74.2</v>
       </c>
       <c r="AQ2">
-        <v>76.5</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="AR2">
-        <v>0.75</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="AS2">
-        <v>0.6</v>
+        <v>0.4782608695652174</v>
       </c>
       <c r="AT2">
-        <v>0.4884292375388056</v>
+        <v>0.5119035347306004</v>
       </c>
       <c r="AU2">
-        <v>0.5079099556161815</v>
+        <v>0.4727089953443124</v>
       </c>
       <c r="AV2">
-        <v>2.16</v>
+        <v>-7.35</v>
       </c>
       <c r="AW2">
-        <v>0.82</v>
+        <v>-3.26</v>
       </c>
       <c r="AX2">
-        <v>0.02916223103971095</v>
+        <v>0.6321074993393103</v>
       </c>
       <c r="AY2">
-        <v>0</v>
+        <v>0.5142321128218399</v>
       </c>
       <c r="AZ2">
-        <v>0.03629353233830845</v>
+        <v>0.4928799019607844</v>
       </c>
       <c r="BA2">
-        <v>0</v>
+        <v>0.4065349264705883</v>
       </c>
       <c r="BB2">
-        <v>0.5279092519844266</v>
+        <v>0.381732064145563</v>
       </c>
     </row>
     <row r="3" spans="1:54">
@@ -902,157 +908,157 @@
         <v>2023</v>
       </c>
       <c r="D3">
-        <v>220</v>
+        <v>244.5</v>
       </c>
       <c r="E3">
-        <v>8</v>
+        <v>-5.5</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H3">
         <v>0.4477611940298508</v>
       </c>
       <c r="I3">
-        <v>0.5454545454545454</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="J3">
-        <v>111.8235294117647</v>
+        <v>117.2794117647059</v>
       </c>
       <c r="K3">
-        <v>111.9855072463768</v>
+        <v>115.4117647058823</v>
       </c>
       <c r="L3">
-        <v>100.4867647058824</v>
+        <v>99.86617647058823</v>
       </c>
       <c r="M3">
-        <v>94.70434782608693</v>
+        <v>100.5676470588235</v>
       </c>
       <c r="N3">
-        <v>110.375</v>
+        <v>116.6279411764706</v>
       </c>
       <c r="O3">
-        <v>116.8666666666667</v>
+        <v>114.1926470588236</v>
       </c>
       <c r="P3">
-        <v>116.0191176470588</v>
+        <v>116.5838235294117</v>
       </c>
       <c r="Q3">
-        <v>111.2985507246377</v>
+        <v>114.4411764705882</v>
       </c>
       <c r="R3">
-        <v>75.62352941176475</v>
+        <v>76.1705882352941</v>
       </c>
       <c r="S3">
-        <v>77.39855072463766</v>
+        <v>74.17941176470589</v>
       </c>
       <c r="T3">
-        <v>0.3563382352941177</v>
+        <v>0.331735294117647</v>
       </c>
       <c r="U3">
-        <v>0.374623188405797</v>
+        <v>0.3853676470588236</v>
       </c>
       <c r="V3">
-        <v>0.5497647058823528</v>
+        <v>0.5791911764705886</v>
       </c>
       <c r="W3">
-        <v>0.5926521739130435</v>
+        <v>0.5939411764705883</v>
       </c>
       <c r="X3">
-        <v>0.2632647058823531</v>
+        <v>0.2402352941176471</v>
       </c>
       <c r="Y3">
-        <v>0.2695507246376813</v>
+        <v>0.2707058823529411</v>
       </c>
       <c r="Z3">
-        <v>11.5764705882353</v>
+        <v>10.81323529411764</v>
       </c>
       <c r="AA3">
-        <v>11.89855072463768</v>
+        <v>13.36764705882353</v>
       </c>
       <c r="AB3">
-        <v>12.41176470588235</v>
+        <v>12.00735294117647</v>
       </c>
       <c r="AC3">
-        <v>13.45942028985507</v>
+        <v>13.09558823529411</v>
       </c>
       <c r="AD3">
-        <v>0.2055294117647059</v>
+        <v>0.2061764705882353</v>
       </c>
       <c r="AE3">
-        <v>0.2096304347826087</v>
+        <v>0.2167794117647059</v>
       </c>
       <c r="AF3">
-        <v>0.9766247110197791</v>
+        <v>1.024274338556383</v>
       </c>
       <c r="AG3">
-        <v>0.9780393645971774</v>
+        <v>1.007963010531724</v>
       </c>
       <c r="AH3">
-        <v>0.9270559354725583</v>
+        <v>1.026039707419018</v>
       </c>
       <c r="AI3">
-        <v>1.003105991976187</v>
+        <v>1.025314305130819</v>
       </c>
       <c r="AJ3">
-        <v>11.55032616864459</v>
+        <v>10.88961403226149</v>
       </c>
       <c r="AK3">
-        <v>10.60009947126309</v>
+        <v>10.87392360341344</v>
       </c>
       <c r="AL3">
-        <v>0.3235294117647059</v>
+        <v>0.5</v>
       </c>
       <c r="AM3">
-        <v>0.6086956521739131</v>
+        <v>0.5</v>
       </c>
       <c r="AN3">
-        <v>34.5</v>
+        <v>46.5</v>
       </c>
       <c r="AO3">
-        <v>46.5</v>
+        <v>49.5</v>
       </c>
       <c r="AP3">
-        <v>75.59999999999999</v>
+        <v>76.8</v>
       </c>
       <c r="AQ3">
-        <v>77.2</v>
+        <v>75.7</v>
       </c>
       <c r="AR3">
-        <v>0.4666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="AS3">
-        <v>0.3529411764705883</v>
+        <v>0.5</v>
       </c>
       <c r="AT3">
-        <v>0.5026769579206853</v>
+        <v>0.4917082551118301</v>
       </c>
       <c r="AU3">
-        <v>0.492151092120753</v>
+        <v>0.5078199054889029</v>
       </c>
       <c r="AV3">
-        <v>0.53</v>
+        <v>1.55</v>
       </c>
       <c r="AW3">
-        <v>2.04</v>
+        <v>2.53</v>
       </c>
       <c r="AX3">
         <v>0</v>
       </c>
       <c r="AY3">
-        <v>0</v>
+        <v>0.1477877086718865</v>
       </c>
       <c r="AZ3">
         <v>0</v>
       </c>
       <c r="BA3">
-        <v>0</v>
+        <v>0.1174101307189543</v>
       </c>
       <c r="BB3">
-        <v>0.5706285307576093</v>
+        <v>0.5216044800801791</v>
       </c>
     </row>
     <row r="4" spans="1:54">
@@ -1063,157 +1069,157 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>227.5</v>
+        <v>224.5</v>
       </c>
       <c r="E4">
-        <v>-7.5</v>
+        <v>1.5</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H4">
-        <v>0.5692307692307692</v>
+        <v>0.3692307692307693</v>
       </c>
       <c r="I4">
         <v>0.484375</v>
       </c>
       <c r="J4">
-        <v>115.0909090909091</v>
+        <v>113.8970588235294</v>
       </c>
       <c r="K4">
-        <v>113.2238805970149</v>
+        <v>115.7878787878788</v>
       </c>
       <c r="L4">
-        <v>96.45454545454545</v>
+        <v>95.55882352941178</v>
       </c>
       <c r="M4">
-        <v>97.78656716417913</v>
+        <v>100.5651515151515</v>
       </c>
       <c r="N4">
-        <v>118.4818181818182</v>
+        <v>117.7823529411765</v>
       </c>
       <c r="O4">
-        <v>115.4029850746269</v>
+        <v>114.8757575757576</v>
       </c>
       <c r="P4">
-        <v>114.359090909091</v>
+        <v>117.1205882352941</v>
       </c>
       <c r="Q4">
-        <v>115.6686567164179</v>
+        <v>111.0136363636364</v>
       </c>
       <c r="R4">
-        <v>77.52727272727272</v>
+        <v>76.65000000000001</v>
       </c>
       <c r="S4">
-        <v>76.34477611940301</v>
+        <v>75.72727272727271</v>
       </c>
       <c r="T4">
-        <v>0.3911969696969697</v>
+        <v>0.48925</v>
       </c>
       <c r="U4">
-        <v>0.3629701492537314</v>
+        <v>0.3619242424242424</v>
       </c>
       <c r="V4">
-        <v>0.6071060606060608</v>
+        <v>0.6000735294117647</v>
       </c>
       <c r="W4">
-        <v>0.589373134328358</v>
+        <v>0.5629242424242427</v>
       </c>
       <c r="X4">
-        <v>0.3085909090909091</v>
+        <v>0.3157205882352941</v>
       </c>
       <c r="Y4">
-        <v>0.2648805970149253</v>
+        <v>0.2699242424242424</v>
       </c>
       <c r="Z4">
-        <v>11.81818181818182</v>
+        <v>10.96029411764705</v>
       </c>
       <c r="AA4">
-        <v>12.40746268656716</v>
+        <v>11.17424242424242</v>
       </c>
       <c r="AB4">
-        <v>12.56212121212121</v>
+        <v>11.74264705882353</v>
       </c>
       <c r="AC4">
-        <v>10.64029850746269</v>
+        <v>12.74393939393939</v>
       </c>
       <c r="AD4">
-        <v>0.2396818181818181</v>
+        <v>0.2355441176470588</v>
       </c>
       <c r="AE4">
-        <v>0.2038059701492537</v>
+        <v>0.2035151515151514</v>
       </c>
       <c r="AF4">
-        <v>1.005160778086542</v>
+        <v>0.9947341381967634</v>
       </c>
       <c r="AG4">
-        <v>0.9888548523756762</v>
+        <v>1.011247849675797</v>
       </c>
       <c r="AH4">
-        <v>1.11216429699842</v>
+        <v>0.9774908543146116</v>
       </c>
       <c r="AI4">
-        <v>1.018630811143334</v>
+        <v>0.9960743260926459</v>
       </c>
       <c r="AJ4">
-        <v>12.31250568094288</v>
+        <v>11.84227187300591</v>
       </c>
       <c r="AK4">
-        <v>10.8940910938849</v>
+        <v>11.49376003503133</v>
       </c>
       <c r="AL4">
-        <v>0.6666666666666666</v>
+        <v>0.5</v>
       </c>
       <c r="AM4">
-        <v>0.4626865671641791</v>
+        <v>0.6060606060606061</v>
       </c>
       <c r="AN4">
-        <v>50.5</v>
+        <v>48.5</v>
       </c>
       <c r="AO4">
-        <v>35.5</v>
+        <v>49.5</v>
       </c>
       <c r="AP4">
-        <v>76.2</v>
+        <v>75.3</v>
       </c>
       <c r="AQ4">
-        <v>76.09999999999999</v>
+        <v>75.2</v>
       </c>
       <c r="AR4">
-        <v>0.7</v>
+        <v>0.5517241379310345</v>
       </c>
       <c r="AS4">
-        <v>0.5555555555555556</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="AT4">
-        <v>0.4820341586818817</v>
+        <v>0.4969860149582434</v>
       </c>
       <c r="AU4">
-        <v>0.489537703351612</v>
+        <v>0.4781875547917167</v>
       </c>
       <c r="AV4">
-        <v>2.57</v>
+        <v>3.12</v>
       </c>
       <c r="AW4">
-        <v>-3.23</v>
+        <v>5.37</v>
       </c>
       <c r="AX4">
-        <v>0</v>
+        <v>0.3082118879973798</v>
       </c>
       <c r="AY4">
-        <v>0</v>
+        <v>0.2629182021531677</v>
       </c>
       <c r="AZ4">
-        <v>0</v>
+        <v>0.1266860702614379</v>
       </c>
       <c r="BA4">
-        <v>0</v>
+        <v>0.2080092592592592</v>
       </c>
       <c r="BB4">
-        <v>0.5007639899963852</v>
+        <v>0.5184085503671141</v>
       </c>
     </row>
     <row r="5" spans="1:54">
@@ -1224,157 +1230,157 @@
         <v>2023</v>
       </c>
       <c r="D5">
-        <v>230.5</v>
+        <v>225.5</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>-8</v>
       </c>
       <c r="F5" t="s">
         <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H5">
-        <v>0.4545454545454545</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="I5">
-        <v>0.5074626865671642</v>
+        <v>0.5606060606060606</v>
       </c>
       <c r="J5">
-        <v>114.0757575757576</v>
+        <v>108.5652173913043</v>
       </c>
       <c r="K5">
-        <v>114.6268656716418</v>
+        <v>117.2647058823529</v>
       </c>
       <c r="L5">
-        <v>98.60303030303029</v>
+        <v>95.85942028985505</v>
       </c>
       <c r="M5">
-        <v>97.2014925373134</v>
+        <v>99.68235294117649</v>
       </c>
       <c r="N5">
-        <v>114.6636363636364</v>
+        <v>112.5246376811594</v>
       </c>
       <c r="O5">
-        <v>117.5970149253731</v>
+        <v>116.9926470588235</v>
       </c>
       <c r="P5">
-        <v>114.0530303030303</v>
+        <v>113.4014492753623</v>
       </c>
       <c r="Q5">
-        <v>118.7835820895522</v>
+        <v>117.0705882352941</v>
       </c>
       <c r="R5">
-        <v>77.1878787878788</v>
+        <v>78.10289855072466</v>
       </c>
       <c r="S5">
-        <v>75.67014925373135</v>
+        <v>74.9911764705882</v>
       </c>
       <c r="T5">
-        <v>0.3455303030303031</v>
+        <v>0.403391304347826</v>
       </c>
       <c r="U5">
-        <v>0.4193134328358208</v>
+        <v>0.4318970588235295</v>
       </c>
       <c r="V5">
-        <v>0.5800151515151516</v>
+        <v>0.5673043478260872</v>
       </c>
       <c r="W5">
-        <v>0.6003432835820898</v>
+        <v>0.5878676470588234</v>
       </c>
       <c r="X5">
-        <v>0.2836363636363636</v>
+        <v>0.2739710144927537</v>
       </c>
       <c r="Y5">
-        <v>0.3039701492537314</v>
+        <v>0.2730294117647058</v>
       </c>
       <c r="Z5">
-        <v>12.56060606060606</v>
+        <v>11.88985507246377</v>
       </c>
       <c r="AA5">
-        <v>12.57910447761194</v>
+        <v>13.08088235294118</v>
       </c>
       <c r="AB5">
-        <v>12.90606060606061</v>
+        <v>14.18985507246377</v>
       </c>
       <c r="AC5">
-        <v>11.51194029850746</v>
+        <v>10.88235294117647</v>
       </c>
       <c r="AD5">
-        <v>0.2182651515151515</v>
+        <v>0.2161231884057971</v>
       </c>
       <c r="AE5">
-        <v>0.2306940298507463</v>
+        <v>0.2111985294117648</v>
       </c>
       <c r="AF5">
-        <v>0.9962948259891492</v>
+        <v>0.9481678374786405</v>
       </c>
       <c r="AG5">
-        <v>1.001107997132243</v>
+        <v>1.024145902902646</v>
       </c>
       <c r="AH5">
-        <v>0.9350511356089787</v>
+        <v>1.022426912294754</v>
       </c>
       <c r="AI5">
-        <v>0.9363715277777777</v>
+        <v>1.040381239026837</v>
       </c>
       <c r="AJ5">
-        <v>10.44075726683016</v>
+        <v>9.383115055307956</v>
       </c>
       <c r="AK5">
-        <v>12.50651868342949</v>
+        <v>9.928594544011613</v>
       </c>
       <c r="AL5">
-        <v>0.4848484848484849</v>
+        <v>0.5217391304347826</v>
       </c>
       <c r="AM5">
-        <v>0.4626865671641791</v>
+        <v>0.4852941176470588</v>
       </c>
       <c r="AN5">
-        <v>45.5</v>
+        <v>49.5</v>
       </c>
       <c r="AO5">
-        <v>39.5</v>
+        <v>23.5</v>
       </c>
       <c r="AP5">
-        <v>77.40000000000001</v>
+        <v>76.2</v>
       </c>
       <c r="AQ5">
-        <v>75.09999999999999</v>
+        <v>74.3</v>
       </c>
       <c r="AR5">
-        <v>0.4705882352941176</v>
+        <v>0.6052631578947368</v>
       </c>
       <c r="AS5">
-        <v>0.5</v>
+        <v>0.4782608695652174</v>
       </c>
       <c r="AT5">
-        <v>0.5188261324245436</v>
+        <v>0.5093381651418217</v>
       </c>
       <c r="AU5">
-        <v>0.4870639960032235</v>
+        <v>0.4952303277325308</v>
       </c>
       <c r="AV5">
-        <v>-0.84</v>
+        <v>4.23</v>
       </c>
       <c r="AW5">
-        <v>-8.550000000000001</v>
+        <v>5.67</v>
       </c>
       <c r="AX5">
-        <v>0.2500043071515946</v>
+        <v>0.04650053654465243</v>
       </c>
       <c r="AY5">
-        <v>0.03251883489450622</v>
+        <v>0.2728716645489199</v>
       </c>
       <c r="AZ5">
-        <v>0.2133217592592592</v>
+        <v>0.0542013888888889</v>
       </c>
       <c r="BA5">
-        <v>0.04824523217247097</v>
+        <v>0.1910365604575164</v>
       </c>
       <c r="BB5">
-        <v>0.5179657086019411</v>
+        <v>0.4905978661794189</v>
       </c>
     </row>
     <row r="6" spans="1:54">
@@ -1385,157 +1391,157 @@
         <v>2023</v>
       </c>
       <c r="D6">
-        <v>237.5</v>
+        <v>231.5</v>
       </c>
       <c r="E6">
-        <v>3.5</v>
+        <v>12.5</v>
       </c>
       <c r="F6" t="s">
         <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H6">
-        <v>0.4090909090909091</v>
+        <v>0.40625</v>
       </c>
       <c r="I6">
-        <v>0.609375</v>
+        <v>0.5441176470588235</v>
       </c>
       <c r="J6">
-        <v>112.3030303030303</v>
+        <v>110.2686567164179</v>
       </c>
       <c r="K6">
-        <v>118.1818181818182</v>
+        <v>117.8529411764706</v>
       </c>
       <c r="L6">
-        <v>100.6090909090909</v>
+        <v>98.61194029850742</v>
       </c>
       <c r="M6">
-        <v>100.6257575757576</v>
+        <v>97.77794117647058</v>
       </c>
       <c r="N6">
-        <v>111.1590909090909</v>
+        <v>111.2716417910448</v>
       </c>
       <c r="O6">
-        <v>116.2181818181818</v>
+        <v>118.5911764705882</v>
       </c>
       <c r="P6">
-        <v>120.9909090909091</v>
+        <v>119.5925373134328</v>
       </c>
       <c r="Q6">
-        <v>115.0924242424242</v>
+        <v>112.875</v>
       </c>
       <c r="R6">
-        <v>75.42272727272727</v>
+        <v>76.25820895522386</v>
       </c>
       <c r="S6">
-        <v>72.85151515151516</v>
+        <v>79.00735294117648</v>
       </c>
       <c r="T6">
-        <v>0.3376060606060606</v>
+        <v>0.368</v>
       </c>
       <c r="U6">
-        <v>0.3678636363636363</v>
+        <v>0.4761470588235292</v>
       </c>
       <c r="V6">
-        <v>0.5577575757575757</v>
+        <v>0.5531044776119403</v>
       </c>
       <c r="W6">
-        <v>0.574681818181818</v>
+        <v>0.6019117647058825</v>
       </c>
       <c r="X6">
-        <v>0.2331969696969697</v>
+        <v>0.2885373134328358</v>
       </c>
       <c r="Y6">
-        <v>0.2529848484848485</v>
+        <v>0.2490294117647059</v>
       </c>
       <c r="Z6">
-        <v>12.95909090909091</v>
+        <v>13.70298507462687</v>
       </c>
       <c r="AA6">
-        <v>11.03484848484849</v>
+        <v>11.62794117647059</v>
       </c>
       <c r="AB6">
-        <v>11.68787878787879</v>
+        <v>11.46865671641791</v>
       </c>
       <c r="AC6">
-        <v>14.08787878787879</v>
+        <v>10.72058823529412</v>
       </c>
       <c r="AD6">
-        <v>0.1899166666666667</v>
+        <v>0.2184626865671641</v>
       </c>
       <c r="AE6">
-        <v>0.2169772727272727</v>
+        <v>0.1953382352941177</v>
       </c>
       <c r="AF6">
-        <v>0.9808124917295222</v>
+        <v>0.9630450368246105</v>
       </c>
       <c r="AG6">
-        <v>1.032155617308456</v>
+        <v>1.029283329052145</v>
       </c>
       <c r="AH6">
-        <v>1.03291958985429</v>
+        <v>1.003609456776755</v>
       </c>
       <c r="AI6">
-        <v>1.035128205128205</v>
+        <v>1.026703269278762</v>
       </c>
       <c r="AJ6">
-        <v>10.54136110033076</v>
+        <v>11.42605309108816</v>
       </c>
       <c r="AK6">
-        <v>12.64900174634597</v>
+        <v>11.83248855765887</v>
       </c>
       <c r="AL6">
-        <v>0.2575757575757576</v>
+        <v>0.2238805970149254</v>
       </c>
       <c r="AM6">
-        <v>0.4696969696969697</v>
+        <v>0.6911764705882353</v>
       </c>
       <c r="AN6">
-        <v>22.5</v>
+        <v>23.5</v>
       </c>
       <c r="AO6">
-        <v>23.5</v>
+        <v>54.5</v>
       </c>
       <c r="AP6">
-        <v>73.2</v>
+        <v>73.7</v>
       </c>
       <c r="AQ6">
-        <v>74.40000000000001</v>
+        <v>78.59999999999999</v>
       </c>
       <c r="AR6">
-        <v>0.4545454545454545</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="AS6">
-        <v>0.3157894736842105</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="AT6">
-        <v>0.4919335263662818</v>
+        <v>0.5240244502285063</v>
       </c>
       <c r="AU6">
-        <v>0.5081090765260694</v>
+        <v>0.4833064703318732</v>
       </c>
       <c r="AV6">
-        <v>0.02</v>
+        <v>-8.26</v>
       </c>
       <c r="AW6">
-        <v>-7.9</v>
+        <v>7.02</v>
       </c>
       <c r="AX6">
         <v>0</v>
       </c>
       <c r="AY6">
-        <v>0.04072586953120923</v>
+        <v>0.06656427584088465</v>
       </c>
       <c r="AZ6">
         <v>0</v>
       </c>
       <c r="BA6">
-        <v>0.04276830808080808</v>
+        <v>0.07608762254901962</v>
       </c>
       <c r="BB6">
-        <v>0.4828193237373674</v>
+        <v>0.5276267923777707</v>
       </c>
     </row>
     <row r="7" spans="1:54">
@@ -1546,157 +1552,318 @@
         <v>2023</v>
       </c>
       <c r="D7">
-        <v>225.5</v>
+        <v>236</v>
       </c>
       <c r="E7">
-        <v>-2.5</v>
+        <v>-4.5</v>
       </c>
       <c r="F7" t="s">
         <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H7">
-        <v>0.5</v>
+        <v>0.4776119402985075</v>
       </c>
       <c r="I7">
-        <v>0.5606060606060606</v>
+        <v>0.5538461538461539</v>
       </c>
       <c r="J7">
-        <v>116.7164179104478</v>
+        <v>118.0882352941177</v>
       </c>
       <c r="K7">
-        <v>115.3382352941177</v>
+        <v>113.3880597014925</v>
       </c>
       <c r="L7">
-        <v>101.3238805970149</v>
+        <v>101.189705882353</v>
       </c>
       <c r="M7">
-        <v>96.04117647058824</v>
+        <v>97.24925373134325</v>
       </c>
       <c r="N7">
-        <v>114.1686567164179</v>
+        <v>115.7882352941176</v>
       </c>
       <c r="O7">
-        <v>118.2220588235294</v>
+        <v>115.9134328358209</v>
       </c>
       <c r="P7">
-        <v>114.7611940298508</v>
+        <v>115.3</v>
       </c>
       <c r="Q7">
-        <v>115.2808823529411</v>
+        <v>113.7014925373134</v>
       </c>
       <c r="R7">
-        <v>76.41492537313432</v>
+        <v>76.43088235294117</v>
       </c>
       <c r="S7">
-        <v>76.61176470588234</v>
+        <v>76.29402985074631</v>
       </c>
       <c r="T7">
-        <v>0.3472835820895522</v>
+        <v>0.4815294117647059</v>
       </c>
       <c r="U7">
-        <v>0.3987205882352943</v>
+        <v>0.3677462686567163</v>
       </c>
       <c r="V7">
-        <v>0.5793582089552238</v>
+        <v>0.5984117647058821</v>
       </c>
       <c r="W7">
-        <v>0.5737058823529413</v>
+        <v>0.5720298507462688</v>
       </c>
       <c r="X7">
-        <v>0.2943432835820896</v>
+        <v>0.2232941176470588</v>
       </c>
       <c r="Y7">
-        <v>0.2870882352941176</v>
+        <v>0.2442238805970149</v>
       </c>
       <c r="Z7">
-        <v>11.85223880597015</v>
+        <v>13.75441176470588</v>
       </c>
       <c r="AA7">
-        <v>10.66470588235294</v>
+        <v>11.73582089552239</v>
       </c>
       <c r="AB7">
-        <v>10.48059701492537</v>
+        <v>12.02794117647059</v>
       </c>
       <c r="AC7">
-        <v>10.72352941176471</v>
+        <v>12.45522388059701</v>
       </c>
       <c r="AD7">
-        <v>0.2044850746268657</v>
+        <v>0.1999632352941177</v>
       </c>
       <c r="AE7">
-        <v>0.2163529411764706</v>
+        <v>0.2154179104477612</v>
       </c>
       <c r="AF7">
-        <v>1.019357361663299</v>
+        <v>1.031338299511945</v>
       </c>
       <c r="AG7">
-        <v>1.007320832263036</v>
+        <v>0.9902887310174021</v>
       </c>
       <c r="AH7">
-        <v>0.9910059676044332</v>
+        <v>1.024657534246575</v>
       </c>
       <c r="AI7">
-        <v>1.020187853287432</v>
+        <v>1.120047387126497</v>
       </c>
       <c r="AJ7">
-        <v>10.52616635881319</v>
+        <v>10.84073919516459</v>
       </c>
       <c r="AK7">
-        <v>11.22839139665168</v>
+        <v>12.27417532127235</v>
       </c>
       <c r="AL7">
-        <v>0.4925373134328358</v>
+        <v>0.5147058823529411</v>
       </c>
       <c r="AM7">
-        <v>0.5735294117647058</v>
+        <v>0.5522388059701493</v>
       </c>
       <c r="AN7">
-        <v>44.5</v>
+        <v>52.5</v>
       </c>
       <c r="AO7">
-        <v>38.5</v>
+        <v>52.5</v>
       </c>
       <c r="AP7">
-        <v>75</v>
+        <v>76.3</v>
       </c>
       <c r="AQ7">
-        <v>75.8</v>
+        <v>77</v>
       </c>
       <c r="AR7">
-        <v>0.4736842105263158</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="AS7">
-        <v>0.6190476190476191</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="AT7">
-        <v>0.5107478346136662</v>
+        <v>0.4714385683098666</v>
       </c>
       <c r="AU7">
-        <v>0.5084661876733064</v>
+        <v>0.5182421709507165</v>
       </c>
       <c r="AV7">
-        <v>-3.08</v>
+        <v>5.52</v>
       </c>
       <c r="AW7">
-        <v>-0.01</v>
+        <v>6.94</v>
       </c>
       <c r="AX7">
-        <v>0.2579974119485635</v>
+        <v>0.07422068283028209</v>
       </c>
       <c r="AY7">
+        <v>0.104940606977748</v>
+      </c>
+      <c r="AZ7">
+        <v>0.07293300653594773</v>
+      </c>
+      <c r="BA7">
+        <v>0.07710933966530982</v>
+      </c>
+      <c r="BB7">
+        <v>0.553060013761983</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2023</v>
+      </c>
+      <c r="D8">
+        <v>244.5</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8">
+        <v>0.5692307692307692</v>
+      </c>
+      <c r="I8">
+        <v>0.5873015873015873</v>
+      </c>
+      <c r="J8">
+        <v>121.2121212121212</v>
+      </c>
+      <c r="K8">
+        <v>115.8805970149254</v>
+      </c>
+      <c r="L8">
+        <v>100.1909090909091</v>
+      </c>
+      <c r="M8">
+        <v>99.67611940298508</v>
+      </c>
+      <c r="N8">
+        <v>119.9772727272727</v>
+      </c>
+      <c r="O8">
+        <v>115.244776119403</v>
+      </c>
+      <c r="P8">
+        <v>117.3015151515152</v>
+      </c>
+      <c r="Q8">
+        <v>111.4044776119403</v>
+      </c>
+      <c r="R8">
+        <v>77.42121212121212</v>
+      </c>
+      <c r="S8">
+        <v>77.94328358208958</v>
+      </c>
+      <c r="T8">
+        <v>0.4156666666666666</v>
+      </c>
+      <c r="U8">
+        <v>0.4485223880597016</v>
+      </c>
+      <c r="V8">
+        <v>0.6145757575757574</v>
+      </c>
+      <c r="W8">
+        <v>0.5789850746268654</v>
+      </c>
+      <c r="X8">
+        <v>0.2936969696969697</v>
+      </c>
+      <c r="Y8">
+        <v>0.2517313432835822</v>
+      </c>
+      <c r="Z8">
+        <v>12.16363636363636</v>
+      </c>
+      <c r="AA8">
+        <v>12.27761194029851</v>
+      </c>
+      <c r="AB8">
+        <v>12.21666666666667</v>
+      </c>
+      <c r="AC8">
+        <v>10.2955223880597</v>
+      </c>
+      <c r="AD8">
+        <v>0.2187348484848485</v>
+      </c>
+      <c r="AE8">
+        <v>0.1839776119402985</v>
+      </c>
+      <c r="AF8">
+        <v>1.058621145957391</v>
+      </c>
+      <c r="AG8">
+        <v>1.012057615850877</v>
+      </c>
+      <c r="AH8">
+        <v>1.02575</v>
+      </c>
+      <c r="AI8">
+        <v>1.058560879271853</v>
+      </c>
+      <c r="AJ8">
+        <v>13.41811885780854</v>
+      </c>
+      <c r="AK8">
+        <v>12.74728228344075</v>
+      </c>
+      <c r="AL8">
+        <v>0.6060606060606061</v>
+      </c>
+      <c r="AM8">
+        <v>0.7164179104477612</v>
+      </c>
+      <c r="AN8">
+        <v>34.5</v>
+      </c>
+      <c r="AO8">
+        <v>53.5</v>
+      </c>
+      <c r="AP8">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="AQ8">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="AR8">
+        <v>0.5652173913043478</v>
+      </c>
+      <c r="AS8">
+        <v>0.6923076923076923</v>
+      </c>
+      <c r="AT8">
+        <v>0.4772801085419492</v>
+      </c>
+      <c r="AU8">
+        <v>0.4889211652235649</v>
+      </c>
+      <c r="AV8">
+        <v>-5.26</v>
+      </c>
+      <c r="AW8">
+        <v>3.22</v>
+      </c>
+      <c r="AX8">
         <v>0</v>
       </c>
-      <c r="AZ7">
-        <v>0.1334501105583195</v>
-      </c>
-      <c r="BA7">
+      <c r="AY8">
         <v>0</v>
       </c>
-      <c r="BB7">
-        <v>0.4371395398434437</v>
+      <c r="AZ8">
+        <v>0</v>
+      </c>
+      <c r="BA8">
+        <v>0</v>
+      </c>
+      <c r="BB8">
+        <v>0.5126683611858208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More improvement to file and directory structures, including a main (bets.py) file
</commit_message>
<xml_diff>
--- a/current_games_spread.xlsx
+++ b/current_games_spread.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>year</t>
   </si>
@@ -175,46 +175,40 @@
     <t>calc_home_prob</t>
   </si>
   <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>NewOrleans</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>LAClippers</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
     <t>Detroit</t>
   </si>
   <si>
-    <t>Atlanta</t>
-  </si>
-  <si>
-    <t>Dallas</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>GoldenState</t>
-  </si>
-  <si>
-    <t>Sacramento</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Memphis</t>
-  </si>
-  <si>
-    <t>Utah</t>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>SanAntonio</t>
   </si>
   <si>
     <t>Boston</t>
   </si>
   <si>
-    <t>Phoenix</t>
-  </si>
-  <si>
-    <t>Milwaukee</t>
+    <t>OklahomaCity</t>
   </si>
 </sst>
 </file>
@@ -572,7 +566,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB8"/>
+  <dimension ref="A1:BB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -747,157 +741,157 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>226.5</v>
+        <v>225.5</v>
       </c>
       <c r="E2">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H2">
-        <v>0.4461538461538462</v>
+        <v>0.5492957746478874</v>
       </c>
       <c r="I2">
-        <v>0.5441176470588235</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="J2">
-        <v>111.3382352941177</v>
+        <v>111.5416666666667</v>
       </c>
       <c r="K2">
-        <v>115.8088235294118</v>
+        <v>112.7887323943662</v>
       </c>
       <c r="L2">
-        <v>99.05588235294118</v>
+        <v>98.5152777777778</v>
       </c>
       <c r="M2">
-        <v>100.0455882352941</v>
+        <v>97.5760563380282</v>
       </c>
       <c r="N2">
-        <v>111.5573529411765</v>
+        <v>112.5958333333333</v>
       </c>
       <c r="O2">
-        <v>115.3838235294117</v>
+        <v>115.2154929577465</v>
       </c>
       <c r="P2">
-        <v>119.135294117647</v>
+        <v>115.5027777777778</v>
       </c>
       <c r="Q2">
-        <v>117.4573529411765</v>
+        <v>116.0056338028169</v>
       </c>
       <c r="R2">
-        <v>74.49999999999999</v>
+        <v>77.43888888888891</v>
       </c>
       <c r="S2">
-        <v>72.68529411764706</v>
+        <v>76.32394366197184</v>
       </c>
       <c r="T2">
-        <v>0.3750882352941175</v>
+        <v>0.3583055555555555</v>
       </c>
       <c r="U2">
-        <v>0.4259117647058823</v>
+        <v>0.3620281690140846</v>
       </c>
       <c r="V2">
-        <v>0.5627205882352941</v>
+        <v>0.5745138888888889</v>
       </c>
       <c r="W2">
-        <v>0.5801617647058823</v>
+        <v>0.5877042253521125</v>
       </c>
       <c r="X2">
-        <v>0.3047941176470588</v>
+        <v>0.2960972222222222</v>
       </c>
       <c r="Y2">
-        <v>0.2639558823529413</v>
+        <v>0.2653521126760564</v>
       </c>
       <c r="Z2">
-        <v>12.76323529411765</v>
+        <v>12.84444444444444</v>
       </c>
       <c r="AA2">
-        <v>12.18823529411765</v>
+        <v>12.33802816901409</v>
       </c>
       <c r="AB2">
-        <v>11.83676470588236</v>
+        <v>12.675</v>
       </c>
       <c r="AC2">
-        <v>12.72205882352941</v>
+        <v>10.53098591549296</v>
       </c>
       <c r="AD2">
-        <v>0.231860294117647</v>
+        <v>0.2234652777777777</v>
       </c>
       <c r="AE2">
-        <v>0.2233088235294117</v>
+        <v>0.2039859154929577</v>
       </c>
       <c r="AF2">
-        <v>0.9723863344464424</v>
+        <v>0.9741630276564774</v>
       </c>
       <c r="AG2">
-        <v>1.011430773182636</v>
+        <v>0.9850544313918445</v>
       </c>
       <c r="AH2">
-        <v>1.002949852507375</v>
+        <v>0.9891669779604033</v>
       </c>
       <c r="AI2">
-        <v>1.145566137566137</v>
+        <v>0.9723193473193474</v>
       </c>
       <c r="AJ2">
-        <v>12.04844424191435</v>
+        <v>9.865677737602327</v>
       </c>
       <c r="AK2">
-        <v>11.51885583694785</v>
+        <v>11.10375585861936</v>
       </c>
       <c r="AL2">
-        <v>0.2205882352941176</v>
+        <v>0.4027777777777778</v>
       </c>
       <c r="AM2">
-        <v>0.4558823529411765</v>
+        <v>0.4507042253521127</v>
       </c>
       <c r="AN2">
-        <v>29.5</v>
+        <v>26.5</v>
       </c>
       <c r="AO2">
-        <v>24.5</v>
+        <v>35.5</v>
       </c>
       <c r="AP2">
-        <v>74.2</v>
+        <v>74.59999999999999</v>
       </c>
       <c r="AQ2">
-        <v>75.90000000000001</v>
+        <v>76.09999999999999</v>
       </c>
       <c r="AR2">
-        <v>0.2142857142857143</v>
+        <v>0.4210526315789473</v>
       </c>
       <c r="AS2">
-        <v>0.4782608695652174</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="AT2">
-        <v>0.5119035347306004</v>
+        <v>0.5079325485319064</v>
       </c>
       <c r="AU2">
-        <v>0.4727089953443124</v>
+        <v>0.4917941353870523</v>
       </c>
       <c r="AV2">
-        <v>-7.35</v>
+        <v>-7.67</v>
       </c>
       <c r="AW2">
-        <v>-3.26</v>
+        <v>-3.23</v>
       </c>
       <c r="AX2">
-        <v>0.6321074993393103</v>
+        <v>0.05908832111593485</v>
       </c>
       <c r="AY2">
-        <v>0.5142321128218399</v>
+        <v>0.1457297333377834</v>
       </c>
       <c r="AZ2">
-        <v>0.4928799019607844</v>
+        <v>0.06178337191358026</v>
       </c>
       <c r="BA2">
-        <v>0.4065349264705883</v>
+        <v>0.1313849765258216</v>
       </c>
       <c r="BB2">
-        <v>0.381732064145563</v>
+        <v>0.4868014905179434</v>
       </c>
     </row>
     <row r="3" spans="1:54">
@@ -908,157 +902,157 @@
         <v>2023</v>
       </c>
       <c r="D3">
-        <v>244.5</v>
+        <v>236</v>
       </c>
       <c r="E3">
-        <v>-5.5</v>
+        <v>-14</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3">
-        <v>0.4477611940298508</v>
+        <v>0.4428571428571428</v>
       </c>
       <c r="I3">
-        <v>0.4705882352941176</v>
+        <v>0.4347826086956522</v>
       </c>
       <c r="J3">
-        <v>117.2794117647059</v>
+        <v>117.3943661971831</v>
       </c>
       <c r="K3">
-        <v>115.4117647058823</v>
+        <v>110.9027777777778</v>
       </c>
       <c r="L3">
-        <v>99.86617647058823</v>
+        <v>100.0056338028169</v>
       </c>
       <c r="M3">
-        <v>100.5676470588235</v>
+        <v>98.72916666666666</v>
       </c>
       <c r="N3">
-        <v>116.6279411764706</v>
+        <v>116.6140845070422</v>
       </c>
       <c r="O3">
-        <v>114.1926470588236</v>
+        <v>111.5305555555556</v>
       </c>
       <c r="P3">
-        <v>116.5838235294117</v>
+        <v>116.8619718309859</v>
       </c>
       <c r="Q3">
-        <v>114.4411764705882</v>
+        <v>119.1569444444444</v>
       </c>
       <c r="R3">
-        <v>76.1705882352941</v>
+        <v>76.17887323943661</v>
       </c>
       <c r="S3">
-        <v>74.17941176470589</v>
+        <v>74.3458333333333</v>
       </c>
       <c r="T3">
-        <v>0.331735294117647</v>
+        <v>0.3297605633802816</v>
       </c>
       <c r="U3">
-        <v>0.3853676470588236</v>
+        <v>0.3738472222222221</v>
       </c>
       <c r="V3">
-        <v>0.5791911764705886</v>
+        <v>0.5777464788732399</v>
       </c>
       <c r="W3">
-        <v>0.5939411764705883</v>
+        <v>0.5609305555555556</v>
       </c>
       <c r="X3">
-        <v>0.2402352941176471</v>
+        <v>0.2404647887323945</v>
       </c>
       <c r="Y3">
-        <v>0.2707058823529411</v>
+        <v>0.29675</v>
       </c>
       <c r="Z3">
-        <v>10.81323529411764</v>
+        <v>10.78309859154929</v>
       </c>
       <c r="AA3">
-        <v>13.36764705882353</v>
+        <v>12.71666666666667</v>
       </c>
       <c r="AB3">
-        <v>12.00735294117647</v>
+        <v>11.96760563380282</v>
       </c>
       <c r="AC3">
-        <v>13.09558823529411</v>
+        <v>11.77777777777779</v>
       </c>
       <c r="AD3">
-        <v>0.2061764705882353</v>
+        <v>0.2044929577464789</v>
       </c>
       <c r="AE3">
-        <v>0.2167794117647059</v>
+        <v>0.2285972222222222</v>
       </c>
       <c r="AF3">
-        <v>1.024274338556383</v>
+        <v>1.025278307398979</v>
       </c>
       <c r="AG3">
-        <v>1.007963010531724</v>
+        <v>0.9685832120329937</v>
       </c>
       <c r="AH3">
-        <v>1.026039707419018</v>
+        <v>1.022195560887822</v>
       </c>
       <c r="AI3">
-        <v>1.025314305130819</v>
+        <v>0.8926737633061992</v>
       </c>
       <c r="AJ3">
-        <v>10.88961403226149</v>
+        <v>10.72246407622332</v>
       </c>
       <c r="AK3">
-        <v>10.87392360341344</v>
+        <v>11.99092217079957</v>
       </c>
       <c r="AL3">
-        <v>0.5</v>
+        <v>0.4929577464788732</v>
       </c>
       <c r="AM3">
-        <v>0.5</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="AN3">
         <v>46.5</v>
       </c>
       <c r="AO3">
-        <v>49.5</v>
+        <v>29.5</v>
       </c>
       <c r="AP3">
         <v>76.8</v>
       </c>
       <c r="AQ3">
-        <v>75.7</v>
+        <v>74.2</v>
       </c>
       <c r="AR3">
         <v>0.55</v>
       </c>
       <c r="AS3">
-        <v>0.5</v>
+        <v>0.2142857142857143</v>
       </c>
       <c r="AT3">
-        <v>0.4917082551118301</v>
+        <v>0.4888392946342679</v>
       </c>
       <c r="AU3">
-        <v>0.5078199054889029</v>
+        <v>0.512717354333439</v>
       </c>
       <c r="AV3">
         <v>1.55</v>
       </c>
       <c r="AW3">
-        <v>2.53</v>
+        <v>-7.35</v>
       </c>
       <c r="AX3">
-        <v>0</v>
+        <v>0.04608542289701704</v>
       </c>
       <c r="AY3">
-        <v>0.1477877086718865</v>
+        <v>0.5276548886270119</v>
       </c>
       <c r="AZ3">
-        <v>0</v>
+        <v>0.05427621283255087</v>
       </c>
       <c r="BA3">
-        <v>0.1174101307189543</v>
+        <v>0.396358989197531</v>
       </c>
       <c r="BB3">
-        <v>0.5216044800801791</v>
+        <v>0.5047612307230167</v>
       </c>
     </row>
     <row r="4" spans="1:54">
@@ -1069,157 +1063,157 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>224.5</v>
+        <v>218.5</v>
       </c>
       <c r="E4">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
         <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4">
-        <v>0.3692307692307693</v>
+        <v>0.5285714285714286</v>
       </c>
       <c r="I4">
-        <v>0.484375</v>
+        <v>0.5428571428571428</v>
       </c>
       <c r="J4">
-        <v>113.8970588235294</v>
+        <v>113.3521126760563</v>
       </c>
       <c r="K4">
-        <v>115.7878787878788</v>
+        <v>112.1506849315068</v>
       </c>
       <c r="L4">
-        <v>95.55882352941178</v>
+        <v>97.80281690140848</v>
       </c>
       <c r="M4">
-        <v>100.5651515151515</v>
+        <v>94.69863013698628</v>
       </c>
       <c r="N4">
-        <v>117.7823529411765</v>
+        <v>115.6323943661972</v>
       </c>
       <c r="O4">
-        <v>114.8757575757576</v>
+        <v>117.1287671232877</v>
       </c>
       <c r="P4">
-        <v>117.1205882352941</v>
+        <v>115.0591549295774</v>
       </c>
       <c r="Q4">
-        <v>111.0136363636364</v>
+        <v>111.3561643835616</v>
       </c>
       <c r="R4">
-        <v>76.65000000000001</v>
+        <v>74.07183098591547</v>
       </c>
       <c r="S4">
-        <v>75.72727272727271</v>
+        <v>77.33835616438354</v>
       </c>
       <c r="T4">
-        <v>0.48925</v>
+        <v>0.3955633802816901</v>
       </c>
       <c r="U4">
-        <v>0.3619242424242424</v>
+        <v>0.3726027397260273</v>
       </c>
       <c r="V4">
-        <v>0.6000735294117647</v>
+        <v>0.6022816901408453</v>
       </c>
       <c r="W4">
-        <v>0.5629242424242427</v>
+        <v>0.5925479452054794</v>
       </c>
       <c r="X4">
-        <v>0.3157205882352941</v>
+        <v>0.2579577464788733</v>
       </c>
       <c r="Y4">
-        <v>0.2699242424242424</v>
+        <v>0.2701095890410961</v>
       </c>
       <c r="Z4">
-        <v>10.96029411764705</v>
+        <v>12.09718309859155</v>
       </c>
       <c r="AA4">
-        <v>11.17424242424242</v>
+        <v>11.73424657534247</v>
       </c>
       <c r="AB4">
-        <v>11.74264705882353</v>
+        <v>11.66197183098592</v>
       </c>
       <c r="AC4">
-        <v>12.74393939393939</v>
+        <v>13.67123287671233</v>
       </c>
       <c r="AD4">
-        <v>0.2355441176470588</v>
+        <v>0.2116408450704225</v>
       </c>
       <c r="AE4">
-        <v>0.2035151515151514</v>
+        <v>0.2098972602739726</v>
       </c>
       <c r="AF4">
-        <v>0.9947341381967634</v>
+        <v>0.9899747831969986</v>
       </c>
       <c r="AG4">
-        <v>1.011247849675797</v>
+        <v>0.9794819644673087</v>
       </c>
       <c r="AH4">
-        <v>0.9774908543146116</v>
+        <v>0.8969102054340623</v>
       </c>
       <c r="AI4">
-        <v>0.9960743260926459</v>
+        <v>1.028378323358169</v>
       </c>
       <c r="AJ4">
-        <v>11.84227187300591</v>
+        <v>11.28391425387097</v>
       </c>
       <c r="AK4">
-        <v>11.49376003503133</v>
+        <v>10.37207953003852</v>
       </c>
       <c r="AL4">
-        <v>0.5</v>
+        <v>0.5492957746478874</v>
       </c>
       <c r="AM4">
-        <v>0.6060606060606061</v>
+        <v>0.6164383561643836</v>
       </c>
       <c r="AN4">
-        <v>48.5</v>
+        <v>50.5</v>
       </c>
       <c r="AO4">
-        <v>49.5</v>
+        <v>46.5</v>
       </c>
       <c r="AP4">
-        <v>75.3</v>
+        <v>76.5</v>
       </c>
       <c r="AQ4">
-        <v>75.2</v>
+        <v>77.2</v>
       </c>
       <c r="AR4">
-        <v>0.5517241379310345</v>
+        <v>0.5909090909090909</v>
       </c>
       <c r="AS4">
-        <v>0.4666666666666667</v>
+        <v>0.3529411764705883</v>
       </c>
       <c r="AT4">
-        <v>0.4969860149582434</v>
+        <v>0.5136160748671383</v>
       </c>
       <c r="AU4">
-        <v>0.4781875547917167</v>
+        <v>0.4894104322919812</v>
       </c>
       <c r="AV4">
-        <v>3.12</v>
+        <v>0.82</v>
       </c>
       <c r="AW4">
-        <v>5.37</v>
+        <v>2.04</v>
       </c>
       <c r="AX4">
-        <v>0.3082118879973798</v>
+        <v>0.07973539923194738</v>
       </c>
       <c r="AY4">
-        <v>0.2629182021531677</v>
+        <v>0</v>
       </c>
       <c r="AZ4">
-        <v>0.1266860702614379</v>
+        <v>0.06484448356807514</v>
       </c>
       <c r="BA4">
-        <v>0.2080092592592592</v>
+        <v>0</v>
       </c>
       <c r="BB4">
-        <v>0.5184085503671141</v>
+        <v>0.5669886270524563</v>
       </c>
     </row>
     <row r="5" spans="1:54">
@@ -1230,157 +1224,157 @@
         <v>2023</v>
       </c>
       <c r="D5">
-        <v>225.5</v>
+        <v>232.5</v>
       </c>
       <c r="E5">
-        <v>-8</v>
+        <v>-13</v>
       </c>
       <c r="F5" t="s">
         <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H5">
-        <v>0.3636363636363636</v>
+        <v>0.4571428571428571</v>
       </c>
       <c r="I5">
-        <v>0.5606060606060606</v>
+        <v>0.4225352112676056</v>
       </c>
       <c r="J5">
-        <v>108.5652173913043</v>
+        <v>113.9295774647887</v>
       </c>
       <c r="K5">
-        <v>117.2647058823529</v>
+        <v>112.7887323943662</v>
       </c>
       <c r="L5">
-        <v>95.85942028985505</v>
+        <v>98.50140845070423</v>
       </c>
       <c r="M5">
-        <v>99.68235294117649</v>
+        <v>100.5464788732394</v>
       </c>
       <c r="N5">
-        <v>112.5246376811594</v>
+        <v>114.7197183098592</v>
       </c>
       <c r="O5">
-        <v>116.9926470588235</v>
+        <v>111.4239436619718</v>
       </c>
       <c r="P5">
-        <v>113.4014492753623</v>
+        <v>114.2112676056338</v>
       </c>
       <c r="Q5">
-        <v>117.0705882352941</v>
+        <v>120.5549295774648</v>
       </c>
       <c r="R5">
-        <v>78.10289855072466</v>
+        <v>77.01408450704226</v>
       </c>
       <c r="S5">
-        <v>74.9911764705882</v>
+        <v>75.1887323943662</v>
       </c>
       <c r="T5">
-        <v>0.403391304347826</v>
+        <v>0.3497887323943663</v>
       </c>
       <c r="U5">
-        <v>0.4318970588235295</v>
+        <v>0.3425352112676056</v>
       </c>
       <c r="V5">
-        <v>0.5673043478260872</v>
+        <v>0.5800140845070423</v>
       </c>
       <c r="W5">
-        <v>0.5878676470588234</v>
+        <v>0.5590845070422535</v>
       </c>
       <c r="X5">
-        <v>0.2739710144927537</v>
+        <v>0.2828591549295774</v>
       </c>
       <c r="Y5">
-        <v>0.2730294117647058</v>
+        <v>0.2327887323943662</v>
       </c>
       <c r="Z5">
-        <v>11.88985507246377</v>
+        <v>12.54084507042253</v>
       </c>
       <c r="AA5">
-        <v>13.08088235294118</v>
+        <v>12.9169014084507</v>
       </c>
       <c r="AB5">
-        <v>14.18985507246377</v>
+        <v>12.88591549295775</v>
       </c>
       <c r="AC5">
-        <v>10.88235294117647</v>
+        <v>11.62535211267605</v>
       </c>
       <c r="AD5">
-        <v>0.2161231884057971</v>
+        <v>0.2209154929577465</v>
       </c>
       <c r="AE5">
-        <v>0.2111985294117648</v>
+        <v>0.1895633802816901</v>
       </c>
       <c r="AF5">
-        <v>0.9481678374786405</v>
+        <v>0.9950181437972815</v>
       </c>
       <c r="AG5">
-        <v>1.024145902902646</v>
+        <v>0.9850544313918445</v>
       </c>
       <c r="AH5">
-        <v>1.022426912294754</v>
+        <v>0.9859892034450075</v>
       </c>
       <c r="AI5">
-        <v>1.040381239026837</v>
+        <v>1.105311355311355</v>
       </c>
       <c r="AJ5">
-        <v>9.383115055307956</v>
+        <v>10.43871982823803</v>
       </c>
       <c r="AK5">
-        <v>9.928594544011613</v>
+        <v>11.06690981075445</v>
       </c>
       <c r="AL5">
-        <v>0.5217391304347826</v>
+        <v>0.4788732394366197</v>
       </c>
       <c r="AM5">
-        <v>0.4852941176470588</v>
+        <v>0.2676056338028169</v>
       </c>
       <c r="AN5">
-        <v>49.5</v>
+        <v>45.5</v>
       </c>
       <c r="AO5">
-        <v>23.5</v>
+        <v>22.5</v>
       </c>
       <c r="AP5">
-        <v>76.2</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="AQ5">
-        <v>74.3</v>
+        <v>73.2</v>
       </c>
       <c r="AR5">
-        <v>0.6052631578947368</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="AS5">
-        <v>0.4782608695652174</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="AT5">
-        <v>0.5093381651418217</v>
+        <v>0.5093481980741569</v>
       </c>
       <c r="AU5">
-        <v>0.4952303277325308</v>
+        <v>0.4922913265635839</v>
       </c>
       <c r="AV5">
-        <v>4.23</v>
+        <v>-0.84</v>
       </c>
       <c r="AW5">
-        <v>5.67</v>
+        <v>0.02</v>
       </c>
       <c r="AX5">
-        <v>0.04650053654465243</v>
+        <v>0.1625152077863866</v>
       </c>
       <c r="AY5">
-        <v>0.2728716645489199</v>
+        <v>0.2994396498834312</v>
       </c>
       <c r="AZ5">
-        <v>0.0542013888888889</v>
+        <v>0.1329831768388106</v>
       </c>
       <c r="BA5">
-        <v>0.1910365604575164</v>
+        <v>0.2264994131455399</v>
       </c>
       <c r="BB5">
-        <v>0.4905978661794189</v>
+        <v>0.4521629164641817</v>
       </c>
     </row>
     <row r="6" spans="1:54">
@@ -1391,139 +1385,139 @@
         <v>2023</v>
       </c>
       <c r="D6">
-        <v>231.5</v>
+        <v>239.5</v>
       </c>
       <c r="E6">
-        <v>12.5</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
         <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H6">
-        <v>0.40625</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="I6">
-        <v>0.5441176470588235</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="J6">
-        <v>110.2686567164179</v>
+        <v>121.0422535211268</v>
       </c>
       <c r="K6">
-        <v>117.8529411764706</v>
+        <v>117.6388888888889</v>
       </c>
       <c r="L6">
-        <v>98.61194029850742</v>
+        <v>100.1549295774648</v>
       </c>
       <c r="M6">
-        <v>97.77794117647058</v>
+        <v>97.68333333333334</v>
       </c>
       <c r="N6">
-        <v>111.2716417910448</v>
+        <v>119.9239436619718</v>
       </c>
       <c r="O6">
-        <v>118.5911764705882</v>
+        <v>118.5916666666667</v>
       </c>
       <c r="P6">
-        <v>119.5925373134328</v>
+        <v>117.3521126760564</v>
       </c>
       <c r="Q6">
-        <v>112.875</v>
+        <v>113.0152777777778</v>
       </c>
       <c r="R6">
-        <v>76.25820895522386</v>
+        <v>77.82394366197182</v>
       </c>
       <c r="S6">
-        <v>79.00735294117648</v>
+        <v>78.71805555555558</v>
       </c>
       <c r="T6">
-        <v>0.368</v>
+        <v>0.4213943661971831</v>
       </c>
       <c r="U6">
-        <v>0.4761470588235292</v>
+        <v>0.4777777777777775</v>
       </c>
       <c r="V6">
-        <v>0.5531044776119403</v>
+        <v>0.6131971830985914</v>
       </c>
       <c r="W6">
-        <v>0.6019117647058825</v>
+        <v>0.6008611111111112</v>
       </c>
       <c r="X6">
-        <v>0.2885373134328358</v>
+        <v>0.2931690140845071</v>
       </c>
       <c r="Y6">
-        <v>0.2490294117647059</v>
+        <v>0.2516111111111112</v>
       </c>
       <c r="Z6">
-        <v>13.70298507462687</v>
+        <v>11.99577464788732</v>
       </c>
       <c r="AA6">
-        <v>11.62794117647059</v>
+        <v>11.53472222222222</v>
       </c>
       <c r="AB6">
-        <v>11.46865671641791</v>
+        <v>12.02816901408451</v>
       </c>
       <c r="AC6">
-        <v>10.72058823529412</v>
+        <v>10.73055555555556</v>
       </c>
       <c r="AD6">
-        <v>0.2184626865671641</v>
+        <v>0.2186056338028169</v>
       </c>
       <c r="AE6">
-        <v>0.1953382352941177</v>
+        <v>0.1971736111111112</v>
       </c>
       <c r="AF6">
-        <v>0.9630450368246105</v>
+        <v>1.057137585337352</v>
       </c>
       <c r="AG6">
-        <v>1.029283329052145</v>
+        <v>1.027413876758855</v>
       </c>
       <c r="AH6">
-        <v>1.003609456776755</v>
+        <v>0.9721123264292918</v>
       </c>
       <c r="AI6">
-        <v>1.026703269278762</v>
+        <v>0.9832349468713105</v>
       </c>
       <c r="AJ6">
-        <v>11.42605309108816</v>
+        <v>13.23294716592983</v>
       </c>
       <c r="AK6">
-        <v>11.83248855765887</v>
+        <v>11.69912811988279</v>
       </c>
       <c r="AL6">
-        <v>0.2238805970149254</v>
+        <v>0.6056338028169014</v>
       </c>
       <c r="AM6">
-        <v>0.6911764705882353</v>
+        <v>0.6805555555555556</v>
       </c>
       <c r="AN6">
-        <v>23.5</v>
+        <v>34.5</v>
       </c>
       <c r="AO6">
         <v>54.5</v>
       </c>
       <c r="AP6">
-        <v>73.7</v>
+        <v>75.90000000000001</v>
       </c>
       <c r="AQ6">
         <v>78.59999999999999</v>
       </c>
       <c r="AR6">
-        <v>0.3636363636363636</v>
+        <v>0.6</v>
       </c>
       <c r="AS6">
-        <v>0.5789473684210527</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="AT6">
-        <v>0.5240244502285063</v>
+        <v>0.4815164250076349</v>
       </c>
       <c r="AU6">
-        <v>0.4833064703318732</v>
+        <v>0.4794930998371938</v>
       </c>
       <c r="AV6">
-        <v>-8.26</v>
+        <v>-5.26</v>
       </c>
       <c r="AW6">
         <v>7.02</v>
@@ -1532,16 +1526,16 @@
         <v>0</v>
       </c>
       <c r="AY6">
-        <v>0.06656427584088465</v>
+        <v>0.01914633791759951</v>
       </c>
       <c r="AZ6">
         <v>0</v>
       </c>
       <c r="BA6">
-        <v>0.07608762254901962</v>
+        <v>0.03260127314814815</v>
       </c>
       <c r="BB6">
-        <v>0.5276267923777707</v>
+        <v>0.5099659956911818</v>
       </c>
     </row>
     <row r="7" spans="1:54">
@@ -1552,318 +1546,157 @@
         <v>2023</v>
       </c>
       <c r="D7">
-        <v>236</v>
+        <v>238.5</v>
       </c>
       <c r="E7">
-        <v>-4.5</v>
+        <v>-7</v>
       </c>
       <c r="F7" t="s">
         <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H7">
-        <v>0.4776119402985075</v>
+        <v>0.5</v>
       </c>
       <c r="I7">
-        <v>0.5538461538461539</v>
+        <v>0.6176470588235294</v>
       </c>
       <c r="J7">
-        <v>118.0882352941177</v>
+        <v>112.8333333333333</v>
       </c>
       <c r="K7">
-        <v>113.3880597014925</v>
+        <v>117.8591549295775</v>
       </c>
       <c r="L7">
-        <v>101.189705882353</v>
+        <v>97.04444444444445</v>
       </c>
       <c r="M7">
-        <v>97.24925373134325</v>
+        <v>100.6816901408451</v>
       </c>
       <c r="N7">
-        <v>115.7882352941176</v>
+        <v>115.2722222222223</v>
       </c>
       <c r="O7">
-        <v>115.9134328358209</v>
+        <v>115.9169014084507</v>
       </c>
       <c r="P7">
-        <v>115.3</v>
+        <v>115.0041666666667</v>
       </c>
       <c r="Q7">
-        <v>113.7014925373134</v>
+        <v>114.5014084507042</v>
       </c>
       <c r="R7">
-        <v>76.43088235294117</v>
+        <v>77.02916666666665</v>
       </c>
       <c r="S7">
-        <v>76.29402985074631</v>
+        <v>73.06901408450706</v>
       </c>
       <c r="T7">
-        <v>0.4815294117647059</v>
+        <v>0.3875416666666667</v>
       </c>
       <c r="U7">
-        <v>0.3677462686567163</v>
+        <v>0.3667042253521127</v>
       </c>
       <c r="V7">
-        <v>0.5984117647058821</v>
+        <v>0.5845833333333333</v>
       </c>
       <c r="W7">
-        <v>0.5720298507462688</v>
+        <v>0.5734366197183097</v>
       </c>
       <c r="X7">
-        <v>0.2232941176470588</v>
+        <v>0.2815277777777779</v>
       </c>
       <c r="Y7">
-        <v>0.2442238805970149</v>
+        <v>0.2565211267605633</v>
       </c>
       <c r="Z7">
-        <v>13.75441176470588</v>
+        <v>12.20694444444444</v>
       </c>
       <c r="AA7">
-        <v>11.73582089552239</v>
+        <v>10.96619718309859</v>
       </c>
       <c r="AB7">
-        <v>12.02794117647059</v>
+        <v>11.28611111111111</v>
       </c>
       <c r="AC7">
-        <v>12.45522388059701</v>
+        <v>14.09295774647887</v>
       </c>
       <c r="AD7">
-        <v>0.1999632352941177</v>
+        <v>0.2105486111111111</v>
       </c>
       <c r="AE7">
-        <v>0.2154179104477612</v>
+        <v>0.2181760563380282</v>
       </c>
       <c r="AF7">
-        <v>1.031338299511945</v>
+        <v>0.9854439592430858</v>
       </c>
       <c r="AG7">
-        <v>0.9902887310174021</v>
+        <v>1.029337597638231</v>
       </c>
       <c r="AH7">
-        <v>1.024657534246575</v>
+        <v>1.06056129985229</v>
       </c>
       <c r="AI7">
-        <v>1.120047387126497</v>
+        <v>1.00685149776928</v>
       </c>
       <c r="AJ7">
-        <v>10.84073919516459</v>
+        <v>14.37590576856522</v>
       </c>
       <c r="AK7">
-        <v>12.27417532127235</v>
+        <v>12.43268723816023</v>
       </c>
       <c r="AL7">
-        <v>0.5147058823529411</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="AM7">
-        <v>0.5522388059701493</v>
+        <v>0.4929577464788732</v>
       </c>
       <c r="AN7">
         <v>52.5</v>
       </c>
       <c r="AO7">
-        <v>52.5</v>
+        <v>23.5</v>
       </c>
       <c r="AP7">
-        <v>76.3</v>
+        <v>76.40000000000001</v>
       </c>
       <c r="AQ7">
-        <v>77</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="AR7">
-        <v>0.4705882352941176</v>
+        <v>0.4117647058823529</v>
       </c>
       <c r="AS7">
-        <v>0.4285714285714285</v>
+        <v>0.35</v>
       </c>
       <c r="AT7">
-        <v>0.4714385683098666</v>
+        <v>0.4708728691011166</v>
       </c>
       <c r="AU7">
-        <v>0.5182421709507165</v>
+        <v>0.5052432495398858</v>
       </c>
       <c r="AV7">
-        <v>5.52</v>
+        <v>0.09</v>
       </c>
       <c r="AW7">
-        <v>6.94</v>
+        <v>-7.9</v>
       </c>
       <c r="AX7">
-        <v>0.07422068283028209</v>
+        <v>0.1225826131164209</v>
       </c>
       <c r="AY7">
-        <v>0.104940606977748</v>
+        <v>0</v>
       </c>
       <c r="AZ7">
-        <v>0.07293300653594773</v>
+        <v>0.08055748456790125</v>
       </c>
       <c r="BA7">
-        <v>0.07710933966530982</v>
+        <v>0</v>
       </c>
       <c r="BB7">
-        <v>0.553060013761983</v>
-      </c>
-    </row>
-    <row r="8" spans="1:54">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>2023</v>
-      </c>
-      <c r="D8">
-        <v>244.5</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8">
-        <v>0.5692307692307692</v>
-      </c>
-      <c r="I8">
-        <v>0.5873015873015873</v>
-      </c>
-      <c r="J8">
-        <v>121.2121212121212</v>
-      </c>
-      <c r="K8">
-        <v>115.8805970149254</v>
-      </c>
-      <c r="L8">
-        <v>100.1909090909091</v>
-      </c>
-      <c r="M8">
-        <v>99.67611940298508</v>
-      </c>
-      <c r="N8">
-        <v>119.9772727272727</v>
-      </c>
-      <c r="O8">
-        <v>115.244776119403</v>
-      </c>
-      <c r="P8">
-        <v>117.3015151515152</v>
-      </c>
-      <c r="Q8">
-        <v>111.4044776119403</v>
-      </c>
-      <c r="R8">
-        <v>77.42121212121212</v>
-      </c>
-      <c r="S8">
-        <v>77.94328358208958</v>
-      </c>
-      <c r="T8">
-        <v>0.4156666666666666</v>
-      </c>
-      <c r="U8">
-        <v>0.4485223880597016</v>
-      </c>
-      <c r="V8">
-        <v>0.6145757575757574</v>
-      </c>
-      <c r="W8">
-        <v>0.5789850746268654</v>
-      </c>
-      <c r="X8">
-        <v>0.2936969696969697</v>
-      </c>
-      <c r="Y8">
-        <v>0.2517313432835822</v>
-      </c>
-      <c r="Z8">
-        <v>12.16363636363636</v>
-      </c>
-      <c r="AA8">
-        <v>12.27761194029851</v>
-      </c>
-      <c r="AB8">
-        <v>12.21666666666667</v>
-      </c>
-      <c r="AC8">
-        <v>10.2955223880597</v>
-      </c>
-      <c r="AD8">
-        <v>0.2187348484848485</v>
-      </c>
-      <c r="AE8">
-        <v>0.1839776119402985</v>
-      </c>
-      <c r="AF8">
-        <v>1.058621145957391</v>
-      </c>
-      <c r="AG8">
-        <v>1.012057615850877</v>
-      </c>
-      <c r="AH8">
-        <v>1.02575</v>
-      </c>
-      <c r="AI8">
-        <v>1.058560879271853</v>
-      </c>
-      <c r="AJ8">
-        <v>13.41811885780854</v>
-      </c>
-      <c r="AK8">
-        <v>12.74728228344075</v>
-      </c>
-      <c r="AL8">
-        <v>0.6060606060606061</v>
-      </c>
-      <c r="AM8">
-        <v>0.7164179104477612</v>
-      </c>
-      <c r="AN8">
-        <v>34.5</v>
-      </c>
-      <c r="AO8">
-        <v>53.5</v>
-      </c>
-      <c r="AP8">
-        <v>75.90000000000001</v>
-      </c>
-      <c r="AQ8">
-        <v>76.09999999999999</v>
-      </c>
-      <c r="AR8">
-        <v>0.5652173913043478</v>
-      </c>
-      <c r="AS8">
-        <v>0.6923076923076923</v>
-      </c>
-      <c r="AT8">
-        <v>0.4772801085419492</v>
-      </c>
-      <c r="AU8">
-        <v>0.4889211652235649</v>
-      </c>
-      <c r="AV8">
-        <v>-5.26</v>
-      </c>
-      <c r="AW8">
-        <v>3.22</v>
-      </c>
-      <c r="AX8">
-        <v>0</v>
-      </c>
-      <c r="AY8">
-        <v>0</v>
-      </c>
-      <c r="AZ8">
-        <v>0</v>
-      </c>
-      <c r="BA8">
-        <v>0</v>
-      </c>
-      <c r="BB8">
-        <v>0.5126683611858208</v>
+        <v>0.5100788144601064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Basic changes in consensus tracker
</commit_message>
<xml_diff>
--- a/current_games_spread.xlsx
+++ b/current_games_spread.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>year</t>
   </si>
@@ -172,16 +172,10 @@
     <t>injury_mins_a</t>
   </si>
   <si>
-    <t>LALakers</t>
+    <t>Denver</t>
   </si>
   <si>
     <t>Miami</t>
-  </si>
-  <si>
-    <t>Denver</t>
-  </si>
-  <si>
-    <t>Boston</t>
   </si>
 </sst>
 </file>
@@ -539,7 +533,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA3"/>
+  <dimension ref="A1:BA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -711,312 +705,154 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E2">
-        <v>-5.5</v>
+        <v>-8.5</v>
       </c>
       <c r="F2" t="s">
         <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H2">
-        <v>0.5208333333333334</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="I2">
-        <v>0.5425531914893617</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="J2">
-        <v>117.1707317073171</v>
+        <v>115.7926829268293</v>
       </c>
       <c r="K2">
-        <v>115.7926829268293</v>
+        <v>109.4756097560976</v>
       </c>
       <c r="L2">
-        <v>100.7658536585366</v>
+        <v>97.49512195121947</v>
       </c>
       <c r="M2">
-        <v>97.49512195121947</v>
+        <v>95.51707317073166</v>
       </c>
       <c r="N2">
-        <v>115.3134146341463</v>
+        <v>118.3817073170732</v>
       </c>
       <c r="O2">
-        <v>118.3817073170732</v>
+        <v>113.9914634146342</v>
       </c>
       <c r="P2">
-        <v>114.7548780487805</v>
+        <v>115.0475609756098</v>
       </c>
       <c r="Q2">
-        <v>115.0475609756098</v>
+        <v>114.4048780487804</v>
       </c>
       <c r="R2">
-        <v>76.46951219512194</v>
+        <v>76.57439024390247</v>
       </c>
       <c r="S2">
-        <v>76.57439024390247</v>
+        <v>77.84146341463416</v>
       </c>
       <c r="T2">
-        <v>0.3502073170731707</v>
+        <v>0.3610853658536586</v>
       </c>
       <c r="U2">
-        <v>0.3610853658536586</v>
+        <v>0.4089268292682925</v>
       </c>
       <c r="V2">
-        <v>0.5831585365853659</v>
+        <v>0.6026829268292681</v>
       </c>
       <c r="W2">
-        <v>0.6026829268292681</v>
+        <v>0.5751097560975612</v>
       </c>
       <c r="X2">
-        <v>0.3024390243902439</v>
+        <v>0.2604024390243902</v>
       </c>
       <c r="Y2">
-        <v>0.2604024390243902</v>
+        <v>0.2742073170731708</v>
       </c>
       <c r="Z2">
-        <v>11.76585365853659</v>
+        <v>12.5280487804878</v>
       </c>
       <c r="AA2">
-        <v>12.5280487804878</v>
+        <v>11.81463414634147</v>
       </c>
       <c r="AB2">
-        <v>10.51341463414634</v>
+        <v>11.67195121951219</v>
       </c>
       <c r="AC2">
-        <v>11.67195121951219</v>
+        <v>13.95121951219512</v>
       </c>
       <c r="AD2">
-        <v>0.2047256097560976</v>
+        <v>0.1996524390243903</v>
       </c>
       <c r="AE2">
-        <v>0.1996524390243903</v>
+        <v>0.214859756097561</v>
       </c>
       <c r="AF2">
-        <v>1.021540816977481</v>
+        <v>1.009526442256576</v>
       </c>
       <c r="AG2">
-        <v>1.009526442256576</v>
+        <v>0.9544516979607459</v>
       </c>
       <c r="AH2">
-        <v>1.04406050513461</v>
+        <v>0.9730033350886431</v>
       </c>
       <c r="AI2">
-        <v>0.9730033350886431</v>
+        <v>1.096134566113401</v>
       </c>
       <c r="AJ2">
-        <v>10.23361853134521</v>
+        <v>11.16695670584409</v>
       </c>
       <c r="AK2">
-        <v>11.16695670584409</v>
+        <v>10.58096036232879</v>
       </c>
       <c r="AL2">
-        <v>0.524390243902439</v>
+        <v>0.6463414634146342</v>
       </c>
       <c r="AM2">
-        <v>0.6463414634146342</v>
+        <v>0.5365853658536586</v>
       </c>
       <c r="AN2">
-        <v>44.5</v>
+        <v>51.5</v>
       </c>
       <c r="AO2">
-        <v>51.5</v>
+        <v>49.5</v>
       </c>
       <c r="AP2">
-        <v>75</v>
+        <v>75.09999999999999</v>
       </c>
       <c r="AQ2">
-        <v>75.09999999999999</v>
+        <v>76.2</v>
       </c>
       <c r="AR2">
-        <v>0.4583333333333333</v>
+        <v>0.68</v>
       </c>
       <c r="AS2">
-        <v>0.68</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="AT2">
-        <v>0.5018545662697778</v>
+        <v>0.4922378056669106</v>
       </c>
       <c r="AU2">
-        <v>0.4922378056669106</v>
+        <v>0.503512542778542</v>
       </c>
       <c r="AV2">
-        <v>-3.08</v>
+        <v>2.16</v>
       </c>
       <c r="AW2">
-        <v>2.16</v>
+        <v>4.23</v>
       </c>
       <c r="AX2">
-        <v>0.009978360182736233</v>
+        <v>0</v>
       </c>
       <c r="AY2">
+        <v>0.1352191751241632</v>
+      </c>
+      <c r="AZ2">
         <v>0</v>
       </c>
-      <c r="AZ2">
-        <v>0.01354938271604938</v>
-      </c>
       <c r="BA2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:53">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2023</v>
-      </c>
-      <c r="D3">
-        <v>214</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3">
-        <v>0.4361702127659575</v>
-      </c>
-      <c r="I3">
-        <v>0.5567010309278351</v>
-      </c>
-      <c r="J3">
-        <v>109.4756097560976</v>
-      </c>
-      <c r="K3">
-        <v>117.9390243902439</v>
-      </c>
-      <c r="L3">
-        <v>95.51707317073166</v>
-      </c>
-      <c r="M3">
-        <v>97.80487804878049</v>
-      </c>
-      <c r="N3">
-        <v>113.9914634146342</v>
-      </c>
-      <c r="O3">
-        <v>118.9780487804878</v>
-      </c>
-      <c r="P3">
-        <v>114.4048780487804</v>
-      </c>
-      <c r="Q3">
-        <v>112.2756097560975</v>
-      </c>
-      <c r="R3">
-        <v>77.84146341463416</v>
-      </c>
-      <c r="S3">
-        <v>78.72926829268295</v>
-      </c>
-      <c r="T3">
-        <v>0.4089268292682925</v>
-      </c>
-      <c r="U3">
-        <v>0.4800365853658533</v>
-      </c>
-      <c r="V3">
-        <v>0.5751097560975612</v>
-      </c>
-      <c r="W3">
-        <v>0.6017560975609757</v>
-      </c>
-      <c r="X3">
-        <v>0.2742073170731708</v>
-      </c>
-      <c r="Y3">
-        <v>0.2458780487804878</v>
-      </c>
-      <c r="Z3">
-        <v>11.81463414634147</v>
-      </c>
-      <c r="AA3">
-        <v>11.45365853658537</v>
-      </c>
-      <c r="AB3">
-        <v>13.95121951219512</v>
-      </c>
-      <c r="AC3">
-        <v>10.71829268292683</v>
-      </c>
-      <c r="AD3">
-        <v>0.214859756097561</v>
-      </c>
-      <c r="AE3">
-        <v>0.1910060975609757</v>
-      </c>
-      <c r="AF3">
-        <v>0.9544516979607459</v>
-      </c>
-      <c r="AG3">
-        <v>1.028239096689136</v>
-      </c>
-      <c r="AH3">
-        <v>1.096134566113401</v>
-      </c>
-      <c r="AI3">
-        <v>0.9552959018371076</v>
-      </c>
-      <c r="AJ3">
-        <v>10.58096036232879</v>
-      </c>
-      <c r="AK3">
-        <v>11.95351521007331</v>
-      </c>
-      <c r="AL3">
-        <v>0.5365853658536586</v>
-      </c>
-      <c r="AM3">
-        <v>0.6951219512195121</v>
-      </c>
-      <c r="AN3">
-        <v>49.5</v>
-      </c>
-      <c r="AO3">
-        <v>54.5</v>
-      </c>
-      <c r="AP3">
-        <v>76.2</v>
-      </c>
-      <c r="AQ3">
-        <v>78.59999999999999</v>
-      </c>
-      <c r="AR3">
-        <v>0.6153846153846154</v>
-      </c>
-      <c r="AS3">
-        <v>0.5416666666666666</v>
-      </c>
-      <c r="AT3">
-        <v>0.503512542778542</v>
-      </c>
-      <c r="AU3">
-        <v>0.4834349398865997</v>
-      </c>
-      <c r="AV3">
-        <v>4.23</v>
-      </c>
-      <c r="AW3">
-        <v>7.02</v>
-      </c>
-      <c r="AX3">
-        <v>0.1352191751241632</v>
-      </c>
-      <c r="AY3">
-        <v>0</v>
-      </c>
-      <c r="AZ3">
         <v>0.1187381436314363</v>
-      </c>
-      <c r="BA3">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>